<commit_message>
A few minor bugfixes. Adding unit tests
</commit_message>
<xml_diff>
--- a/src/test/resources/SBAC-IAB-FIXED-G11M-Winter-2017-2018.xlsx
+++ b/src/test/resources/SBAC-IAB-FIXED-G11M-Winter-2017-2018.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10116"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\AP_FixedFormPackager\FixedFormPackager\bin\Debug\inputs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/emunoz/trunk/sbrepo/repositories/TDS_FixedFormPackager/src/test/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{9F030C5C-90E6-43A9-906F-D3CF97C71C65}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" tabRatio="644" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="440" windowWidth="28800" windowHeight="12440" tabRatio="644" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Package" sheetId="16" r:id="rId1"/>
@@ -603,9 +602,6 @@
     <t>SegmentSlope</t>
   </si>
   <si>
-    <t>SegementIntercept</t>
-  </si>
-  <si>
     <t>MATH</t>
   </si>
   <si>
@@ -1000,12 +996,15 @@
   </si>
   <si>
     <t>Unique segment form ID per SegmentId</t>
+  </si>
+  <si>
+    <t>SegmentIntercept</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.000000E+00"/>
     <numFmt numFmtId="165" formatCode="0.0"/>
@@ -2014,7 +2013,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6A1B9193-2321-4710-B4AB-EB38DCF0796F}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2024,30 +2023,30 @@
       <selection pane="bottomRight" activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="11" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="53.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="30.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="23.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="9.140625" style="2"/>
+    <col min="1" max="1" width="53.83203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.1640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="30.83203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="23.5" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="9.1640625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="22" t="s">
         <v>186</v>
       </c>
       <c r="B1" s="22"/>
       <c r="C1" s="22" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="D1" s="22"/>
       <c r="E1" s="7" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A2" s="7" t="s">
         <v>187</v>
       </c>
@@ -2055,16 +2054,16 @@
         <v>188</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="E2" s="7" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A3" s="9" t="s">
         <v>112</v>
       </c>
@@ -2072,16 +2071,16 @@
         <v>110</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D3" s="9" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>317</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A4" s="9" t="s">
         <v>113</v>
       </c>
@@ -2089,16 +2088,16 @@
         <v>110</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="D4" s="17" t="s">
         <v>53</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>319</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="18" t="s">
         <v>147</v>
       </c>
@@ -2106,7 +2105,7 @@
         <v>110</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D5" s="9" t="s">
         <v>169</v>
@@ -2115,7 +2114,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="18" t="s">
         <v>148</v>
       </c>
@@ -2123,7 +2122,7 @@
         <v>110</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="D6" s="9" t="s">
         <v>170</v>
@@ -2132,7 +2131,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="9" t="s">
         <v>149</v>
       </c>
@@ -2140,7 +2139,7 @@
         <v>110</v>
       </c>
       <c r="C7" s="9" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D7" s="9" t="s">
         <v>185</v>
@@ -2149,7 +2148,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A8" s="9" t="s">
         <v>116</v>
       </c>
@@ -2157,7 +2156,7 @@
         <v>110</v>
       </c>
       <c r="C8" s="9" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D8" s="9" t="s">
         <v>39</v>
@@ -2166,7 +2165,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A9" s="9" t="s">
         <v>117</v>
       </c>
@@ -2174,16 +2173,16 @@
         <v>110</v>
       </c>
       <c r="C9" s="9" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="D9" s="9" t="s">
         <v>40</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A10" s="9" t="s">
         <v>118</v>
       </c>
@@ -2191,7 +2190,7 @@
         <v>110</v>
       </c>
       <c r="C10" s="9" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="D10" s="9" t="s">
         <v>41</v>
@@ -2200,7 +2199,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A11" s="9" t="s">
         <v>119</v>
       </c>
@@ -2208,7 +2207,7 @@
         <v>110</v>
       </c>
       <c r="C11" s="9" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="D11" s="9" t="s">
         <v>42</v>
@@ -2217,7 +2216,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A12" s="9" t="s">
         <v>111</v>
       </c>
@@ -2225,16 +2224,16 @@
         <v>111</v>
       </c>
       <c r="C12" s="9" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="D12" s="9" t="s">
         <v>43</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>318</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A13" s="9" t="s">
         <v>114</v>
       </c>
@@ -2242,7 +2241,7 @@
         <v>110</v>
       </c>
       <c r="C13" s="9" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="D13" s="9" t="s">
         <v>44</v>
@@ -2251,7 +2250,7 @@
         <v>2280</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A14" s="9" t="s">
         <v>115</v>
       </c>
@@ -2259,7 +2258,7 @@
         <v>110</v>
       </c>
       <c r="C14" s="9" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="D14" s="9" t="s">
         <v>45</v>
@@ -2268,7 +2267,7 @@
         <v>2543</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A15" s="9" t="s">
         <v>115</v>
       </c>
@@ -2276,7 +2275,7 @@
         <v>110</v>
       </c>
       <c r="C15" s="9" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="D15" s="9" t="s">
         <v>46</v>
@@ -2285,7 +2284,7 @@
         <v>2628</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A16" s="9" t="s">
         <v>115</v>
       </c>
@@ -2293,7 +2292,7 @@
         <v>110</v>
       </c>
       <c r="C16" s="9" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="D16" s="9" t="s">
         <v>47</v>
@@ -2302,7 +2301,7 @@
         <v>2718</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A17" s="9" t="s">
         <v>115</v>
       </c>
@@ -2310,7 +2309,7 @@
         <v>110</v>
       </c>
       <c r="C17" s="9" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="D17" s="9" t="s">
         <v>48</v>
@@ -2329,7 +2328,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I46"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
@@ -2339,25 +2338,25 @@
       <selection pane="bottomRight" activeCell="J5" sqref="J5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="55" defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="55" defaultRowHeight="11" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="61.28515625" style="14" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.140625" style="14" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="30.28515625" style="14" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="26.85546875" style="14" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="61.33203125" style="14" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.1640625" style="14" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="30.33203125" style="14" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="26.83203125" style="14" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12" style="15" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="11.85546875" style="15" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="11.83203125" style="15" bestFit="1" customWidth="1"/>
     <col min="8" max="9" width="12" style="15" bestFit="1" customWidth="1"/>
     <col min="10" max="16384" width="55" style="14"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A1" s="22" t="s">
         <v>186</v>
       </c>
       <c r="B1" s="22"/>
       <c r="C1" s="22" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="D1" s="22"/>
       <c r="E1" s="23"/>
@@ -2366,7 +2365,7 @@
       <c r="H1" s="23"/>
       <c r="I1" s="23"/>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A2" s="7" t="s">
         <v>187</v>
       </c>
@@ -2374,10 +2373,10 @@
         <v>188</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="E2" s="20" t="s">
         <v>189</v>
@@ -2395,7 +2394,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="22.5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9" ht="22" x14ac:dyDescent="0.15">
       <c r="A3" s="17" t="s">
         <v>113</v>
       </c>
@@ -2403,28 +2402,28 @@
         <v>110</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="D3" s="17" t="s">
         <v>53</v>
       </c>
       <c r="E3" s="16" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="F3" s="16" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="G3" s="16" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="H3" s="16" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="I3" s="16" t="s">
-        <v>319</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A4" s="17" t="s">
         <v>129</v>
       </c>
@@ -2432,7 +2431,7 @@
         <v>110</v>
       </c>
       <c r="C4" s="17" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="D4" s="17" t="s">
         <v>52</v>
@@ -2453,7 +2452,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="22.5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9" ht="22" x14ac:dyDescent="0.15">
       <c r="A5" s="17" t="s">
         <v>128</v>
       </c>
@@ -2461,13 +2460,13 @@
         <v>110</v>
       </c>
       <c r="C5" s="17" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="D5" s="17" t="s">
         <v>51</v>
       </c>
       <c r="E5" s="16" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="F5" s="16" t="s">
         <v>76</v>
@@ -2482,7 +2481,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="22.5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:9" ht="22" x14ac:dyDescent="0.15">
       <c r="A6" s="17" t="s">
         <v>168</v>
       </c>
@@ -2490,24 +2489,24 @@
         <v>172</v>
       </c>
       <c r="C6" s="17" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="D6" s="17" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="E6" s="16"/>
       <c r="F6" s="16" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="G6" s="16"/>
       <c r="H6" s="16" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="I6" s="16" t="s">
-        <v>294</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A7" s="17" t="s">
         <v>131</v>
       </c>
@@ -2515,7 +2514,7 @@
         <v>172</v>
       </c>
       <c r="C7" s="17" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="D7" s="17" t="s">
         <v>54</v>
@@ -2532,7 +2531,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A8" s="17" t="s">
         <v>130</v>
       </c>
@@ -2540,7 +2539,7 @@
         <v>172</v>
       </c>
       <c r="C8" s="17" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="D8" s="17" t="s">
         <v>55</v>
@@ -2557,7 +2556,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A9" s="17" t="s">
         <v>133</v>
       </c>
@@ -2565,7 +2564,7 @@
         <v>172</v>
       </c>
       <c r="C9" s="17" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="D9" s="17" t="s">
         <v>56</v>
@@ -2578,7 +2577,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A10" s="17" t="s">
         <v>134</v>
       </c>
@@ -2586,7 +2585,7 @@
         <v>172</v>
       </c>
       <c r="C10" s="17" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="D10" s="17" t="s">
         <v>57</v>
@@ -2599,7 +2598,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="22.5" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A11" s="17" t="s">
         <v>135</v>
       </c>
@@ -2607,7 +2606,7 @@
         <v>172</v>
       </c>
       <c r="C11" s="17" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="D11" s="17" t="s">
         <v>58</v>
@@ -2620,7 +2619,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="12" spans="1:9" ht="22.5" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A12" s="17" t="s">
         <v>132</v>
       </c>
@@ -2628,7 +2627,7 @@
         <v>172</v>
       </c>
       <c r="C12" s="17" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="D12" s="17" t="s">
         <v>59</v>
@@ -2645,7 +2644,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="13" spans="1:9" ht="22.5" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A13" s="17" t="s">
         <v>135</v>
       </c>
@@ -2653,7 +2652,7 @@
         <v>172</v>
       </c>
       <c r="C13" s="17" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="D13" s="17" t="s">
         <v>60</v>
@@ -2664,7 +2663,7 @@
       <c r="H13" s="16"/>
       <c r="I13" s="16"/>
     </row>
-    <row r="14" spans="1:9" ht="22.5" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A14" s="17" t="s">
         <v>132</v>
       </c>
@@ -2672,7 +2671,7 @@
         <v>172</v>
       </c>
       <c r="C14" s="17" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="D14" s="17" t="s">
         <v>61</v>
@@ -2683,7 +2682,7 @@
       <c r="H14" s="16"/>
       <c r="I14" s="16"/>
     </row>
-    <row r="15" spans="1:9" ht="22.5" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A15" s="17" t="s">
         <v>135</v>
       </c>
@@ -2691,7 +2690,7 @@
         <v>172</v>
       </c>
       <c r="C15" s="17" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="D15" s="17" t="s">
         <v>62</v>
@@ -2702,7 +2701,7 @@
       <c r="H15" s="16"/>
       <c r="I15" s="16"/>
     </row>
-    <row r="16" spans="1:9" ht="22.5" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A16" s="17" t="s">
         <v>132</v>
       </c>
@@ -2710,7 +2709,7 @@
         <v>172</v>
       </c>
       <c r="C16" s="17" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="D16" s="17" t="s">
         <v>63</v>
@@ -2721,7 +2720,7 @@
       <c r="H16" s="16"/>
       <c r="I16" s="16"/>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A17" s="17" t="s">
         <v>131</v>
       </c>
@@ -2729,7 +2728,7 @@
         <v>172</v>
       </c>
       <c r="C17" s="17" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="D17" s="17" t="s">
         <v>64</v>
@@ -2744,7 +2743,7 @@
       </c>
       <c r="I17" s="16"/>
     </row>
-    <row r="18" spans="1:9" ht="22.5" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:9" ht="22" x14ac:dyDescent="0.15">
       <c r="A18" s="17" t="s">
         <v>130</v>
       </c>
@@ -2752,7 +2751,7 @@
         <v>172</v>
       </c>
       <c r="C18" s="17" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="D18" s="17" t="s">
         <v>65</v>
@@ -2767,7 +2766,7 @@
       </c>
       <c r="I18" s="16"/>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A19" s="9" t="s">
         <v>133</v>
       </c>
@@ -2775,7 +2774,7 @@
         <v>172</v>
       </c>
       <c r="C19" s="17" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="D19" s="17" t="s">
         <v>66</v>
@@ -2786,7 +2785,7 @@
       <c r="H19" s="16"/>
       <c r="I19" s="16"/>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A20" s="9" t="s">
         <v>134</v>
       </c>
@@ -2794,7 +2793,7 @@
         <v>172</v>
       </c>
       <c r="C20" s="17" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="D20" s="17" t="s">
         <v>67</v>
@@ -2805,7 +2804,7 @@
       <c r="H20" s="16"/>
       <c r="I20" s="16"/>
     </row>
-    <row r="21" spans="1:9" ht="22.5" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A21" s="9" t="s">
         <v>135</v>
       </c>
@@ -2813,7 +2812,7 @@
         <v>172</v>
       </c>
       <c r="C21" s="17" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="D21" s="17" t="s">
         <v>87</v>
@@ -2824,7 +2823,7 @@
       <c r="H21" s="16"/>
       <c r="I21" s="16"/>
     </row>
-    <row r="22" spans="1:9" ht="22.5" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A22" s="9" t="s">
         <v>132</v>
       </c>
@@ -2832,7 +2831,7 @@
         <v>172</v>
       </c>
       <c r="C22" s="17" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="D22" s="17" t="s">
         <v>68</v>
@@ -2847,7 +2846,7 @@
       </c>
       <c r="I22" s="16"/>
     </row>
-    <row r="23" spans="1:9" ht="22.5" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A23" s="9" t="s">
         <v>135</v>
       </c>
@@ -2855,7 +2854,7 @@
         <v>172</v>
       </c>
       <c r="C23" s="17" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="D23" s="17" t="s">
         <v>78</v>
@@ -2866,7 +2865,7 @@
       <c r="H23" s="16"/>
       <c r="I23" s="16"/>
     </row>
-    <row r="24" spans="1:9" ht="22.5" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A24" s="9" t="s">
         <v>132</v>
       </c>
@@ -2874,7 +2873,7 @@
         <v>172</v>
       </c>
       <c r="C24" s="17" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="D24" s="17" t="s">
         <v>69</v>
@@ -2885,7 +2884,7 @@
       <c r="H24" s="16"/>
       <c r="I24" s="16"/>
     </row>
-    <row r="25" spans="1:9" ht="22.5" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A25" s="9" t="s">
         <v>135</v>
       </c>
@@ -2893,7 +2892,7 @@
         <v>172</v>
       </c>
       <c r="C25" s="17" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="D25" s="17" t="s">
         <v>79</v>
@@ -2904,7 +2903,7 @@
       <c r="H25" s="16"/>
       <c r="I25" s="16"/>
     </row>
-    <row r="26" spans="1:9" ht="22.5" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A26" s="9" t="s">
         <v>132</v>
       </c>
@@ -2912,7 +2911,7 @@
         <v>172</v>
       </c>
       <c r="C26" s="17" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="D26" s="17" t="s">
         <v>80</v>
@@ -2923,7 +2922,7 @@
       <c r="H26" s="16"/>
       <c r="I26" s="16"/>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A27" s="9" t="s">
         <v>131</v>
       </c>
@@ -2931,7 +2930,7 @@
         <v>172</v>
       </c>
       <c r="C27" s="17" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="D27" s="17" t="s">
         <v>81</v>
@@ -2946,7 +2945,7 @@
       </c>
       <c r="I27" s="16"/>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A28" s="9" t="s">
         <v>130</v>
       </c>
@@ -2954,7 +2953,7 @@
         <v>172</v>
       </c>
       <c r="C28" s="17" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="D28" s="17" t="s">
         <v>82</v>
@@ -2969,7 +2968,7 @@
       </c>
       <c r="I28" s="16"/>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A29" s="9" t="s">
         <v>133</v>
       </c>
@@ -2977,7 +2976,7 @@
         <v>172</v>
       </c>
       <c r="C29" s="17" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="D29" s="17" t="s">
         <v>83</v>
@@ -2988,7 +2987,7 @@
       <c r="H29" s="16"/>
       <c r="I29" s="16"/>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A30" s="9" t="s">
         <v>134</v>
       </c>
@@ -2996,7 +2995,7 @@
         <v>172</v>
       </c>
       <c r="C30" s="17" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="D30" s="17" t="s">
         <v>84</v>
@@ -3007,7 +3006,7 @@
       <c r="H30" s="16"/>
       <c r="I30" s="16"/>
     </row>
-    <row r="31" spans="1:9" ht="22.5" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A31" s="9" t="s">
         <v>135</v>
       </c>
@@ -3015,7 +3014,7 @@
         <v>172</v>
       </c>
       <c r="C31" s="17" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="D31" s="17" t="s">
         <v>88</v>
@@ -3026,7 +3025,7 @@
       <c r="H31" s="16"/>
       <c r="I31" s="16"/>
     </row>
-    <row r="32" spans="1:9" ht="22.5" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A32" s="9" t="s">
         <v>132</v>
       </c>
@@ -3034,7 +3033,7 @@
         <v>172</v>
       </c>
       <c r="C32" s="17" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="D32" s="17" t="s">
         <v>85</v>
@@ -3049,7 +3048,7 @@
       </c>
       <c r="I32" s="16"/>
     </row>
-    <row r="33" spans="1:9" ht="22.5" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A33" s="9" t="s">
         <v>135</v>
       </c>
@@ -3057,7 +3056,7 @@
         <v>172</v>
       </c>
       <c r="C33" s="17" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="D33" s="17" t="s">
         <v>90</v>
@@ -3068,7 +3067,7 @@
       <c r="H33" s="16"/>
       <c r="I33" s="16"/>
     </row>
-    <row r="34" spans="1:9" ht="22.5" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A34" s="9" t="s">
         <v>132</v>
       </c>
@@ -3076,7 +3075,7 @@
         <v>172</v>
       </c>
       <c r="C34" s="17" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="D34" s="17" t="s">
         <v>89</v>
@@ -3087,7 +3086,7 @@
       <c r="H34" s="16"/>
       <c r="I34" s="16"/>
     </row>
-    <row r="35" spans="1:9" ht="22.5" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A35" s="9" t="s">
         <v>135</v>
       </c>
@@ -3095,7 +3094,7 @@
         <v>172</v>
       </c>
       <c r="C35" s="17" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="D35" s="17" t="s">
         <v>91</v>
@@ -3106,7 +3105,7 @@
       <c r="H35" s="16"/>
       <c r="I35" s="16"/>
     </row>
-    <row r="36" spans="1:9" ht="22.5" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A36" s="9" t="s">
         <v>132</v>
       </c>
@@ -3114,7 +3113,7 @@
         <v>172</v>
       </c>
       <c r="C36" s="17" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="D36" s="17" t="s">
         <v>86</v>
@@ -3125,7 +3124,7 @@
       <c r="H36" s="16"/>
       <c r="I36" s="16"/>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A37" s="9" t="s">
         <v>131</v>
       </c>
@@ -3133,7 +3132,7 @@
         <v>172</v>
       </c>
       <c r="C37" s="17" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="D37" s="17" t="s">
         <v>96</v>
@@ -3146,7 +3145,7 @@
       </c>
       <c r="I37" s="16"/>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A38" s="9" t="s">
         <v>130</v>
       </c>
@@ -3154,7 +3153,7 @@
         <v>172</v>
       </c>
       <c r="C38" s="17" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="D38" s="17" t="s">
         <v>97</v>
@@ -3167,7 +3166,7 @@
       </c>
       <c r="I38" s="16"/>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A39" s="9" t="s">
         <v>133</v>
       </c>
@@ -3175,7 +3174,7 @@
         <v>172</v>
       </c>
       <c r="C39" s="17" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="D39" s="17" t="s">
         <v>98</v>
@@ -3186,7 +3185,7 @@
       <c r="H39" s="16"/>
       <c r="I39" s="16"/>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A40" s="9" t="s">
         <v>134</v>
       </c>
@@ -3194,7 +3193,7 @@
         <v>172</v>
       </c>
       <c r="C40" s="17" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="D40" s="17" t="s">
         <v>99</v>
@@ -3205,7 +3204,7 @@
       <c r="H40" s="16"/>
       <c r="I40" s="16"/>
     </row>
-    <row r="41" spans="1:9" ht="22.5" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A41" s="9" t="s">
         <v>135</v>
       </c>
@@ -3213,7 +3212,7 @@
         <v>172</v>
       </c>
       <c r="C41" s="17" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="D41" s="17" t="s">
         <v>100</v>
@@ -3224,7 +3223,7 @@
       <c r="H41" s="16"/>
       <c r="I41" s="16"/>
     </row>
-    <row r="42" spans="1:9" ht="22.5" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A42" s="9" t="s">
         <v>132</v>
       </c>
@@ -3232,7 +3231,7 @@
         <v>172</v>
       </c>
       <c r="C42" s="17" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="D42" s="17" t="s">
         <v>101</v>
@@ -3245,7 +3244,7 @@
       </c>
       <c r="I42" s="16"/>
     </row>
-    <row r="43" spans="1:9" ht="22.5" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A43" s="9" t="s">
         <v>135</v>
       </c>
@@ -3253,7 +3252,7 @@
         <v>172</v>
       </c>
       <c r="C43" s="17" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="D43" s="17" t="s">
         <v>102</v>
@@ -3264,7 +3263,7 @@
       <c r="H43" s="16"/>
       <c r="I43" s="16"/>
     </row>
-    <row r="44" spans="1:9" ht="22.5" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A44" s="9" t="s">
         <v>132</v>
       </c>
@@ -3272,7 +3271,7 @@
         <v>172</v>
       </c>
       <c r="C44" s="17" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="D44" s="17" t="s">
         <v>103</v>
@@ -3283,7 +3282,7 @@
       <c r="H44" s="16"/>
       <c r="I44" s="16"/>
     </row>
-    <row r="45" spans="1:9" ht="22.5" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A45" s="9" t="s">
         <v>135</v>
       </c>
@@ -3291,7 +3290,7 @@
         <v>172</v>
       </c>
       <c r="C45" s="17" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="D45" s="17" t="s">
         <v>104</v>
@@ -3302,7 +3301,7 @@
       <c r="H45" s="16"/>
       <c r="I45" s="16"/>
     </row>
-    <row r="46" spans="1:9" ht="22.5" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A46" s="9" t="s">
         <v>132</v>
       </c>
@@ -3310,7 +3309,7 @@
         <v>172</v>
       </c>
       <c r="C46" s="17" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="D46" s="17" t="s">
         <v>105</v>
@@ -3336,7 +3335,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
@@ -3346,30 +3345,30 @@
       <selection pane="bottomRight" activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="11" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="16.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="41.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="33.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="9.140625" style="2"/>
+    <col min="1" max="1" width="16.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.1640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="41.5" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.5" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="33.1640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="9.1640625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A1" s="22" t="s">
         <v>186</v>
       </c>
       <c r="B1" s="22"/>
       <c r="C1" s="22" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="D1" s="22"/>
       <c r="E1" s="19" t="s">
-        <v>291</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A2" s="7" t="s">
         <v>187</v>
       </c>
@@ -3377,16 +3376,16 @@
         <v>188</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="E2" s="7" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A3" s="9" t="s">
         <v>151</v>
       </c>
@@ -3394,16 +3393,16 @@
         <v>110</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="D3" s="9" t="s">
         <v>184</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>319</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A4" s="9" t="s">
         <v>112</v>
       </c>
@@ -3411,16 +3410,16 @@
         <v>110</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="D4" s="9" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>317</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A5" s="9" t="s">
         <v>150</v>
       </c>
@@ -3428,13 +3427,13 @@
         <v>110</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="D5" s="9" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
     </row>
   </sheetData>
@@ -3448,42 +3447,42 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F13"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="4" ySplit="2" topLeftCell="E3" activePane="bottomRight" state="frozenSplit"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="E3" sqref="E3:F3"/>
+      <selection pane="bottomRight" activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="38.140625" defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="38.1640625" defaultRowHeight="11" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="79.42578125" style="11" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.140625" style="11" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="36.140625" style="11" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="21.42578125" style="11" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="43.28515625" style="11" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="45.140625" style="11" bestFit="1" customWidth="1"/>
-    <col min="7" max="16384" width="38.140625" style="11"/>
+    <col min="1" max="1" width="79.5" style="11" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.1640625" style="11" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="36.1640625" style="11" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.5" style="11" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="43.33203125" style="11" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="45.1640625" style="11" bestFit="1" customWidth="1"/>
+    <col min="7" max="16384" width="38.1640625" style="11"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A1" s="22" t="s">
         <v>186</v>
       </c>
       <c r="B1" s="22"/>
       <c r="C1" s="22" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="D1" s="22"/>
       <c r="E1" s="22" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="F1" s="22"/>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A2" s="7" t="s">
         <v>187</v>
       </c>
@@ -3491,10 +3490,10 @@
         <v>188</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="E2" s="7" t="s">
         <v>189</v>
@@ -3503,7 +3502,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="3" spans="1:6" s="2" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" s="2" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="9" t="s">
         <v>122</v>
       </c>
@@ -3511,19 +3510,19 @@
         <v>110</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="D3" s="9" t="s">
         <v>1</v>
       </c>
       <c r="E3" s="3" t="s">
+        <v>320</v>
+      </c>
+      <c r="F3" s="3" t="s">
         <v>321</v>
       </c>
-      <c r="F3" s="3" t="s">
-        <v>322</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="4" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A4" s="9" t="s">
         <v>151</v>
       </c>
@@ -3531,19 +3530,19 @@
         <v>110</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="D4" s="9" t="s">
         <v>184</v>
       </c>
-      <c r="E4" s="3" t="s">
-        <v>321</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>322</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" s="2" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E4" s="11" t="s">
+        <v>318</v>
+      </c>
+      <c r="F4" s="11" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" s="2" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="9" t="s">
         <v>121</v>
       </c>
@@ -3551,7 +3550,7 @@
         <v>110</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="D5" s="9" t="s">
         <v>2</v>
@@ -3563,7 +3562,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:6" s="2" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" s="2" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="18" t="s">
         <v>144</v>
       </c>
@@ -3571,19 +3570,19 @@
         <v>172</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="D6" s="9" t="s">
         <v>181</v>
       </c>
       <c r="E6" s="3" t="s">
+        <v>320</v>
+      </c>
+      <c r="F6" s="3" t="s">
         <v>321</v>
       </c>
-      <c r="F6" s="3" t="s">
-        <v>322</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" s="2" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="7" spans="1:6" s="2" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="18" t="s">
         <v>145</v>
       </c>
@@ -3591,7 +3590,7 @@
         <v>172</v>
       </c>
       <c r="C7" s="9" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="D7" s="9" t="s">
         <v>182</v>
@@ -3603,7 +3602,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:6" s="2" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6" s="2" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="18" t="s">
         <v>146</v>
       </c>
@@ -3611,7 +3610,7 @@
         <v>172</v>
       </c>
       <c r="C8" s="9" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="D8" s="9" t="s">
         <v>183</v>
@@ -3623,7 +3622,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:6" s="2" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:6" s="2" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="9" t="s">
         <v>166</v>
       </c>
@@ -3631,10 +3630,10 @@
         <v>110</v>
       </c>
       <c r="C9" s="9" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="D9" s="9" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="E9" s="3" t="b">
         <v>1</v>
@@ -3643,7 +3642,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:6" s="2" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:6" s="2" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="9" t="s">
         <v>166</v>
       </c>
@@ -3651,10 +3650,10 @@
         <v>172</v>
       </c>
       <c r="C10" s="9" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="D10" s="9" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="E10" s="3" t="b">
         <v>1</v>
@@ -3663,7 +3662,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:6" s="2" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:6" s="2" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="9" t="s">
         <v>166</v>
       </c>
@@ -3671,10 +3670,10 @@
         <v>172</v>
       </c>
       <c r="C11" s="9" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="D11" s="9" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="E11" s="3" t="b">
         <v>1</v>
@@ -3683,7 +3682,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:6" s="2" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:6" s="2" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="9" t="s">
         <v>167</v>
       </c>
@@ -3691,7 +3690,7 @@
         <v>110</v>
       </c>
       <c r="C12" s="9" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="D12" s="9" t="s">
         <v>191</v>
@@ -3703,7 +3702,7 @@
         <v>79.3</v>
       </c>
     </row>
-    <row r="13" spans="1:6" s="2" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:6" s="2" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="9" t="s">
         <v>167</v>
       </c>
@@ -3711,10 +3710,10 @@
         <v>110</v>
       </c>
       <c r="C13" s="9" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="D13" s="9" t="s">
-        <v>192</v>
+        <v>324</v>
       </c>
       <c r="E13" s="8">
         <v>2514.9</v>
@@ -3734,43 +3733,43 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S55"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="4" ySplit="2" topLeftCell="E3" activePane="bottomRight" state="frozenSplit"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
       <selection pane="bottomRight" activeCell="E8" sqref="E8:S8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="32.85546875" defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="32.83203125" defaultRowHeight="11" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="55" style="21" customWidth="1"/>
-    <col min="2" max="2" width="7.140625" style="21" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.1640625" style="21" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="18" style="21" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="40.5703125" style="21" bestFit="1" customWidth="1"/>
-    <col min="5" max="10" width="27.5703125" style="21" bestFit="1" customWidth="1"/>
-    <col min="11" max="19" width="25.7109375" style="21" bestFit="1" customWidth="1"/>
-    <col min="20" max="16384" width="32.85546875" style="21"/>
+    <col min="4" max="4" width="40.5" style="21" bestFit="1" customWidth="1"/>
+    <col min="5" max="10" width="27.5" style="21" bestFit="1" customWidth="1"/>
+    <col min="11" max="19" width="25.6640625" style="21" bestFit="1" customWidth="1"/>
+    <col min="20" max="16384" width="32.83203125" style="21"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A1" s="22" t="s">
         <v>186</v>
       </c>
       <c r="B1" s="22"/>
       <c r="C1" s="22" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="D1" s="22"/>
       <c r="E1" s="24" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="F1" s="25"/>
       <c r="G1" s="26"/>
       <c r="H1" s="27" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="I1" s="28"/>
       <c r="J1" s="28"/>
@@ -3784,7 +3783,7 @@
       <c r="R1" s="28"/>
       <c r="S1" s="29"/>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A2" s="7" t="s">
         <v>187</v>
       </c>
@@ -3792,10 +3791,10 @@
         <v>188</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="E2" s="10" t="s">
         <v>189</v>
@@ -3843,7 +3842,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="3" spans="1:19" ht="22.5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A3" s="9" t="s">
         <v>122</v>
       </c>
@@ -3854,182 +3853,182 @@
         <v>1</v>
       </c>
       <c r="D3" s="9" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="E3" s="3" t="s">
+        <v>320</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>320</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>320</v>
+      </c>
+      <c r="H3" s="3" t="s">
         <v>321</v>
       </c>
-      <c r="F3" s="3" t="s">
+      <c r="I3" s="3" t="s">
         <v>321</v>
       </c>
-      <c r="G3" s="3" t="s">
+      <c r="J3" s="3" t="s">
         <v>321</v>
       </c>
-      <c r="H3" s="3" t="s">
-        <v>322</v>
-      </c>
-      <c r="I3" s="3" t="s">
-        <v>322</v>
-      </c>
-      <c r="J3" s="3" t="s">
-        <v>322</v>
-      </c>
       <c r="K3" s="3" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="L3" s="3" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="M3" s="3" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="N3" s="3" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="O3" s="3" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="P3" s="3" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="Q3" s="3" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="R3" s="3" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="S3" s="3" t="s">
-        <v>322</v>
-      </c>
-    </row>
-    <row r="4" spans="1:19" ht="22.5" x14ac:dyDescent="0.2">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A4" s="9" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="B4" s="9" t="s">
         <v>110</v>
       </c>
       <c r="C4" s="9" t="s">
+        <v>269</v>
+      </c>
+      <c r="D4" s="9" t="s">
+        <v>323</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>320</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>320</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>320</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>321</v>
+      </c>
+      <c r="I4" s="3" t="s">
+        <v>321</v>
+      </c>
+      <c r="J4" s="3" t="s">
+        <v>321</v>
+      </c>
+      <c r="K4" s="3" t="s">
+        <v>321</v>
+      </c>
+      <c r="L4" s="3" t="s">
+        <v>321</v>
+      </c>
+      <c r="M4" s="3" t="s">
+        <v>321</v>
+      </c>
+      <c r="N4" s="3" t="s">
+        <v>321</v>
+      </c>
+      <c r="O4" s="3" t="s">
+        <v>321</v>
+      </c>
+      <c r="P4" s="3" t="s">
+        <v>321</v>
+      </c>
+      <c r="Q4" s="3" t="s">
+        <v>321</v>
+      </c>
+      <c r="R4" s="3" t="s">
+        <v>321</v>
+      </c>
+      <c r="S4" s="3" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.15">
+      <c r="A5" s="9" t="s">
         <v>270</v>
       </c>
-      <c r="D4" s="9" t="s">
-        <v>324</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>321</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>321</v>
-      </c>
-      <c r="G4" s="3" t="s">
-        <v>321</v>
-      </c>
-      <c r="H4" s="3" t="s">
-        <v>322</v>
-      </c>
-      <c r="I4" s="3" t="s">
-        <v>322</v>
-      </c>
-      <c r="J4" s="3" t="s">
-        <v>322</v>
-      </c>
-      <c r="K4" s="3" t="s">
-        <v>322</v>
-      </c>
-      <c r="L4" s="3" t="s">
-        <v>322</v>
-      </c>
-      <c r="M4" s="3" t="s">
-        <v>322</v>
-      </c>
-      <c r="N4" s="3" t="s">
-        <v>322</v>
-      </c>
-      <c r="O4" s="3" t="s">
-        <v>322</v>
-      </c>
-      <c r="P4" s="3" t="s">
-        <v>322</v>
-      </c>
-      <c r="Q4" s="3" t="s">
-        <v>322</v>
-      </c>
-      <c r="R4" s="3" t="s">
-        <v>322</v>
-      </c>
-      <c r="S4" s="3" t="s">
-        <v>322</v>
-      </c>
-    </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A5" s="9" t="s">
+      <c r="B5" s="9" t="s">
+        <v>172</v>
+      </c>
+      <c r="C5" s="9" t="s">
         <v>271</v>
       </c>
-      <c r="B5" s="9" t="s">
-        <v>172</v>
-      </c>
-      <c r="C5" s="9" t="s">
+      <c r="D5" s="9" t="s">
+        <v>315</v>
+      </c>
+      <c r="E5" s="12" t="s">
         <v>272</v>
       </c>
-      <c r="D5" s="9" t="s">
-        <v>316</v>
-      </c>
-      <c r="E5" s="12" t="s">
-        <v>273</v>
-      </c>
       <c r="F5" s="12" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="G5" s="12" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="H5" s="12" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="I5" s="12" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="J5" s="12" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="K5" s="12" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="L5" s="12" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="M5" s="12" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="N5" s="12" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="O5" s="12" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="P5" s="12" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="Q5" s="12" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="R5" s="12" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="S5" s="12" t="s">
-        <v>273</v>
-      </c>
-    </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.2">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A6" s="9"/>
       <c r="B6" s="9" t="s">
         <v>110</v>
       </c>
       <c r="C6" s="9" t="s">
+        <v>285</v>
+      </c>
+      <c r="D6" s="9" t="s">
         <v>286</v>
-      </c>
-      <c r="D6" s="9" t="s">
-        <v>287</v>
       </c>
       <c r="E6" s="5">
         <v>1</v>
@@ -4077,7 +4076,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A7" s="9" t="s">
         <v>171</v>
       </c>
@@ -4085,10 +4084,10 @@
         <v>110</v>
       </c>
       <c r="C7" s="9" t="s">
+        <v>287</v>
+      </c>
+      <c r="D7" s="9" t="s">
         <v>288</v>
-      </c>
-      <c r="D7" s="9" t="s">
-        <v>289</v>
       </c>
       <c r="E7" s="5">
         <v>1</v>
@@ -4136,7 +4135,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A8" s="9" t="s">
         <v>120</v>
       </c>
@@ -4147,7 +4146,7 @@
         <v>0</v>
       </c>
       <c r="D8" s="9" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="E8" s="1">
         <v>83834</v>
@@ -4195,18 +4194,18 @@
         <v>30309</v>
       </c>
     </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A9" s="9" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="B9" s="9" t="s">
         <v>110</v>
       </c>
       <c r="C9" s="9" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="D9" s="9" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="E9" s="1" t="b">
         <v>1</v>
@@ -4254,18 +4253,18 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A10" s="9" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="B10" s="9" t="s">
         <v>172</v>
       </c>
       <c r="C10" s="9" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="D10" s="9" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="E10" s="1" t="b">
         <v>1</v>
@@ -4313,18 +4312,18 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A11" s="9" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="B11" s="9" t="s">
         <v>172</v>
       </c>
       <c r="C11" s="9" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="D11" s="9" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="E11" s="1" t="b">
         <v>1</v>
@@ -4372,7 +4371,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A12" s="18" t="s">
         <v>143</v>
       </c>
@@ -4399,7 +4398,7 @@
       <c r="R12" s="4"/>
       <c r="S12" s="4"/>
     </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A13" s="18" t="s">
         <v>142</v>
       </c>
@@ -4426,7 +4425,7 @@
       <c r="R13" s="4"/>
       <c r="S13" s="4"/>
     </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A14" s="18" t="s">
         <v>136</v>
       </c>
@@ -4453,7 +4452,7 @@
       <c r="R14" s="4"/>
       <c r="S14" s="4"/>
     </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A15" s="18" t="s">
         <v>137</v>
       </c>
@@ -4480,7 +4479,7 @@
       <c r="R15" s="4"/>
       <c r="S15" s="4"/>
     </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A16" s="18" t="s">
         <v>138</v>
       </c>
@@ -4507,7 +4506,7 @@
       <c r="R16" s="4"/>
       <c r="S16" s="4"/>
     </row>
-    <row r="17" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A17" s="18" t="s">
         <v>139</v>
       </c>
@@ -4534,7 +4533,7 @@
       <c r="R17" s="4"/>
       <c r="S17" s="4"/>
     </row>
-    <row r="18" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A18" s="18" t="s">
         <v>140</v>
       </c>
@@ -4561,7 +4560,7 @@
       <c r="R18" s="4"/>
       <c r="S18" s="4"/>
     </row>
-    <row r="19" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A19" s="18" t="s">
         <v>141</v>
       </c>
@@ -4588,7 +4587,7 @@
       <c r="R19" s="4"/>
       <c r="S19" s="4"/>
     </row>
-    <row r="20" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A20" s="9" t="s">
         <v>123</v>
       </c>
@@ -4615,7 +4614,7 @@
       <c r="R20" s="1"/>
       <c r="S20" s="1"/>
     </row>
-    <row r="21" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A21" s="9" t="s">
         <v>124</v>
       </c>
@@ -4642,7 +4641,7 @@
       <c r="R21" s="1"/>
       <c r="S21" s="1"/>
     </row>
-    <row r="22" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A22" s="9" t="s">
         <v>125</v>
       </c>
@@ -4669,7 +4668,7 @@
       <c r="R22" s="1"/>
       <c r="S22" s="1"/>
     </row>
-    <row r="23" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A23" s="9" t="s">
         <v>126</v>
       </c>
@@ -4696,7 +4695,7 @@
       <c r="R23" s="4"/>
       <c r="S23" s="4"/>
     </row>
-    <row r="24" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A24" s="9" t="s">
         <v>127</v>
       </c>
@@ -4723,7 +4722,7 @@
       <c r="R24" s="4"/>
       <c r="S24" s="4"/>
     </row>
-    <row r="25" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A25" s="9" t="s">
         <v>127</v>
       </c>
@@ -4750,7 +4749,7 @@
       <c r="R25" s="4"/>
       <c r="S25" s="4"/>
     </row>
-    <row r="26" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A26" s="9" t="s">
         <v>127</v>
       </c>
@@ -4777,7 +4776,7 @@
       <c r="R26" s="4"/>
       <c r="S26" s="4"/>
     </row>
-    <row r="27" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A27" s="9" t="s">
         <v>127</v>
       </c>
@@ -4804,7 +4803,7 @@
       <c r="R27" s="4"/>
       <c r="S27" s="4"/>
     </row>
-    <row r="28" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A28" s="9" t="s">
         <v>127</v>
       </c>
@@ -4831,7 +4830,7 @@
       <c r="R28" s="4"/>
       <c r="S28" s="4"/>
     </row>
-    <row r="29" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A29" s="9" t="s">
         <v>127</v>
       </c>
@@ -4858,7 +4857,7 @@
       <c r="R29" s="4"/>
       <c r="S29" s="4"/>
     </row>
-    <row r="30" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A30" s="9" t="s">
         <v>127</v>
       </c>
@@ -4885,7 +4884,7 @@
       <c r="R30" s="4"/>
       <c r="S30" s="4"/>
     </row>
-    <row r="31" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A31" s="9" t="s">
         <v>127</v>
       </c>
@@ -4912,7 +4911,7 @@
       <c r="R31" s="4"/>
       <c r="S31" s="4"/>
     </row>
-    <row r="32" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A32" s="9" t="s">
         <v>123</v>
       </c>
@@ -4939,7 +4938,7 @@
       <c r="R32" s="1"/>
       <c r="S32" s="1"/>
     </row>
-    <row r="33" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A33" s="9" t="s">
         <v>124</v>
       </c>
@@ -4966,7 +4965,7 @@
       <c r="R33" s="1"/>
       <c r="S33" s="1"/>
     </row>
-    <row r="34" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A34" s="9" t="s">
         <v>125</v>
       </c>
@@ -4993,7 +4992,7 @@
       <c r="R34" s="1"/>
       <c r="S34" s="1"/>
     </row>
-    <row r="35" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A35" s="9" t="s">
         <v>126</v>
       </c>
@@ -5020,7 +5019,7 @@
       <c r="R35" s="4"/>
       <c r="S35" s="4"/>
     </row>
-    <row r="36" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A36" s="9" t="s">
         <v>127</v>
       </c>
@@ -5047,7 +5046,7 @@
       <c r="R36" s="4"/>
       <c r="S36" s="4"/>
     </row>
-    <row r="37" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A37" s="9" t="s">
         <v>127</v>
       </c>
@@ -5074,7 +5073,7 @@
       <c r="R37" s="4"/>
       <c r="S37" s="4"/>
     </row>
-    <row r="38" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A38" s="9" t="s">
         <v>127</v>
       </c>
@@ -5101,7 +5100,7 @@
       <c r="R38" s="4"/>
       <c r="S38" s="4"/>
     </row>
-    <row r="39" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A39" s="9" t="s">
         <v>127</v>
       </c>
@@ -5128,7 +5127,7 @@
       <c r="R39" s="4"/>
       <c r="S39" s="4"/>
     </row>
-    <row r="40" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A40" s="9" t="s">
         <v>127</v>
       </c>
@@ -5155,7 +5154,7 @@
       <c r="R40" s="4"/>
       <c r="S40" s="4"/>
     </row>
-    <row r="41" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A41" s="9" t="s">
         <v>127</v>
       </c>
@@ -5182,7 +5181,7 @@
       <c r="R41" s="4"/>
       <c r="S41" s="4"/>
     </row>
-    <row r="42" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A42" s="9" t="s">
         <v>127</v>
       </c>
@@ -5209,7 +5208,7 @@
       <c r="R42" s="4"/>
       <c r="S42" s="4"/>
     </row>
-    <row r="43" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A43" s="9" t="s">
         <v>127</v>
       </c>
@@ -5236,7 +5235,7 @@
       <c r="R43" s="4"/>
       <c r="S43" s="4"/>
     </row>
-    <row r="44" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A44" s="9" t="s">
         <v>123</v>
       </c>
@@ -5263,7 +5262,7 @@
       <c r="R44" s="1"/>
       <c r="S44" s="1"/>
     </row>
-    <row r="45" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A45" s="9" t="s">
         <v>124</v>
       </c>
@@ -5290,7 +5289,7 @@
       <c r="R45" s="1"/>
       <c r="S45" s="1"/>
     </row>
-    <row r="46" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A46" s="9" t="s">
         <v>125</v>
       </c>
@@ -5317,7 +5316,7 @@
       <c r="R46" s="1"/>
       <c r="S46" s="1"/>
     </row>
-    <row r="47" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A47" s="9" t="s">
         <v>126</v>
       </c>
@@ -5344,7 +5343,7 @@
       <c r="R47" s="4"/>
       <c r="S47" s="4"/>
     </row>
-    <row r="48" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A48" s="9" t="s">
         <v>127</v>
       </c>
@@ -5371,7 +5370,7 @@
       <c r="R48" s="4"/>
       <c r="S48" s="4"/>
     </row>
-    <row r="49" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A49" s="9" t="s">
         <v>127</v>
       </c>
@@ -5398,7 +5397,7 @@
       <c r="R49" s="4"/>
       <c r="S49" s="4"/>
     </row>
-    <row r="50" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A50" s="9" t="s">
         <v>127</v>
       </c>
@@ -5425,7 +5424,7 @@
       <c r="R50" s="4"/>
       <c r="S50" s="4"/>
     </row>
-    <row r="51" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A51" s="9" t="s">
         <v>127</v>
       </c>
@@ -5452,7 +5451,7 @@
       <c r="R51" s="4"/>
       <c r="S51" s="4"/>
     </row>
-    <row r="52" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A52" s="9" t="s">
         <v>127</v>
       </c>
@@ -5479,7 +5478,7 @@
       <c r="R52" s="4"/>
       <c r="S52" s="4"/>
     </row>
-    <row r="53" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A53" s="9" t="s">
         <v>127</v>
       </c>
@@ -5506,7 +5505,7 @@
       <c r="R53" s="4"/>
       <c r="S53" s="4"/>
     </row>
-    <row r="54" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A54" s="9" t="s">
         <v>127</v>
       </c>
@@ -5533,7 +5532,7 @@
       <c r="R54" s="4"/>
       <c r="S54" s="4"/>
     </row>
-    <row r="55" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A55" s="9" t="s">
         <v>127</v>
       </c>
@@ -5573,7 +5572,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F33"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
@@ -5583,33 +5582,33 @@
       <selection pane="bottomRight" activeCell="I36" sqref="I36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="16" defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="16" defaultRowHeight="11" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="57.85546875" style="11" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.140625" style="11" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="57.83203125" style="11" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.1640625" style="11" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="46" style="11" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="27.140625" style="11" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="38.28515625" style="11" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="27.1640625" style="11" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="38.33203125" style="11" bestFit="1" customWidth="1"/>
     <col min="7" max="16384" width="16" style="11"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A1" s="22" t="s">
         <v>186</v>
       </c>
       <c r="B1" s="22"/>
       <c r="C1" s="22" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="D1" s="22"/>
       <c r="E1" s="13" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="F1" s="13" t="s">
-        <v>313</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A2" s="7" t="s">
         <v>187</v>
       </c>
@@ -5617,10 +5616,10 @@
         <v>188</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="E2" s="7" t="s">
         <v>189</v>
@@ -5629,7 +5628,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="3" spans="1:6" s="2" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" s="2" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="9" t="s">
         <v>122</v>
       </c>
@@ -5637,19 +5636,19 @@
         <v>110</v>
       </c>
       <c r="C3" s="9" t="s">
+        <v>310</v>
+      </c>
+      <c r="D3" s="9" t="s">
         <v>311</v>
       </c>
-      <c r="D3" s="9" t="s">
-        <v>312</v>
-      </c>
       <c r="E3" s="3" t="s">
+        <v>320</v>
+      </c>
+      <c r="F3" s="3" t="s">
         <v>321</v>
       </c>
-      <c r="F3" s="3" t="s">
-        <v>322</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" s="2" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="4" spans="1:6" s="2" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="18" t="s">
         <v>156</v>
       </c>
@@ -5657,15 +5656,15 @@
         <v>110</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="D4" s="9" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
     </row>
-    <row r="5" spans="1:6" s="2" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" s="2" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="18" t="s">
         <v>152</v>
       </c>
@@ -5673,15 +5672,15 @@
         <v>172</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="D5" s="9" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
     </row>
-    <row r="6" spans="1:6" s="2" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" s="2" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="18" t="s">
         <v>153</v>
       </c>
@@ -5689,15 +5688,15 @@
         <v>172</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="D6" s="9" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
     </row>
-    <row r="7" spans="1:6" s="2" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6" s="2" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="18" t="s">
         <v>154</v>
       </c>
@@ -5705,15 +5704,15 @@
         <v>172</v>
       </c>
       <c r="C7" s="9" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="D7" s="9" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
     </row>
-    <row r="8" spans="1:6" s="2" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6" s="2" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="18" t="s">
         <v>155</v>
       </c>
@@ -5721,15 +5720,15 @@
         <v>172</v>
       </c>
       <c r="C8" s="9" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="D8" s="9" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
     </row>
-    <row r="9" spans="1:6" s="2" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:6" s="2" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="18" t="s">
         <v>157</v>
       </c>
@@ -5737,15 +5736,15 @@
         <v>172</v>
       </c>
       <c r="C9" s="9" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="D9" s="9" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
     </row>
-    <row r="10" spans="1:6" s="2" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:6" s="2" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="18" t="s">
         <v>158</v>
       </c>
@@ -5753,15 +5752,15 @@
         <v>172</v>
       </c>
       <c r="C10" s="9" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="D10" s="9" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="E10" s="1"/>
       <c r="F10" s="1"/>
     </row>
-    <row r="11" spans="1:6" s="2" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:6" s="2" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="18" t="s">
         <v>159</v>
       </c>
@@ -5769,15 +5768,15 @@
         <v>172</v>
       </c>
       <c r="C11" s="9" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="D11" s="9" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="E11" s="1"/>
       <c r="F11" s="1"/>
     </row>
-    <row r="12" spans="1:6" s="2" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:6" s="2" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="18" t="s">
         <v>163</v>
       </c>
@@ -5785,15 +5784,15 @@
         <v>110</v>
       </c>
       <c r="C12" s="9" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="D12" s="9" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="E12" s="1"/>
       <c r="F12" s="1"/>
     </row>
-    <row r="13" spans="1:6" s="2" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:6" s="2" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="18" t="s">
         <v>160</v>
       </c>
@@ -5801,15 +5800,15 @@
         <v>110</v>
       </c>
       <c r="C13" s="9" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="D13" s="9" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="E13" s="1"/>
       <c r="F13" s="1"/>
     </row>
-    <row r="14" spans="1:6" s="2" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:6" s="2" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="18" t="s">
         <v>161</v>
       </c>
@@ -5817,15 +5816,15 @@
         <v>172</v>
       </c>
       <c r="C14" s="9" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="D14" s="9" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="E14" s="1"/>
       <c r="F14" s="1"/>
     </row>
-    <row r="15" spans="1:6" s="2" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:6" s="2" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="18" t="s">
         <v>162</v>
       </c>
@@ -5833,15 +5832,15 @@
         <v>172</v>
       </c>
       <c r="C15" s="9" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="D15" s="9" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="E15" s="1"/>
       <c r="F15" s="1"/>
     </row>
-    <row r="16" spans="1:6" s="2" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:6" s="2" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" s="18" t="s">
         <v>164</v>
       </c>
@@ -5849,15 +5848,15 @@
         <v>110</v>
       </c>
       <c r="C16" s="9" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="D16" s="9" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="E16" s="1"/>
       <c r="F16" s="1"/>
     </row>
-    <row r="17" spans="1:6" s="2" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:6" s="2" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" s="18" t="s">
         <v>165</v>
       </c>
@@ -5865,31 +5864,31 @@
         <v>110</v>
       </c>
       <c r="C17" s="9" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="D17" s="9" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="E17" s="1"/>
       <c r="F17" s="1"/>
     </row>
-    <row r="18" spans="1:6" s="2" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:6" s="2" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A18" s="18" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B18" s="18" t="s">
         <v>172</v>
       </c>
       <c r="C18" s="9" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="D18" s="9" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="E18" s="1"/>
       <c r="F18" s="1"/>
     </row>
-    <row r="19" spans="1:6" s="2" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:6" s="2" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A19" s="18" t="s">
         <v>156</v>
       </c>
@@ -5897,15 +5896,15 @@
         <v>110</v>
       </c>
       <c r="C19" s="9" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="D19" s="9" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="E19" s="1"/>
       <c r="F19" s="1"/>
     </row>
-    <row r="20" spans="1:6" s="2" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:6" s="2" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A20" s="18" t="s">
         <v>152</v>
       </c>
@@ -5913,15 +5912,15 @@
         <v>172</v>
       </c>
       <c r="C20" s="9" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="D20" s="9" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="E20" s="1"/>
       <c r="F20" s="1"/>
     </row>
-    <row r="21" spans="1:6" s="2" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:6" s="2" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A21" s="18" t="s">
         <v>153</v>
       </c>
@@ -5929,15 +5928,15 @@
         <v>172</v>
       </c>
       <c r="C21" s="9" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="D21" s="9" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="E21" s="1"/>
       <c r="F21" s="1"/>
     </row>
-    <row r="22" spans="1:6" s="2" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:6" s="2" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A22" s="18" t="s">
         <v>154</v>
       </c>
@@ -5945,15 +5944,15 @@
         <v>172</v>
       </c>
       <c r="C22" s="9" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="D22" s="9" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="E22" s="1"/>
       <c r="F22" s="1"/>
     </row>
-    <row r="23" spans="1:6" s="2" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:6" s="2" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A23" s="18" t="s">
         <v>155</v>
       </c>
@@ -5961,15 +5960,15 @@
         <v>172</v>
       </c>
       <c r="C23" s="9" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="D23" s="9" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="E23" s="1"/>
       <c r="F23" s="1"/>
     </row>
-    <row r="24" spans="1:6" s="2" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:6" s="2" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A24" s="18" t="s">
         <v>157</v>
       </c>
@@ -5977,15 +5976,15 @@
         <v>172</v>
       </c>
       <c r="C24" s="9" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="D24" s="9" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="E24" s="1"/>
       <c r="F24" s="1"/>
     </row>
-    <row r="25" spans="1:6" s="2" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:6" s="2" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A25" s="18" t="s">
         <v>158</v>
       </c>
@@ -5993,15 +5992,15 @@
         <v>172</v>
       </c>
       <c r="C25" s="9" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="D25" s="9" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="E25" s="1"/>
       <c r="F25" s="1"/>
     </row>
-    <row r="26" spans="1:6" s="2" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:6" s="2" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A26" s="18" t="s">
         <v>159</v>
       </c>
@@ -6009,15 +6008,15 @@
         <v>172</v>
       </c>
       <c r="C26" s="9" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="D26" s="9" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="E26" s="1"/>
       <c r="F26" s="1"/>
     </row>
-    <row r="27" spans="1:6" s="2" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:6" s="2" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A27" s="18" t="s">
         <v>163</v>
       </c>
@@ -6025,15 +6024,15 @@
         <v>110</v>
       </c>
       <c r="C27" s="9" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="D27" s="9" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="E27" s="1"/>
       <c r="F27" s="1"/>
     </row>
-    <row r="28" spans="1:6" s="2" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:6" s="2" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A28" s="18" t="s">
         <v>160</v>
       </c>
@@ -6041,15 +6040,15 @@
         <v>110</v>
       </c>
       <c r="C28" s="9" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="D28" s="9" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="E28" s="1"/>
       <c r="F28" s="1"/>
     </row>
-    <row r="29" spans="1:6" s="2" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:6" s="2" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A29" s="18" t="s">
         <v>161</v>
       </c>
@@ -6057,15 +6056,15 @@
         <v>172</v>
       </c>
       <c r="C29" s="9" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="D29" s="9" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="E29" s="1"/>
       <c r="F29" s="1"/>
     </row>
-    <row r="30" spans="1:6" s="2" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:6" s="2" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A30" s="18" t="s">
         <v>162</v>
       </c>
@@ -6073,15 +6072,15 @@
         <v>172</v>
       </c>
       <c r="C30" s="9" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="D30" s="9" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="E30" s="1"/>
       <c r="F30" s="1"/>
     </row>
-    <row r="31" spans="1:6" s="2" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:6" s="2" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A31" s="18" t="s">
         <v>164</v>
       </c>
@@ -6089,15 +6088,15 @@
         <v>110</v>
       </c>
       <c r="C31" s="9" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="D31" s="9" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="E31" s="1"/>
       <c r="F31" s="1"/>
     </row>
-    <row r="32" spans="1:6" s="2" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:6" s="2" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A32" s="18" t="s">
         <v>165</v>
       </c>
@@ -6105,26 +6104,26 @@
         <v>110</v>
       </c>
       <c r="C32" s="9" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="D32" s="9" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="E32" s="1"/>
       <c r="F32" s="1"/>
     </row>
-    <row r="33" spans="1:6" s="2" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:6" s="2" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A33" s="18" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B33" s="18" t="s">
         <v>172</v>
       </c>
       <c r="C33" s="9" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="D33" s="9" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E33" s="1"/>
       <c r="F33" s="1"/>

</xml_diff>

<commit_message>
Adding segment blueprint element counts
</commit_message>
<xml_diff>
--- a/src/test/resources/SBAC-IAB-FIXED-G11M-Winter-2017-2018.xlsx
+++ b/src/test/resources/SBAC-IAB-FIXED-G11M-Winter-2017-2018.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="440" windowWidth="28800" windowHeight="12440" tabRatio="644" activeTab="3"/>
+    <workbookView xWindow="-28800" yWindow="4780" windowWidth="28800" windowHeight="16640" tabRatio="644" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Package" sheetId="16" r:id="rId1"/>
@@ -3450,11 +3450,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F13"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="4" ySplit="2" topLeftCell="E3" activePane="bottomRight" state="frozenSplit"/>
+    <sheetView tabSelected="1" zoomScale="132" zoomScaleNormal="132" workbookViewId="0">
+      <pane xSplit="4" ySplit="2" topLeftCell="F3" activePane="bottomRight" state="frozenSplit"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="D14" sqref="D14"/>
+      <selection pane="bottomRight" activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="38.1640625" defaultRowHeight="11" x14ac:dyDescent="0.15"/>
@@ -3556,10 +3556,10 @@
         <v>2</v>
       </c>
       <c r="E5" s="5">
+        <v>1</v>
+      </c>
+      <c r="F5" s="5">
         <v>2</v>
-      </c>
-      <c r="F5" s="5">
-        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:6" s="2" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -3736,11 +3736,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S55"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <pane xSplit="4" ySplit="2" topLeftCell="E3" activePane="bottomRight" state="frozenSplit"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="E8" sqref="E8:S8"/>
+      <selection pane="bottomRight" activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="32.83203125" defaultRowHeight="11" x14ac:dyDescent="0.15"/>
@@ -3748,7 +3748,7 @@
     <col min="1" max="1" width="55" style="21" customWidth="1"/>
     <col min="2" max="2" width="7.1640625" style="21" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="18" style="21" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="40.5" style="21" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="31.83203125" style="21" customWidth="1"/>
     <col min="5" max="10" width="27.5" style="21" bestFit="1" customWidth="1"/>
     <col min="11" max="19" width="25.6640625" style="21" bestFit="1" customWidth="1"/>
     <col min="20" max="16384" width="32.83203125" style="21"/>

</xml_diff>

<commit_message>
Making test package id = test id. Updating blueprint mapper to consume scoring map
</commit_message>
<xml_diff>
--- a/src/test/resources/SBAC-IAB-FIXED-G11M-Winter-2017-2018.xlsx
+++ b/src/test/resources/SBAC-IAB-FIXED-G11M-Winter-2017-2018.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-30040" yWindow="4780" windowWidth="33460" windowHeight="17560" tabRatio="644" activeTab="5"/>
+    <workbookView xWindow="23320" yWindow="6280" windowWidth="28800" windowHeight="17560" tabRatio="644" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Package" sheetId="16" r:id="rId1"/>
@@ -20,6 +20,7 @@
     <sheet name="Tools" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="152511"/>
+  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
@@ -912,9 +913,6 @@
   </si>
   <si>
     <t>A string used to link forms of different segments</t>
-  </si>
-  <si>
-    <t>SBAC-IAB-FIXED-G11M</t>
   </si>
   <si>
     <t>IAB</t>
@@ -1838,6 +1836,9 @@
   </si>
   <si>
     <t>Masking</t>
+  </si>
+  <si>
+    <t>BlueprintElementId</t>
   </si>
 </sst>
 </file>
@@ -2955,7 +2956,7 @@
       <pane xSplit="4" ySplit="2" topLeftCell="E3" activePane="bottomRight" state="frozenSplit"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="A30" sqref="A30"/>
+      <selection pane="bottomRight" activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="11" x14ac:dyDescent="0.15"/>
@@ -3012,7 +3013,7 @@
         <v>194</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -3148,7 +3149,7 @@
         <v>43</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.15">
@@ -3253,7 +3254,7 @@
       <pane xSplit="4" ySplit="2" topLeftCell="E3" activePane="bottomRight" state="frozenSplit"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="J13" sqref="J13"/>
+      <selection pane="bottomRight" activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="55" defaultRowHeight="11" x14ac:dyDescent="0.15"/>
@@ -3289,7 +3290,7 @@
         <v>186</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="D2" s="7" t="s">
         <v>208</v>
@@ -3321,22 +3322,22 @@
         <v>195</v>
       </c>
       <c r="D3" s="9" t="s">
-        <v>194</v>
+        <v>585</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.15">
@@ -4239,7 +4240,7 @@
     <row r="48" spans="1:9" ht="12" thickBot="1" x14ac:dyDescent="0.2"/>
     <row r="49" spans="1:1" ht="59" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A49" s="22" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
     </row>
   </sheetData>
@@ -4264,7 +4265,7 @@
       <pane xSplit="4" ySplit="2" topLeftCell="E3" activePane="bottomRight" state="frozenSplit"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="E3" sqref="E3"/>
+      <selection pane="bottomRight" activeCell="E41" sqref="E41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="11" x14ac:dyDescent="0.15"/>
@@ -4321,7 +4322,7 @@
         <v>182</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.15">
@@ -4338,7 +4339,7 @@
         <v>193</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
     </row>
   </sheetData>
@@ -4355,11 +4356,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F13"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="4" ySplit="2" topLeftCell="E3" activePane="bottomRight" state="frozenSplit"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="E15" sqref="E15"/>
+      <selection pane="bottomRight" activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="38.1640625" defaultRowHeight="11" x14ac:dyDescent="0.15"/>
@@ -4421,10 +4422,10 @@
         <v>1</v>
       </c>
       <c r="E3" s="3" t="s">
+        <v>299</v>
+      </c>
+      <c r="F3" s="3" t="s">
         <v>300</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>301</v>
       </c>
     </row>
     <row r="4" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.15">
@@ -4441,10 +4442,10 @@
         <v>182</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
     </row>
     <row r="5" spans="1:6" s="2" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -4481,10 +4482,10 @@
         <v>179</v>
       </c>
       <c r="E6" s="3" t="s">
+        <v>299</v>
+      </c>
+      <c r="F6" s="3" t="s">
         <v>300</v>
-      </c>
-      <c r="F6" s="3" t="s">
-        <v>301</v>
       </c>
     </row>
     <row r="7" spans="1:6" s="2" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -4618,7 +4619,7 @@
         <v>215</v>
       </c>
       <c r="D13" s="9" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
       <c r="E13" s="8">
         <v>2514.9</v>
@@ -4642,10 +4643,10 @@
   <dimension ref="A1:S56"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="4" ySplit="2" topLeftCell="E9" activePane="bottomRight" state="frozenSplit"/>
+      <pane xSplit="4" ySplit="2" topLeftCell="E3" activePane="bottomRight" state="frozenSplit"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="E3" sqref="E3"/>
+      <selection pane="bottomRight" activeCell="E8" sqref="E8:K8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="32.83203125" defaultRowHeight="11" x14ac:dyDescent="0.15"/>
@@ -4668,7 +4669,7 @@
       </c>
       <c r="D1" s="25"/>
       <c r="E1" s="27" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="F1" s="28"/>
       <c r="G1" s="29"/>
@@ -4760,49 +4761,49 @@
         <v>1</v>
       </c>
       <c r="E3" s="3" t="s">
+        <v>299</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>299</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>299</v>
+      </c>
+      <c r="H3" s="3" t="s">
         <v>300</v>
       </c>
-      <c r="F3" s="3" t="s">
+      <c r="I3" s="3" t="s">
         <v>300</v>
       </c>
-      <c r="G3" s="3" t="s">
+      <c r="J3" s="3" t="s">
         <v>300</v>
       </c>
-      <c r="H3" s="3" t="s">
-        <v>301</v>
-      </c>
-      <c r="I3" s="3" t="s">
-        <v>301</v>
-      </c>
-      <c r="J3" s="3" t="s">
-        <v>301</v>
-      </c>
       <c r="K3" s="3" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="L3" s="3" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="M3" s="3" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="N3" s="3" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="O3" s="3" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="P3" s="3" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="Q3" s="3" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="R3" s="3" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="S3" s="3" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
     </row>
     <row r="4" spans="1:19" ht="22" x14ac:dyDescent="0.15">
@@ -4813,55 +4814,55 @@
         <v>109</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="D4" s="9" t="s">
         <v>250</v>
       </c>
       <c r="E4" s="3" t="s">
+        <v>299</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>299</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>299</v>
+      </c>
+      <c r="H4" s="3" t="s">
         <v>300</v>
       </c>
-      <c r="F4" s="3" t="s">
+      <c r="I4" s="3" t="s">
         <v>300</v>
       </c>
-      <c r="G4" s="3" t="s">
+      <c r="J4" s="3" t="s">
         <v>300</v>
       </c>
-      <c r="H4" s="3" t="s">
-        <v>301</v>
-      </c>
-      <c r="I4" s="3" t="s">
-        <v>301</v>
-      </c>
-      <c r="J4" s="3" t="s">
-        <v>301</v>
-      </c>
       <c r="K4" s="3" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="L4" s="3" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="M4" s="3" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="N4" s="3" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="O4" s="3" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="P4" s="3" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="Q4" s="3" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="R4" s="3" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="S4" s="3" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.15">
@@ -5277,16 +5278,16 @@
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A12" s="9" t="s">
+        <v>548</v>
+      </c>
+      <c r="B12" s="9" t="s">
+        <v>170</v>
+      </c>
+      <c r="C12" s="9" t="s">
+        <v>550</v>
+      </c>
+      <c r="D12" s="9" t="s">
         <v>549</v>
-      </c>
-      <c r="B12" s="9" t="s">
-        <v>170</v>
-      </c>
-      <c r="C12" s="9" t="s">
-        <v>551</v>
-      </c>
-      <c r="D12" s="9" t="s">
-        <v>550</v>
       </c>
       <c r="E12" s="1"/>
       <c r="F12" s="1"/>
@@ -5312,7 +5313,7 @@
         <v>170</v>
       </c>
       <c r="C13" s="9" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="D13" s="9" t="s">
         <v>171</v>
@@ -6510,7 +6511,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I230"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <pane xSplit="4" ySplit="2" topLeftCell="E29" activePane="bottomRight" state="frozenSplit"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
@@ -6584,13 +6585,13 @@
         <v>291</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="F3" s="3" t="s">
+        <v>299</v>
+      </c>
+      <c r="G3" s="3" t="s">
         <v>300</v>
-      </c>
-      <c r="G3" s="3" t="s">
-        <v>301</v>
       </c>
     </row>
     <row r="4" spans="1:9" s="2" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -6607,11 +6608,11 @@
         <v>223</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="F4" s="3"/>
       <c r="G4" s="3" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
     </row>
     <row r="5" spans="1:9" s="2" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -6622,7 +6623,7 @@
         <v>170</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="D5" s="9" t="s">
         <v>219</v>
@@ -6675,7 +6676,7 @@
         <v>170</v>
       </c>
       <c r="C8" s="9" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="D8" s="9" t="s">
         <v>222</v>
@@ -6696,7 +6697,7 @@
         <v>170</v>
       </c>
       <c r="C9" s="9" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="D9" s="9" t="s">
         <v>224</v>
@@ -6717,7 +6718,7 @@
         <v>170</v>
       </c>
       <c r="C10" s="9" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="D10" s="9" t="s">
         <v>225</v>
@@ -6738,7 +6739,7 @@
         <v>170</v>
       </c>
       <c r="C11" s="9" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="D11" s="9" t="s">
         <v>226</v>
@@ -6765,11 +6766,11 @@
         <v>230</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="F12" s="3"/>
       <c r="G12" s="3" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="H12" s="23"/>
       <c r="I12" s="24"/>
@@ -6785,14 +6786,14 @@
         <v>235</v>
       </c>
       <c r="D13" s="9" t="s">
+        <v>317</v>
+      </c>
+      <c r="E13" s="3" t="s">
         <v>318</v>
-      </c>
-      <c r="E13" s="3" t="s">
-        <v>319</v>
       </c>
       <c r="F13" s="3"/>
       <c r="G13" s="3" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="H13" s="23"/>
       <c r="I13" s="24"/>
@@ -6808,12 +6809,12 @@
         <v>235</v>
       </c>
       <c r="D14" s="9" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="E14" s="3"/>
       <c r="F14" s="3"/>
       <c r="G14" s="3" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="H14" s="23"/>
       <c r="I14" s="24"/>
@@ -6829,12 +6830,12 @@
         <v>235</v>
       </c>
       <c r="D15" s="9" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="E15" s="3"/>
       <c r="F15" s="3"/>
       <c r="G15" s="3" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="H15" s="23"/>
       <c r="I15" s="24"/>
@@ -6850,12 +6851,12 @@
         <v>235</v>
       </c>
       <c r="D16" s="9" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="E16" s="3"/>
       <c r="F16" s="3"/>
       <c r="G16" s="3" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="H16" s="23"/>
       <c r="I16" s="24"/>
@@ -6892,7 +6893,7 @@
         <v>236</v>
       </c>
       <c r="D18" s="9" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="E18" s="3">
         <v>1</v>
@@ -6913,7 +6914,7 @@
         <v>236</v>
       </c>
       <c r="D19" s="9" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="E19" s="3"/>
       <c r="F19" s="3"/>
@@ -6932,7 +6933,7 @@
         <v>236</v>
       </c>
       <c r="D20" s="9" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="E20" s="3"/>
       <c r="F20" s="3"/>
@@ -6951,7 +6952,7 @@
         <v>236</v>
       </c>
       <c r="D21" s="9" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="E21" s="3"/>
       <c r="F21" s="3"/>
@@ -6967,7 +6968,7 @@
         <v>170</v>
       </c>
       <c r="C22" s="9" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="D22" s="9" t="s">
         <v>228</v>
@@ -6977,7 +6978,7 @@
       </c>
       <c r="F22" s="3"/>
       <c r="G22" s="3" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.15">
@@ -6988,17 +6989,17 @@
         <v>170</v>
       </c>
       <c r="C23" s="9" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="D23" s="9" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="E23" s="3" t="b">
         <v>1</v>
       </c>
       <c r="F23" s="3"/>
       <c r="G23" s="3" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.15">
@@ -7009,15 +7010,15 @@
         <v>170</v>
       </c>
       <c r="C24" s="9" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="D24" s="9" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="E24" s="3"/>
       <c r="F24" s="3"/>
       <c r="G24" s="3" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.15">
@@ -7028,15 +7029,15 @@
         <v>170</v>
       </c>
       <c r="C25" s="9" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="D25" s="9" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="E25" s="3"/>
       <c r="F25" s="3"/>
       <c r="G25" s="3" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.15">
@@ -7047,15 +7048,15 @@
         <v>170</v>
       </c>
       <c r="C26" s="9" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="D26" s="9" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="E26" s="3"/>
       <c r="F26" s="3"/>
       <c r="G26" s="3" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.15">
@@ -7066,7 +7067,7 @@
         <v>170</v>
       </c>
       <c r="C27" s="9" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="D27" s="9" t="s">
         <v>229</v>
@@ -7087,10 +7088,10 @@
         <v>170</v>
       </c>
       <c r="C28" s="9" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="D28" s="9" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="E28" s="3" t="b">
         <v>0</v>
@@ -7108,10 +7109,10 @@
         <v>170</v>
       </c>
       <c r="C29" s="9" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="D29" s="9" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="E29" s="3"/>
       <c r="F29" s="3"/>
@@ -7127,10 +7128,10 @@
         <v>170</v>
       </c>
       <c r="C30" s="9" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="D30" s="9" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="E30" s="3"/>
       <c r="F30" s="3"/>
@@ -7146,10 +7147,10 @@
         <v>170</v>
       </c>
       <c r="C31" s="9" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="D31" s="9" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="E31" s="3"/>
       <c r="F31" s="3"/>
@@ -7165,13 +7166,13 @@
         <v>170</v>
       </c>
       <c r="C32" s="9" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="D32" s="9" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="E32" s="3" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="F32" s="3"/>
       <c r="G32" s="3"/>
@@ -7187,10 +7188,10 @@
         <v>237</v>
       </c>
       <c r="D33" s="9" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="E33" s="3" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="F33" s="3"/>
       <c r="G33" s="3"/>
@@ -7203,10 +7204,10 @@
         <v>170</v>
       </c>
       <c r="C34" s="9" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="D34" s="9" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="E34" s="3" t="b">
         <v>0</v>
@@ -7222,13 +7223,13 @@
         <v>170</v>
       </c>
       <c r="C35" s="9" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="D35" s="9" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
       <c r="E35" s="3" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="F35" s="3"/>
       <c r="G35" s="3"/>
@@ -7244,10 +7245,10 @@
         <v>237</v>
       </c>
       <c r="D36" s="9" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
       <c r="E36" s="3" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
       <c r="F36" s="3"/>
       <c r="G36" s="3"/>
@@ -7260,10 +7261,10 @@
         <v>170</v>
       </c>
       <c r="C37" s="9" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="D37" s="9" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
       <c r="E37" s="3" t="b">
         <v>0</v>
@@ -7279,13 +7280,13 @@
         <v>170</v>
       </c>
       <c r="C38" s="9" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="D38" s="9" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="E38" s="3" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="F38" s="3"/>
       <c r="G38" s="3"/>
@@ -7301,10 +7302,10 @@
         <v>237</v>
       </c>
       <c r="D39" s="9" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
       <c r="E39" s="3" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="F39" s="3"/>
       <c r="G39" s="3"/>
@@ -7317,10 +7318,10 @@
         <v>170</v>
       </c>
       <c r="C40" s="9" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="D40" s="9" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
       <c r="E40" s="3" t="b">
         <v>0</v>
@@ -7336,17 +7337,17 @@
         <v>170</v>
       </c>
       <c r="C41" s="9" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="D41" s="9" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="E41" s="3" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="F41" s="3"/>
       <c r="G41" s="3" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.15">
@@ -7360,14 +7361,14 @@
         <v>237</v>
       </c>
       <c r="D42" s="9" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="E42" s="3" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="F42" s="3"/>
       <c r="G42" s="3" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
     </row>
     <row r="43" spans="1:7" s="2" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -7378,10 +7379,10 @@
         <v>170</v>
       </c>
       <c r="C43" s="9" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="D43" s="9" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
       <c r="E43" s="3" t="b">
         <v>1</v>
@@ -7399,17 +7400,17 @@
         <v>170</v>
       </c>
       <c r="C44" s="9" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="D44" s="9" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
       <c r="E44" s="3" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="F44" s="3"/>
       <c r="G44" s="3" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.15">
@@ -7423,14 +7424,14 @@
         <v>237</v>
       </c>
       <c r="D45" s="9" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="E45" s="3" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="F45" s="3"/>
       <c r="G45" s="3" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
     </row>
     <row r="46" spans="1:7" s="2" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -7441,10 +7442,10 @@
         <v>170</v>
       </c>
       <c r="C46" s="9" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="D46" s="9" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
       <c r="E46" s="3" t="b">
         <v>1</v>
@@ -7465,10 +7466,10 @@
         <v>234</v>
       </c>
       <c r="D47" s="9" t="s">
+        <v>583</v>
+      </c>
+      <c r="E47" s="3" t="s">
         <v>584</v>
-      </c>
-      <c r="E47" s="3" t="s">
-        <v>585</v>
       </c>
       <c r="F47" s="3"/>
       <c r="G47" s="3"/>
@@ -7481,7 +7482,7 @@
         <v>170</v>
       </c>
       <c r="C48" s="9" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="D48" s="9" t="s">
         <v>241</v>
@@ -7532,7 +7533,7 @@
         <v>170</v>
       </c>
       <c r="C51" s="9" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="D51" s="9" t="s">
         <v>244</v>
@@ -7551,7 +7552,7 @@
         <v>170</v>
       </c>
       <c r="C52" s="9" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="D52" s="9" t="s">
         <v>245</v>
@@ -7570,7 +7571,7 @@
         <v>170</v>
       </c>
       <c r="C53" s="9" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="D53" s="9" t="s">
         <v>246</v>
@@ -7589,7 +7590,7 @@
         <v>170</v>
       </c>
       <c r="C54" s="9" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="D54" s="9" t="s">
         <v>247</v>
@@ -7614,7 +7615,7 @@
         <v>238</v>
       </c>
       <c r="E55" s="3" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="F55" s="3"/>
       <c r="G55" s="3"/>
@@ -7630,10 +7631,10 @@
         <v>235</v>
       </c>
       <c r="D56" s="9" t="s">
+        <v>348</v>
+      </c>
+      <c r="E56" s="3" t="s">
         <v>349</v>
-      </c>
-      <c r="E56" s="3" t="s">
-        <v>350</v>
       </c>
       <c r="F56" s="3"/>
       <c r="G56" s="3"/>
@@ -7668,7 +7669,7 @@
         <v>236</v>
       </c>
       <c r="D58" s="9" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="E58" s="3">
         <v>1</v>
@@ -7684,13 +7685,13 @@
         <v>170</v>
       </c>
       <c r="C59" s="9" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="D59" s="9" t="s">
         <v>239</v>
       </c>
       <c r="E59" s="3" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="F59" s="3"/>
       <c r="G59" s="3"/>
@@ -7703,13 +7704,13 @@
         <v>170</v>
       </c>
       <c r="C60" s="9" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="D60" s="9" t="s">
+        <v>352</v>
+      </c>
+      <c r="E60" s="3" t="s">
         <v>353</v>
-      </c>
-      <c r="E60" s="3" t="s">
-        <v>354</v>
       </c>
       <c r="F60" s="3"/>
       <c r="G60" s="3"/>
@@ -7722,7 +7723,7 @@
         <v>170</v>
       </c>
       <c r="C61" s="9" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="D61" s="9" t="s">
         <v>240</v>
@@ -7741,10 +7742,10 @@
         <v>170</v>
       </c>
       <c r="C62" s="9" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="D62" s="9" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="E62" s="3" t="b">
         <v>0</v>
@@ -7760,13 +7761,13 @@
         <v>170</v>
       </c>
       <c r="C63" s="9" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="D63" s="9" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="E63" s="3" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="F63" s="3"/>
       <c r="G63" s="3"/>
@@ -7782,10 +7783,10 @@
         <v>237</v>
       </c>
       <c r="D64" s="9" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
       <c r="E64" s="3" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="F64" s="3"/>
       <c r="G64" s="3"/>
@@ -7798,10 +7799,10 @@
         <v>170</v>
       </c>
       <c r="C65" s="9" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="D65" s="9" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
       <c r="E65" s="3" t="b">
         <v>0</v>
@@ -7817,13 +7818,13 @@
         <v>170</v>
       </c>
       <c r="C66" s="9" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="D66" s="9" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
       <c r="E66" s="3" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="F66" s="3"/>
       <c r="G66" s="3"/>
@@ -7839,10 +7840,10 @@
         <v>237</v>
       </c>
       <c r="D67" s="9" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
       <c r="E67" s="3" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
       <c r="F67" s="3"/>
       <c r="G67" s="3"/>
@@ -7855,10 +7856,10 @@
         <v>170</v>
       </c>
       <c r="C68" s="9" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="D68" s="9" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="E68" s="3" t="b">
         <v>0</v>
@@ -7874,13 +7875,13 @@
         <v>170</v>
       </c>
       <c r="C69" s="9" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="D69" s="9" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="E69" s="3" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="F69" s="3"/>
       <c r="G69" s="3"/>
@@ -7896,10 +7897,10 @@
         <v>237</v>
       </c>
       <c r="D70" s="9" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
       <c r="E70" s="3" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="F70" s="3"/>
       <c r="G70" s="3"/>
@@ -7912,10 +7913,10 @@
         <v>170</v>
       </c>
       <c r="C71" s="9" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="D71" s="9" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="E71" s="3" t="b">
         <v>0</v>
@@ -7931,13 +7932,13 @@
         <v>170</v>
       </c>
       <c r="C72" s="9" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="D72" s="9" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
       <c r="E72" s="3" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="F72" s="3"/>
       <c r="G72" s="3"/>
@@ -7953,10 +7954,10 @@
         <v>237</v>
       </c>
       <c r="D73" s="9" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
       <c r="E73" s="3" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="F73" s="3"/>
       <c r="G73" s="3"/>
@@ -7969,10 +7970,10 @@
         <v>170</v>
       </c>
       <c r="C74" s="9" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="D74" s="9" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
       <c r="E74" s="3" t="b">
         <v>1</v>
@@ -7988,13 +7989,13 @@
         <v>170</v>
       </c>
       <c r="C75" s="9" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="D75" s="9" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="E75" s="3" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="F75" s="3"/>
       <c r="G75" s="3"/>
@@ -8010,10 +8011,10 @@
         <v>237</v>
       </c>
       <c r="D76" s="9" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="E76" s="3" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="F76" s="3"/>
       <c r="G76" s="3"/>
@@ -8026,10 +8027,10 @@
         <v>170</v>
       </c>
       <c r="C77" s="9" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="D77" s="9" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
       <c r="E77" s="3" t="b">
         <v>1</v>
@@ -8048,10 +8049,10 @@
         <v>234</v>
       </c>
       <c r="D78" s="9" t="s">
+        <v>355</v>
+      </c>
+      <c r="E78" s="3" t="s">
         <v>356</v>
-      </c>
-      <c r="E78" s="3" t="s">
-        <v>357</v>
       </c>
       <c r="F78" s="3"/>
       <c r="G78" s="3"/>
@@ -8064,10 +8065,10 @@
         <v>170</v>
       </c>
       <c r="C79" s="9" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="D79" s="9" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="E79" s="3"/>
       <c r="F79" s="3"/>
@@ -8084,7 +8085,7 @@
         <v>232</v>
       </c>
       <c r="D80" s="9" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="E80" s="3"/>
       <c r="F80" s="3"/>
@@ -8101,7 +8102,7 @@
         <v>233</v>
       </c>
       <c r="D81" s="9" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="E81" s="3"/>
       <c r="F81" s="3"/>
@@ -8115,10 +8116,10 @@
         <v>170</v>
       </c>
       <c r="C82" s="9" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="D82" s="9" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="E82" s="3" t="b">
         <v>1</v>
@@ -8134,10 +8135,10 @@
         <v>170</v>
       </c>
       <c r="C83" s="9" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="D83" s="9" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="E83" s="3" t="b">
         <v>0</v>
@@ -8153,10 +8154,10 @@
         <v>170</v>
       </c>
       <c r="C84" s="9" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="D84" s="9" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="E84" s="3" t="b">
         <v>0</v>
@@ -8172,10 +8173,10 @@
         <v>170</v>
       </c>
       <c r="C85" s="9" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="D85" s="9" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="E85" s="3" t="b">
         <v>1</v>
@@ -8194,10 +8195,10 @@
         <v>235</v>
       </c>
       <c r="D86" s="9" t="s">
+        <v>364</v>
+      </c>
+      <c r="E86" s="3" t="s">
         <v>365</v>
-      </c>
-      <c r="E86" s="3" t="s">
-        <v>366</v>
       </c>
       <c r="F86" s="3"/>
       <c r="G86" s="3"/>
@@ -8213,10 +8214,10 @@
         <v>235</v>
       </c>
       <c r="D87" s="9" t="s">
+        <v>366</v>
+      </c>
+      <c r="E87" s="3" t="s">
         <v>367</v>
-      </c>
-      <c r="E87" s="3" t="s">
-        <v>368</v>
       </c>
       <c r="F87" s="3"/>
       <c r="G87" s="3"/>
@@ -8232,7 +8233,7 @@
         <v>236</v>
       </c>
       <c r="D88" s="9" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="E88" s="3">
         <v>0</v>
@@ -8251,7 +8252,7 @@
         <v>236</v>
       </c>
       <c r="D89" s="9" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="E89" s="3">
         <v>1</v>
@@ -8267,13 +8268,13 @@
         <v>170</v>
       </c>
       <c r="C90" s="9" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="D90" s="9" t="s">
+        <v>370</v>
+      </c>
+      <c r="E90" s="3" t="s">
         <v>371</v>
-      </c>
-      <c r="E90" s="3" t="s">
-        <v>372</v>
       </c>
       <c r="F90" s="3"/>
       <c r="G90" s="3"/>
@@ -8286,13 +8287,13 @@
         <v>170</v>
       </c>
       <c r="C91" s="9" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="D91" s="9" t="s">
+        <v>372</v>
+      </c>
+      <c r="E91" s="3" t="s">
         <v>373</v>
-      </c>
-      <c r="E91" s="3" t="s">
-        <v>374</v>
       </c>
       <c r="F91" s="3"/>
       <c r="G91" s="3"/>
@@ -8305,10 +8306,10 @@
         <v>170</v>
       </c>
       <c r="C92" s="9" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="D92" s="9" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="E92" s="3" t="b">
         <v>1</v>
@@ -8324,10 +8325,10 @@
         <v>170</v>
       </c>
       <c r="C93" s="9" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="D93" s="9" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="E93" s="3" t="b">
         <v>0</v>
@@ -8343,10 +8344,10 @@
         <v>170</v>
       </c>
       <c r="C94" s="9" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="D94" s="9" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="E94" s="3"/>
       <c r="F94" s="3"/>
@@ -8363,7 +8364,7 @@
         <v>237</v>
       </c>
       <c r="D95" s="9" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="E95" s="3"/>
       <c r="F95" s="3"/>
@@ -8377,10 +8378,10 @@
         <v>170</v>
       </c>
       <c r="C96" s="9" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="D96" s="9" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="E96" s="3" t="b">
         <v>0</v>
@@ -8399,10 +8400,10 @@
         <v>234</v>
       </c>
       <c r="D97" s="9" t="s">
+        <v>379</v>
+      </c>
+      <c r="E97" s="3" t="s">
         <v>380</v>
-      </c>
-      <c r="E97" s="3" t="s">
-        <v>381</v>
       </c>
       <c r="F97" s="3"/>
       <c r="G97" s="3"/>
@@ -8415,10 +8416,10 @@
         <v>170</v>
       </c>
       <c r="C98" s="9" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="D98" s="9" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="E98" s="3"/>
       <c r="F98" s="3"/>
@@ -8435,7 +8436,7 @@
         <v>232</v>
       </c>
       <c r="D99" s="9" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="E99" s="3"/>
       <c r="F99" s="3"/>
@@ -8452,7 +8453,7 @@
         <v>233</v>
       </c>
       <c r="D100" s="9" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="E100" s="3"/>
       <c r="F100" s="3"/>
@@ -8466,10 +8467,10 @@
         <v>170</v>
       </c>
       <c r="C101" s="9" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="D101" s="9" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="E101" s="3" t="b">
         <v>1</v>
@@ -8485,10 +8486,10 @@
         <v>170</v>
       </c>
       <c r="C102" s="9" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="D102" s="9" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="E102" s="3" t="b">
         <v>0</v>
@@ -8504,10 +8505,10 @@
         <v>170</v>
       </c>
       <c r="C103" s="9" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="D103" s="9" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="E103" s="3" t="b">
         <v>0</v>
@@ -8523,10 +8524,10 @@
         <v>170</v>
       </c>
       <c r="C104" s="9" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="D104" s="9" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="E104" s="3" t="b">
         <v>1</v>
@@ -8545,10 +8546,10 @@
         <v>235</v>
       </c>
       <c r="D105" s="9" t="s">
+        <v>388</v>
+      </c>
+      <c r="E105" s="3" t="s">
         <v>389</v>
-      </c>
-      <c r="E105" s="3" t="s">
-        <v>390</v>
       </c>
       <c r="F105" s="3"/>
       <c r="G105" s="3"/>
@@ -8564,10 +8565,10 @@
         <v>235</v>
       </c>
       <c r="D106" s="9" t="s">
+        <v>390</v>
+      </c>
+      <c r="E106" s="3" t="s">
         <v>391</v>
-      </c>
-      <c r="E106" s="3" t="s">
-        <v>392</v>
       </c>
       <c r="F106" s="3"/>
       <c r="G106" s="3"/>
@@ -8583,7 +8584,7 @@
         <v>236</v>
       </c>
       <c r="D107" s="9" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="E107" s="3">
         <v>0</v>
@@ -8602,7 +8603,7 @@
         <v>236</v>
       </c>
       <c r="D108" s="9" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="E108" s="3">
         <v>1</v>
@@ -8618,10 +8619,10 @@
         <v>170</v>
       </c>
       <c r="C109" s="9" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="D109" s="9" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="E109" s="3" t="b">
         <v>0</v>
@@ -8637,10 +8638,10 @@
         <v>170</v>
       </c>
       <c r="C110" s="9" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="D110" s="9" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="E110" s="3" t="b">
         <v>1</v>
@@ -8656,10 +8657,10 @@
         <v>170</v>
       </c>
       <c r="C111" s="9" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="D111" s="9" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="E111" s="3" t="b">
         <v>1</v>
@@ -8675,10 +8676,10 @@
         <v>170</v>
       </c>
       <c r="C112" s="9" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="D112" s="9" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="E112" s="3" t="b">
         <v>0</v>
@@ -8697,10 +8698,10 @@
         <v>234</v>
       </c>
       <c r="D113" s="9" t="s">
+        <v>398</v>
+      </c>
+      <c r="E113" s="3" t="s">
         <v>399</v>
-      </c>
-      <c r="E113" s="3" t="s">
-        <v>400</v>
       </c>
       <c r="F113" s="3"/>
       <c r="G113" s="3"/>
@@ -8713,10 +8714,10 @@
         <v>170</v>
       </c>
       <c r="C114" s="9" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="D114" s="9" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="E114" s="3"/>
       <c r="F114" s="3"/>
@@ -8733,7 +8734,7 @@
         <v>232</v>
       </c>
       <c r="D115" s="9" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="E115" s="3"/>
       <c r="F115" s="3"/>
@@ -8750,7 +8751,7 @@
         <v>233</v>
       </c>
       <c r="D116" s="9" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="E116" s="3"/>
       <c r="F116" s="3"/>
@@ -8764,10 +8765,10 @@
         <v>170</v>
       </c>
       <c r="C117" s="9" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="D117" s="9" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="E117" s="3" t="b">
         <v>1</v>
@@ -8783,10 +8784,10 @@
         <v>170</v>
       </c>
       <c r="C118" s="9" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="D118" s="9" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="E118" s="3" t="b">
         <v>0</v>
@@ -8802,10 +8803,10 @@
         <v>170</v>
       </c>
       <c r="C119" s="9" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="D119" s="9" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="E119" s="3" t="b">
         <v>0</v>
@@ -8821,10 +8822,10 @@
         <v>170</v>
       </c>
       <c r="C120" s="9" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="D120" s="9" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="E120" s="3" t="b">
         <v>1</v>
@@ -8843,10 +8844,10 @@
         <v>235</v>
       </c>
       <c r="D121" s="9" t="s">
+        <v>407</v>
+      </c>
+      <c r="E121" s="3" t="s">
         <v>408</v>
-      </c>
-      <c r="E121" s="3" t="s">
-        <v>409</v>
       </c>
       <c r="F121" s="3"/>
       <c r="G121" s="3"/>
@@ -8862,10 +8863,10 @@
         <v>235</v>
       </c>
       <c r="D122" s="9" t="s">
+        <v>409</v>
+      </c>
+      <c r="E122" s="3" t="s">
         <v>410</v>
-      </c>
-      <c r="E122" s="3" t="s">
-        <v>411</v>
       </c>
       <c r="F122" s="3"/>
       <c r="G122" s="3"/>
@@ -8881,7 +8882,7 @@
         <v>236</v>
       </c>
       <c r="D123" s="9" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="E123" s="3">
         <v>0</v>
@@ -8900,7 +8901,7 @@
         <v>236</v>
       </c>
       <c r="D124" s="9" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="E124" s="3">
         <v>1</v>
@@ -8916,13 +8917,13 @@
         <v>170</v>
       </c>
       <c r="C125" s="9" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="D125" s="9" t="s">
+        <v>413</v>
+      </c>
+      <c r="E125" s="3" t="s">
         <v>414</v>
-      </c>
-      <c r="E125" s="3" t="s">
-        <v>415</v>
       </c>
       <c r="F125" s="3"/>
       <c r="G125" s="3"/>
@@ -8935,13 +8936,13 @@
         <v>170</v>
       </c>
       <c r="C126" s="9" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="D126" s="9" t="s">
+        <v>415</v>
+      </c>
+      <c r="E126" s="3" t="s">
         <v>416</v>
-      </c>
-      <c r="E126" s="3" t="s">
-        <v>417</v>
       </c>
       <c r="F126" s="3"/>
       <c r="G126" s="3"/>
@@ -8954,10 +8955,10 @@
         <v>170</v>
       </c>
       <c r="C127" s="9" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="D127" s="9" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="E127" s="3" t="b">
         <v>1</v>
@@ -8973,10 +8974,10 @@
         <v>170</v>
       </c>
       <c r="C128" s="9" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="D128" s="9" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="E128" s="3" t="b">
         <v>0</v>
@@ -8995,10 +8996,10 @@
         <v>234</v>
       </c>
       <c r="D129" s="9" t="s">
+        <v>419</v>
+      </c>
+      <c r="E129" s="3" t="s">
         <v>420</v>
-      </c>
-      <c r="E129" s="3" t="s">
-        <v>421</v>
       </c>
       <c r="F129" s="3"/>
       <c r="G129" s="3"/>
@@ -9011,10 +9012,10 @@
         <v>170</v>
       </c>
       <c r="C130" s="9" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="D130" s="9" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="E130" s="3"/>
       <c r="F130" s="3"/>
@@ -9031,7 +9032,7 @@
         <v>232</v>
       </c>
       <c r="D131" s="9" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="E131" s="3"/>
       <c r="F131" s="3"/>
@@ -9048,7 +9049,7 @@
         <v>233</v>
       </c>
       <c r="D132" s="9" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="E132" s="3"/>
       <c r="F132" s="3"/>
@@ -9062,10 +9063,10 @@
         <v>170</v>
       </c>
       <c r="C133" s="9" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="D133" s="9" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="E133" s="3" t="b">
         <v>1</v>
@@ -9081,10 +9082,10 @@
         <v>170</v>
       </c>
       <c r="C134" s="9" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="D134" s="9" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="E134" s="3" t="b">
         <v>0</v>
@@ -9100,10 +9101,10 @@
         <v>170</v>
       </c>
       <c r="C135" s="9" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="D135" s="9" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="E135" s="3" t="b">
         <v>0</v>
@@ -9119,10 +9120,10 @@
         <v>170</v>
       </c>
       <c r="C136" s="9" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="D136" s="9" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="E136" s="3" t="b">
         <v>1</v>
@@ -9141,10 +9142,10 @@
         <v>235</v>
       </c>
       <c r="D137" s="9" t="s">
+        <v>428</v>
+      </c>
+      <c r="E137" s="3" t="s">
         <v>429</v>
-      </c>
-      <c r="E137" s="3" t="s">
-        <v>430</v>
       </c>
       <c r="F137" s="3"/>
       <c r="G137" s="3"/>
@@ -9160,10 +9161,10 @@
         <v>235</v>
       </c>
       <c r="D138" s="9" t="s">
+        <v>430</v>
+      </c>
+      <c r="E138" s="3" t="s">
         <v>431</v>
-      </c>
-      <c r="E138" s="3" t="s">
-        <v>432</v>
       </c>
       <c r="F138" s="3"/>
       <c r="G138" s="3"/>
@@ -9179,7 +9180,7 @@
         <v>236</v>
       </c>
       <c r="D139" s="9" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="E139" s="3">
         <v>0</v>
@@ -9198,7 +9199,7 @@
         <v>236</v>
       </c>
       <c r="D140" s="9" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="E140" s="3">
         <v>1</v>
@@ -9214,13 +9215,13 @@
         <v>170</v>
       </c>
       <c r="C141" s="9" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="D141" s="9" t="s">
+        <v>434</v>
+      </c>
+      <c r="E141" s="3" t="s">
         <v>435</v>
-      </c>
-      <c r="E141" s="3" t="s">
-        <v>436</v>
       </c>
       <c r="F141" s="3"/>
       <c r="G141" s="3"/>
@@ -9233,13 +9234,13 @@
         <v>170</v>
       </c>
       <c r="C142" s="9" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="D142" s="9" t="s">
+        <v>436</v>
+      </c>
+      <c r="E142" s="3" t="s">
         <v>437</v>
-      </c>
-      <c r="E142" s="3" t="s">
-        <v>438</v>
       </c>
       <c r="F142" s="3"/>
       <c r="G142" s="3"/>
@@ -9252,10 +9253,10 @@
         <v>170</v>
       </c>
       <c r="C143" s="9" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="D143" s="9" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="E143" s="3" t="b">
         <v>1</v>
@@ -9271,10 +9272,10 @@
         <v>170</v>
       </c>
       <c r="C144" s="9" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="D144" s="9" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="E144" s="3" t="b">
         <v>0</v>
@@ -9293,10 +9294,10 @@
         <v>234</v>
       </c>
       <c r="D145" s="9" t="s">
+        <v>440</v>
+      </c>
+      <c r="E145" s="3" t="s">
         <v>441</v>
-      </c>
-      <c r="E145" s="3" t="s">
-        <v>442</v>
       </c>
       <c r="F145" s="3"/>
       <c r="G145" s="3"/>
@@ -9309,10 +9310,10 @@
         <v>170</v>
       </c>
       <c r="C146" s="9" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="D146" s="9" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="E146" s="3"/>
       <c r="F146" s="3"/>
@@ -9329,7 +9330,7 @@
         <v>232</v>
       </c>
       <c r="D147" s="9" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="E147" s="3"/>
       <c r="F147" s="3"/>
@@ -9346,7 +9347,7 @@
         <v>233</v>
       </c>
       <c r="D148" s="9" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="E148" s="3"/>
       <c r="F148" s="3"/>
@@ -9360,10 +9361,10 @@
         <v>170</v>
       </c>
       <c r="C149" s="9" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="D149" s="9" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="E149" s="3" t="b">
         <v>1</v>
@@ -9379,10 +9380,10 @@
         <v>170</v>
       </c>
       <c r="C150" s="9" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="D150" s="9" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="E150" s="3" t="b">
         <v>0</v>
@@ -9398,10 +9399,10 @@
         <v>170</v>
       </c>
       <c r="C151" s="9" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="D151" s="9" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="E151" s="3" t="b">
         <v>0</v>
@@ -9417,10 +9418,10 @@
         <v>170</v>
       </c>
       <c r="C152" s="9" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="D152" s="9" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="E152" s="3" t="b">
         <v>1</v>
@@ -9439,10 +9440,10 @@
         <v>235</v>
       </c>
       <c r="D153" s="9" t="s">
+        <v>449</v>
+      </c>
+      <c r="E153" s="3" t="s">
         <v>450</v>
-      </c>
-      <c r="E153" s="3" t="s">
-        <v>451</v>
       </c>
       <c r="F153" s="3"/>
       <c r="G153" s="3"/>
@@ -9458,10 +9459,10 @@
         <v>235</v>
       </c>
       <c r="D154" s="9" t="s">
+        <v>451</v>
+      </c>
+      <c r="E154" s="3" t="s">
         <v>452</v>
-      </c>
-      <c r="E154" s="3" t="s">
-        <v>453</v>
       </c>
       <c r="F154" s="3"/>
       <c r="G154" s="3"/>
@@ -9477,7 +9478,7 @@
         <v>236</v>
       </c>
       <c r="D155" s="9" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="E155" s="3">
         <v>0</v>
@@ -9496,7 +9497,7 @@
         <v>236</v>
       </c>
       <c r="D156" s="9" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="E156" s="3">
         <v>1</v>
@@ -9512,13 +9513,13 @@
         <v>170</v>
       </c>
       <c r="C157" s="9" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="D157" s="9" t="s">
+        <v>455</v>
+      </c>
+      <c r="E157" s="3" t="s">
         <v>456</v>
-      </c>
-      <c r="E157" s="3" t="s">
-        <v>457</v>
       </c>
       <c r="F157" s="3"/>
       <c r="G157" s="3"/>
@@ -9531,13 +9532,13 @@
         <v>170</v>
       </c>
       <c r="C158" s="9" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="D158" s="9" t="s">
+        <v>457</v>
+      </c>
+      <c r="E158" s="3" t="s">
         <v>458</v>
-      </c>
-      <c r="E158" s="3" t="s">
-        <v>459</v>
       </c>
       <c r="F158" s="3"/>
       <c r="G158" s="3"/>
@@ -9550,10 +9551,10 @@
         <v>170</v>
       </c>
       <c r="C159" s="9" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="D159" s="9" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="E159" s="3" t="b">
         <v>1</v>
@@ -9569,10 +9570,10 @@
         <v>170</v>
       </c>
       <c r="C160" s="9" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="D160" s="9" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="E160" s="3" t="b">
         <v>0</v>
@@ -9591,10 +9592,10 @@
         <v>234</v>
       </c>
       <c r="D161" s="9" t="s">
+        <v>461</v>
+      </c>
+      <c r="E161" s="3" t="s">
         <v>462</v>
-      </c>
-      <c r="E161" s="3" t="s">
-        <v>463</v>
       </c>
       <c r="F161" s="3"/>
       <c r="G161" s="3"/>
@@ -9607,10 +9608,10 @@
         <v>170</v>
       </c>
       <c r="C162" s="9" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="D162" s="9" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="E162" s="3"/>
       <c r="F162" s="3"/>
@@ -9627,7 +9628,7 @@
         <v>232</v>
       </c>
       <c r="D163" s="9" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="E163" s="3"/>
       <c r="F163" s="3"/>
@@ -9644,7 +9645,7 @@
         <v>233</v>
       </c>
       <c r="D164" s="9" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="E164" s="3"/>
       <c r="F164" s="3"/>
@@ -9658,10 +9659,10 @@
         <v>170</v>
       </c>
       <c r="C165" s="9" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="D165" s="9" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="E165" s="3" t="b">
         <v>1</v>
@@ -9677,10 +9678,10 @@
         <v>170</v>
       </c>
       <c r="C166" s="9" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="D166" s="9" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="E166" s="3" t="b">
         <v>0</v>
@@ -9696,10 +9697,10 @@
         <v>170</v>
       </c>
       <c r="C167" s="9" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="D167" s="9" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="E167" s="3" t="b">
         <v>0</v>
@@ -9715,10 +9716,10 @@
         <v>170</v>
       </c>
       <c r="C168" s="9" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="D168" s="9" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="E168" s="3" t="b">
         <v>1</v>
@@ -9737,10 +9738,10 @@
         <v>235</v>
       </c>
       <c r="D169" s="9" t="s">
+        <v>470</v>
+      </c>
+      <c r="E169" s="3" t="s">
         <v>471</v>
-      </c>
-      <c r="E169" s="3" t="s">
-        <v>472</v>
       </c>
       <c r="F169" s="3"/>
       <c r="G169" s="3"/>
@@ -9756,10 +9757,10 @@
         <v>235</v>
       </c>
       <c r="D170" s="9" t="s">
+        <v>472</v>
+      </c>
+      <c r="E170" s="3" t="s">
         <v>473</v>
-      </c>
-      <c r="E170" s="3" t="s">
-        <v>474</v>
       </c>
       <c r="F170" s="3"/>
       <c r="G170" s="3"/>
@@ -9775,7 +9776,7 @@
         <v>236</v>
       </c>
       <c r="D171" s="9" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="E171" s="3">
         <v>0</v>
@@ -9794,7 +9795,7 @@
         <v>236</v>
       </c>
       <c r="D172" s="9" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="E172" s="3">
         <v>1</v>
@@ -9810,13 +9811,13 @@
         <v>170</v>
       </c>
       <c r="C173" s="9" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="D173" s="9" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="E173" s="3" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="F173" s="3"/>
       <c r="G173" s="3"/>
@@ -9829,13 +9830,13 @@
         <v>170</v>
       </c>
       <c r="C174" s="9" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="D174" s="9" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="E174" s="3" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="F174" s="3"/>
       <c r="G174" s="3"/>
@@ -9848,10 +9849,10 @@
         <v>170</v>
       </c>
       <c r="C175" s="9" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="D175" s="9" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="E175" s="3" t="b">
         <v>1</v>
@@ -9867,10 +9868,10 @@
         <v>170</v>
       </c>
       <c r="C176" s="9" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="D176" s="9" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="E176" s="3" t="b">
         <v>0</v>
@@ -9889,10 +9890,10 @@
         <v>234</v>
       </c>
       <c r="D177" s="9" t="s">
+        <v>480</v>
+      </c>
+      <c r="E177" s="3" t="s">
         <v>481</v>
-      </c>
-      <c r="E177" s="3" t="s">
-        <v>482</v>
       </c>
       <c r="F177" s="3"/>
       <c r="G177" s="3"/>
@@ -9905,10 +9906,10 @@
         <v>170</v>
       </c>
       <c r="C178" s="9" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="D178" s="9" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="E178" s="3"/>
       <c r="F178" s="3"/>
@@ -9925,7 +9926,7 @@
         <v>232</v>
       </c>
       <c r="D179" s="9" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="E179" s="3"/>
       <c r="F179" s="3"/>
@@ -9942,7 +9943,7 @@
         <v>233</v>
       </c>
       <c r="D180" s="9" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="E180" s="3"/>
       <c r="F180" s="3"/>
@@ -9956,10 +9957,10 @@
         <v>170</v>
       </c>
       <c r="C181" s="9" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="D181" s="9" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="E181" s="3" t="b">
         <v>1</v>
@@ -9975,10 +9976,10 @@
         <v>170</v>
       </c>
       <c r="C182" s="9" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="D182" s="9" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="E182" s="3" t="b">
         <v>0</v>
@@ -9994,10 +9995,10 @@
         <v>170</v>
       </c>
       <c r="C183" s="9" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="D183" s="9" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="E183" s="3" t="b">
         <v>0</v>
@@ -10013,10 +10014,10 @@
         <v>170</v>
       </c>
       <c r="C184" s="9" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="D184" s="9" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="E184" s="3" t="b">
         <v>1</v>
@@ -10035,10 +10036,10 @@
         <v>235</v>
       </c>
       <c r="D185" s="9" t="s">
+        <v>489</v>
+      </c>
+      <c r="E185" s="3" t="s">
         <v>490</v>
-      </c>
-      <c r="E185" s="3" t="s">
-        <v>491</v>
       </c>
       <c r="F185" s="3"/>
       <c r="G185" s="3"/>
@@ -10054,10 +10055,10 @@
         <v>235</v>
       </c>
       <c r="D186" s="9" t="s">
+        <v>491</v>
+      </c>
+      <c r="E186" s="3" t="s">
         <v>492</v>
-      </c>
-      <c r="E186" s="3" t="s">
-        <v>493</v>
       </c>
       <c r="F186" s="3"/>
       <c r="G186" s="3"/>
@@ -10073,10 +10074,10 @@
         <v>235</v>
       </c>
       <c r="D187" s="9" t="s">
+        <v>493</v>
+      </c>
+      <c r="E187" s="3" t="s">
         <v>494</v>
-      </c>
-      <c r="E187" s="3" t="s">
-        <v>495</v>
       </c>
       <c r="F187" s="3"/>
       <c r="G187" s="3"/>
@@ -10092,10 +10093,10 @@
         <v>235</v>
       </c>
       <c r="D188" s="9" t="s">
+        <v>495</v>
+      </c>
+      <c r="E188" s="3" t="s">
         <v>496</v>
-      </c>
-      <c r="E188" s="3" t="s">
-        <v>497</v>
       </c>
       <c r="F188" s="3"/>
       <c r="G188" s="3"/>
@@ -10111,7 +10112,7 @@
         <v>236</v>
       </c>
       <c r="D189" s="9" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="E189" s="3">
         <v>0</v>
@@ -10130,7 +10131,7 @@
         <v>236</v>
       </c>
       <c r="D190" s="9" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="E190" s="3">
         <v>1</v>
@@ -10149,7 +10150,7 @@
         <v>236</v>
       </c>
       <c r="D191" s="9" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="E191" s="3">
         <v>2</v>
@@ -10168,7 +10169,7 @@
         <v>236</v>
       </c>
       <c r="D192" s="9" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="E192" s="3">
         <v>3</v>
@@ -10184,13 +10185,13 @@
         <v>170</v>
       </c>
       <c r="C193" s="9" t="s">
+        <v>330</v>
+      </c>
+      <c r="D193" s="9" t="s">
+        <v>501</v>
+      </c>
+      <c r="E193" s="3" t="s">
         <v>331</v>
-      </c>
-      <c r="D193" s="9" t="s">
-        <v>502</v>
-      </c>
-      <c r="E193" s="3" t="s">
-        <v>332</v>
       </c>
       <c r="F193" s="3"/>
       <c r="G193" s="3"/>
@@ -10203,13 +10204,13 @@
         <v>170</v>
       </c>
       <c r="C194" s="9" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="D194" s="9" t="s">
+        <v>502</v>
+      </c>
+      <c r="E194" s="3" t="s">
         <v>503</v>
-      </c>
-      <c r="E194" s="3" t="s">
-        <v>504</v>
       </c>
       <c r="F194" s="3"/>
       <c r="G194" s="3"/>
@@ -10222,13 +10223,13 @@
         <v>170</v>
       </c>
       <c r="C195" s="9" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="D195" s="9" t="s">
+        <v>504</v>
+      </c>
+      <c r="E195" s="3" t="s">
         <v>505</v>
-      </c>
-      <c r="E195" s="3" t="s">
-        <v>506</v>
       </c>
       <c r="F195" s="3"/>
       <c r="G195" s="3"/>
@@ -10241,13 +10242,13 @@
         <v>170</v>
       </c>
       <c r="C196" s="9" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="D196" s="9" t="s">
+        <v>506</v>
+      </c>
+      <c r="E196" s="3" t="s">
         <v>507</v>
-      </c>
-      <c r="E196" s="3" t="s">
-        <v>508</v>
       </c>
       <c r="F196" s="3"/>
       <c r="G196" s="3"/>
@@ -10260,10 +10261,10 @@
         <v>170</v>
       </c>
       <c r="C197" s="9" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="D197" s="9" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="E197" s="3" t="b">
         <v>1</v>
@@ -10279,10 +10280,10 @@
         <v>170</v>
       </c>
       <c r="C198" s="9" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="D198" s="9" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="E198" s="3" t="b">
         <v>0</v>
@@ -10301,10 +10302,10 @@
         <v>234</v>
       </c>
       <c r="D199" s="9" t="s">
+        <v>510</v>
+      </c>
+      <c r="E199" s="3" t="s">
         <v>511</v>
-      </c>
-      <c r="E199" s="3" t="s">
-        <v>512</v>
       </c>
       <c r="F199" s="3"/>
       <c r="G199" s="3"/>
@@ -10317,10 +10318,10 @@
         <v>170</v>
       </c>
       <c r="C200" s="9" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="D200" s="9" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="E200" s="3"/>
       <c r="F200" s="3"/>
@@ -10337,7 +10338,7 @@
         <v>232</v>
       </c>
       <c r="D201" s="9" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="E201" s="3"/>
       <c r="F201" s="3"/>
@@ -10354,7 +10355,7 @@
         <v>233</v>
       </c>
       <c r="D202" s="9" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="E202" s="3"/>
       <c r="F202" s="3"/>
@@ -10368,10 +10369,10 @@
         <v>170</v>
       </c>
       <c r="C203" s="9" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="D203" s="9" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="E203" s="3" t="b">
         <v>1</v>
@@ -10387,10 +10388,10 @@
         <v>170</v>
       </c>
       <c r="C204" s="9" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="D204" s="9" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="E204" s="3" t="b">
         <v>0</v>
@@ -10406,10 +10407,10 @@
         <v>170</v>
       </c>
       <c r="C205" s="9" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="D205" s="9" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="E205" s="3" t="b">
         <v>0</v>
@@ -10425,10 +10426,10 @@
         <v>170</v>
       </c>
       <c r="C206" s="9" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="D206" s="9" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="E206" s="3" t="b">
         <v>1</v>
@@ -10447,10 +10448,10 @@
         <v>235</v>
       </c>
       <c r="D207" s="9" t="s">
+        <v>519</v>
+      </c>
+      <c r="E207" s="3" t="s">
         <v>520</v>
-      </c>
-      <c r="E207" s="3" t="s">
-        <v>521</v>
       </c>
       <c r="F207" s="3"/>
       <c r="G207" s="3"/>
@@ -10466,10 +10467,10 @@
         <v>235</v>
       </c>
       <c r="D208" s="9" t="s">
+        <v>521</v>
+      </c>
+      <c r="E208" s="3" t="s">
         <v>522</v>
-      </c>
-      <c r="E208" s="3" t="s">
-        <v>523</v>
       </c>
       <c r="F208" s="3"/>
       <c r="G208" s="3"/>
@@ -10485,7 +10486,7 @@
         <v>236</v>
       </c>
       <c r="D209" s="9" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="E209" s="3">
         <v>0</v>
@@ -10504,7 +10505,7 @@
         <v>236</v>
       </c>
       <c r="D210" s="9" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="E210" s="3">
         <v>1</v>
@@ -10520,10 +10521,10 @@
         <v>170</v>
       </c>
       <c r="C211" s="9" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="D211" s="9" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="E211" s="3" t="b">
         <v>0</v>
@@ -10539,10 +10540,10 @@
         <v>170</v>
       </c>
       <c r="C212" s="9" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="D212" s="9" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="E212" s="3" t="b">
         <v>1</v>
@@ -10558,10 +10559,10 @@
         <v>170</v>
       </c>
       <c r="C213" s="9" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="D213" s="9" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="E213" s="3" t="b">
         <v>1</v>
@@ -10577,10 +10578,10 @@
         <v>170</v>
       </c>
       <c r="C214" s="9" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="D214" s="9" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="E214" s="3" t="b">
         <v>0</v>
@@ -10599,10 +10600,10 @@
         <v>234</v>
       </c>
       <c r="D215" s="9" t="s">
+        <v>529</v>
+      </c>
+      <c r="E215" s="3" t="s">
         <v>530</v>
-      </c>
-      <c r="E215" s="3" t="s">
-        <v>531</v>
       </c>
       <c r="F215" s="3"/>
       <c r="G215" s="3"/>
@@ -10615,10 +10616,10 @@
         <v>170</v>
       </c>
       <c r="C216" s="9" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="D216" s="9" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="E216" s="3"/>
       <c r="F216" s="3"/>
@@ -10635,7 +10636,7 @@
         <v>232</v>
       </c>
       <c r="D217" s="9" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
       <c r="E217" s="3"/>
       <c r="F217" s="3"/>
@@ -10652,7 +10653,7 @@
         <v>233</v>
       </c>
       <c r="D218" s="9" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
       <c r="E218" s="3"/>
       <c r="F218" s="3"/>
@@ -10666,10 +10667,10 @@
         <v>170</v>
       </c>
       <c r="C219" s="9" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="D219" s="9" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="E219" s="3" t="b">
         <v>1</v>
@@ -10685,10 +10686,10 @@
         <v>170</v>
       </c>
       <c r="C220" s="9" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="D220" s="9" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="E220" s="3" t="b">
         <v>0</v>
@@ -10704,10 +10705,10 @@
         <v>170</v>
       </c>
       <c r="C221" s="9" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="D221" s="9" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="E221" s="3" t="b">
         <v>0</v>
@@ -10723,10 +10724,10 @@
         <v>170</v>
       </c>
       <c r="C222" s="9" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="D222" s="9" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="E222" s="3" t="b">
         <v>1</v>
@@ -10745,10 +10746,10 @@
         <v>235</v>
       </c>
       <c r="D223" s="9" t="s">
+        <v>538</v>
+      </c>
+      <c r="E223" s="3" t="s">
         <v>539</v>
-      </c>
-      <c r="E223" s="3" t="s">
-        <v>540</v>
       </c>
       <c r="F223" s="3"/>
       <c r="G223" s="3"/>
@@ -10764,10 +10765,10 @@
         <v>235</v>
       </c>
       <c r="D224" s="9" t="s">
+        <v>540</v>
+      </c>
+      <c r="E224" s="3" t="s">
         <v>541</v>
-      </c>
-      <c r="E224" s="3" t="s">
-        <v>542</v>
       </c>
       <c r="F224" s="3"/>
       <c r="G224" s="3"/>
@@ -10783,7 +10784,7 @@
         <v>236</v>
       </c>
       <c r="D225" s="9" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
       <c r="E225" s="3">
         <v>0</v>
@@ -10802,7 +10803,7 @@
         <v>236</v>
       </c>
       <c r="D226" s="9" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="E226" s="3">
         <v>1</v>
@@ -10818,10 +10819,10 @@
         <v>170</v>
       </c>
       <c r="C227" s="9" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="D227" s="9" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="E227" s="3" t="b">
         <v>0</v>
@@ -10837,10 +10838,10 @@
         <v>170</v>
       </c>
       <c r="C228" s="9" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="D228" s="9" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="E228" s="3" t="b">
         <v>1</v>
@@ -10856,10 +10857,10 @@
         <v>170</v>
       </c>
       <c r="C229" s="9" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="D229" s="9" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="E229" s="3" t="b">
         <v>1</v>
@@ -10875,10 +10876,10 @@
         <v>170</v>
       </c>
       <c r="C230" s="9" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="D230" s="9" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="E230" s="3" t="b">
         <v>0</v>

</xml_diff>

<commit_message>
New version of xlsx
</commit_message>
<xml_diff>
--- a/src/test/resources/SBAC-IAB-FIXED-G11M-Winter-2017-2018.xlsx
+++ b/src/test/resources/SBAC-IAB-FIXED-G11M-Winter-2017-2018.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="23320" yWindow="6280" windowWidth="28800" windowHeight="17560" tabRatio="644" activeTab="3"/>
+    <workbookView xWindow="34240" yWindow="6100" windowWidth="28800" windowHeight="17560" tabRatio="644" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Package" sheetId="16" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1621" uniqueCount="586">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1621" uniqueCount="587">
   <si>
     <t>ItemId</t>
   </si>
@@ -913,6 +913,9 @@
   </si>
   <si>
     <t>A string used to link forms of different segments</t>
+  </si>
+  <si>
+    <t>SBAC-IAB-FIXED-G11M</t>
   </si>
   <si>
     <t>IAB</t>
@@ -3013,7 +3016,7 @@
         <v>194</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -3149,7 +3152,7 @@
         <v>43</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.15">
@@ -3254,7 +3257,7 @@
       <pane xSplit="4" ySplit="2" topLeftCell="E3" activePane="bottomRight" state="frozenSplit"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="H16" sqref="H16"/>
+      <selection pane="bottomRight" activeCell="F26" sqref="F26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="55" defaultRowHeight="11" x14ac:dyDescent="0.15"/>
@@ -3290,7 +3293,7 @@
         <v>186</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="D2" s="7" t="s">
         <v>208</v>
@@ -3322,22 +3325,22 @@
         <v>195</v>
       </c>
       <c r="D3" s="9" t="s">
-        <v>585</v>
+        <v>586</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.15">
@@ -4240,7 +4243,7 @@
     <row r="48" spans="1:9" ht="12" thickBot="1" x14ac:dyDescent="0.2"/>
     <row r="49" spans="1:1" ht="59" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A49" s="22" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
     </row>
   </sheetData>
@@ -4265,7 +4268,7 @@
       <pane xSplit="4" ySplit="2" topLeftCell="E3" activePane="bottomRight" state="frozenSplit"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="E41" sqref="E41"/>
+      <selection pane="bottomRight" activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="11" x14ac:dyDescent="0.15"/>
@@ -4322,7 +4325,7 @@
         <v>182</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.15">
@@ -4339,7 +4342,7 @@
         <v>193</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
     </row>
   </sheetData>
@@ -4360,7 +4363,7 @@
       <pane xSplit="4" ySplit="2" topLeftCell="E3" activePane="bottomRight" state="frozenSplit"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="D24" sqref="D24"/>
+      <selection pane="bottomRight" activeCell="E4" sqref="E4:F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="38.1640625" defaultRowHeight="11" x14ac:dyDescent="0.15"/>
@@ -4422,10 +4425,10 @@
         <v>1</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
     </row>
     <row r="4" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.15">
@@ -4442,10 +4445,10 @@
         <v>182</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
     </row>
     <row r="5" spans="1:6" s="2" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -4482,10 +4485,10 @@
         <v>179</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
     </row>
     <row r="7" spans="1:6" s="2" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -4619,7 +4622,7 @@
         <v>215</v>
       </c>
       <c r="D13" s="9" t="s">
-        <v>551</v>
+        <v>552</v>
       </c>
       <c r="E13" s="8">
         <v>2514.9</v>
@@ -4669,7 +4672,7 @@
       </c>
       <c r="D1" s="25"/>
       <c r="E1" s="27" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="F1" s="28"/>
       <c r="G1" s="29"/>
@@ -4761,49 +4764,49 @@
         <v>1</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="H3" s="3" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="I3" s="3" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="J3" s="3" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="K3" s="3" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="L3" s="3" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="M3" s="3" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="N3" s="3" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="O3" s="3" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="P3" s="3" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="Q3" s="3" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="R3" s="3" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="S3" s="3" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
     </row>
     <row r="4" spans="1:19" ht="22" x14ac:dyDescent="0.15">
@@ -4814,55 +4817,55 @@
         <v>109</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="D4" s="9" t="s">
         <v>250</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="H4" s="3" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="I4" s="3" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="J4" s="3" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="K4" s="3" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="L4" s="3" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="M4" s="3" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="N4" s="3" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="O4" s="3" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="P4" s="3" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="Q4" s="3" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="R4" s="3" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="S4" s="3" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.15">
@@ -5278,16 +5281,16 @@
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A12" s="9" t="s">
-        <v>548</v>
+        <v>549</v>
       </c>
       <c r="B12" s="9" t="s">
         <v>170</v>
       </c>
       <c r="C12" s="9" t="s">
+        <v>551</v>
+      </c>
+      <c r="D12" s="9" t="s">
         <v>550</v>
-      </c>
-      <c r="D12" s="9" t="s">
-        <v>549</v>
       </c>
       <c r="E12" s="1"/>
       <c r="F12" s="1"/>
@@ -5313,7 +5316,7 @@
         <v>170</v>
       </c>
       <c r="C13" s="9" t="s">
-        <v>550</v>
+        <v>551</v>
       </c>
       <c r="D13" s="9" t="s">
         <v>171</v>
@@ -6585,13 +6588,13 @@
         <v>291</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
     </row>
     <row r="4" spans="1:9" s="2" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -6608,11 +6611,11 @@
         <v>223</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="F4" s="3"/>
       <c r="G4" s="3" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
     </row>
     <row r="5" spans="1:9" s="2" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -6623,7 +6626,7 @@
         <v>170</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="D5" s="9" t="s">
         <v>219</v>
@@ -6676,7 +6679,7 @@
         <v>170</v>
       </c>
       <c r="C8" s="9" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="D8" s="9" t="s">
         <v>222</v>
@@ -6697,7 +6700,7 @@
         <v>170</v>
       </c>
       <c r="C9" s="9" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="D9" s="9" t="s">
         <v>224</v>
@@ -6718,7 +6721,7 @@
         <v>170</v>
       </c>
       <c r="C10" s="9" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="D10" s="9" t="s">
         <v>225</v>
@@ -6739,7 +6742,7 @@
         <v>170</v>
       </c>
       <c r="C11" s="9" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="D11" s="9" t="s">
         <v>226</v>
@@ -6766,11 +6769,11 @@
         <v>230</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="F12" s="3"/>
       <c r="G12" s="3" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="H12" s="23"/>
       <c r="I12" s="24"/>
@@ -6786,14 +6789,14 @@
         <v>235</v>
       </c>
       <c r="D13" s="9" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
       <c r="F13" s="3"/>
       <c r="G13" s="3" t="s">
-        <v>319</v>
+        <v>320</v>
       </c>
       <c r="H13" s="23"/>
       <c r="I13" s="24"/>
@@ -6809,12 +6812,12 @@
         <v>235</v>
       </c>
       <c r="D14" s="9" t="s">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="E14" s="3"/>
       <c r="F14" s="3"/>
       <c r="G14" s="3" t="s">
-        <v>321</v>
+        <v>322</v>
       </c>
       <c r="H14" s="23"/>
       <c r="I14" s="24"/>
@@ -6830,12 +6833,12 @@
         <v>235</v>
       </c>
       <c r="D15" s="9" t="s">
-        <v>322</v>
+        <v>323</v>
       </c>
       <c r="E15" s="3"/>
       <c r="F15" s="3"/>
       <c r="G15" s="3" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="H15" s="23"/>
       <c r="I15" s="24"/>
@@ -6851,12 +6854,12 @@
         <v>235</v>
       </c>
       <c r="D16" s="9" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="E16" s="3"/>
       <c r="F16" s="3"/>
       <c r="G16" s="3" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
       <c r="H16" s="23"/>
       <c r="I16" s="24"/>
@@ -6893,7 +6896,7 @@
         <v>236</v>
       </c>
       <c r="D18" s="9" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
       <c r="E18" s="3">
         <v>1</v>
@@ -6914,7 +6917,7 @@
         <v>236</v>
       </c>
       <c r="D19" s="9" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="E19" s="3"/>
       <c r="F19" s="3"/>
@@ -6933,7 +6936,7 @@
         <v>236</v>
       </c>
       <c r="D20" s="9" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="E20" s="3"/>
       <c r="F20" s="3"/>
@@ -6952,7 +6955,7 @@
         <v>236</v>
       </c>
       <c r="D21" s="9" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="E21" s="3"/>
       <c r="F21" s="3"/>
@@ -6968,7 +6971,7 @@
         <v>170</v>
       </c>
       <c r="C22" s="9" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="D22" s="9" t="s">
         <v>228</v>
@@ -6978,7 +6981,7 @@
       </c>
       <c r="F22" s="3"/>
       <c r="G22" s="3" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.15">
@@ -6989,17 +6992,17 @@
         <v>170</v>
       </c>
       <c r="C23" s="9" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="D23" s="9" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="E23" s="3" t="b">
         <v>1</v>
       </c>
       <c r="F23" s="3"/>
       <c r="G23" s="3" t="s">
-        <v>333</v>
+        <v>334</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.15">
@@ -7010,15 +7013,15 @@
         <v>170</v>
       </c>
       <c r="C24" s="9" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="D24" s="9" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="E24" s="3"/>
       <c r="F24" s="3"/>
       <c r="G24" s="3" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.15">
@@ -7029,15 +7032,15 @@
         <v>170</v>
       </c>
       <c r="C25" s="9" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="D25" s="9" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="E25" s="3"/>
       <c r="F25" s="3"/>
       <c r="G25" s="3" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.15">
@@ -7048,15 +7051,15 @@
         <v>170</v>
       </c>
       <c r="C26" s="9" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="D26" s="9" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="E26" s="3"/>
       <c r="F26" s="3"/>
       <c r="G26" s="3" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.15">
@@ -7067,7 +7070,7 @@
         <v>170</v>
       </c>
       <c r="C27" s="9" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="D27" s="9" t="s">
         <v>229</v>
@@ -7088,10 +7091,10 @@
         <v>170</v>
       </c>
       <c r="C28" s="9" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="D28" s="9" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="E28" s="3" t="b">
         <v>0</v>
@@ -7109,10 +7112,10 @@
         <v>170</v>
       </c>
       <c r="C29" s="9" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="D29" s="9" t="s">
-        <v>341</v>
+        <v>342</v>
       </c>
       <c r="E29" s="3"/>
       <c r="F29" s="3"/>
@@ -7128,10 +7131,10 @@
         <v>170</v>
       </c>
       <c r="C30" s="9" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="D30" s="9" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="E30" s="3"/>
       <c r="F30" s="3"/>
@@ -7147,10 +7150,10 @@
         <v>170</v>
       </c>
       <c r="C31" s="9" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="D31" s="9" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
       <c r="E31" s="3"/>
       <c r="F31" s="3"/>
@@ -7166,13 +7169,13 @@
         <v>170</v>
       </c>
       <c r="C32" s="9" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="D32" s="9" t="s">
-        <v>552</v>
+        <v>553</v>
       </c>
       <c r="E32" s="3" t="s">
-        <v>344</v>
+        <v>345</v>
       </c>
       <c r="F32" s="3"/>
       <c r="G32" s="3"/>
@@ -7188,10 +7191,10 @@
         <v>237</v>
       </c>
       <c r="D33" s="9" t="s">
-        <v>553</v>
+        <v>554</v>
       </c>
       <c r="E33" s="3" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="F33" s="3"/>
       <c r="G33" s="3"/>
@@ -7204,10 +7207,10 @@
         <v>170</v>
       </c>
       <c r="C34" s="9" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="D34" s="9" t="s">
-        <v>554</v>
+        <v>555</v>
       </c>
       <c r="E34" s="3" t="b">
         <v>0</v>
@@ -7223,13 +7226,13 @@
         <v>170</v>
       </c>
       <c r="C35" s="9" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="D35" s="9" t="s">
-        <v>560</v>
+        <v>561</v>
       </c>
       <c r="E35" s="3" t="s">
-        <v>344</v>
+        <v>345</v>
       </c>
       <c r="F35" s="3"/>
       <c r="G35" s="3"/>
@@ -7245,10 +7248,10 @@
         <v>237</v>
       </c>
       <c r="D36" s="9" t="s">
-        <v>559</v>
+        <v>560</v>
       </c>
       <c r="E36" s="3" t="s">
-        <v>567</v>
+        <v>568</v>
       </c>
       <c r="F36" s="3"/>
       <c r="G36" s="3"/>
@@ -7261,10 +7264,10 @@
         <v>170</v>
       </c>
       <c r="C37" s="9" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="D37" s="9" t="s">
-        <v>558</v>
+        <v>559</v>
       </c>
       <c r="E37" s="3" t="b">
         <v>0</v>
@@ -7280,13 +7283,13 @@
         <v>170</v>
       </c>
       <c r="C38" s="9" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="D38" s="9" t="s">
-        <v>564</v>
+        <v>565</v>
       </c>
       <c r="E38" s="3" t="s">
-        <v>344</v>
+        <v>345</v>
       </c>
       <c r="F38" s="3"/>
       <c r="G38" s="3"/>
@@ -7302,10 +7305,10 @@
         <v>237</v>
       </c>
       <c r="D39" s="9" t="s">
-        <v>565</v>
+        <v>566</v>
       </c>
       <c r="E39" s="3" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="F39" s="3"/>
       <c r="G39" s="3"/>
@@ -7318,10 +7321,10 @@
         <v>170</v>
       </c>
       <c r="C40" s="9" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="D40" s="9" t="s">
-        <v>566</v>
+        <v>567</v>
       </c>
       <c r="E40" s="3" t="b">
         <v>0</v>
@@ -7337,17 +7340,17 @@
         <v>170</v>
       </c>
       <c r="C41" s="9" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="D41" s="9" t="s">
-        <v>555</v>
+        <v>556</v>
       </c>
       <c r="E41" s="3" t="s">
-        <v>344</v>
+        <v>345</v>
       </c>
       <c r="F41" s="3"/>
       <c r="G41" s="3" t="s">
-        <v>344</v>
+        <v>345</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.15">
@@ -7361,14 +7364,14 @@
         <v>237</v>
       </c>
       <c r="D42" s="9" t="s">
-        <v>556</v>
+        <v>557</v>
       </c>
       <c r="E42" s="3" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="F42" s="3"/>
       <c r="G42" s="3" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
     </row>
     <row r="43" spans="1:7" s="2" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -7379,10 +7382,10 @@
         <v>170</v>
       </c>
       <c r="C43" s="9" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="D43" s="9" t="s">
-        <v>557</v>
+        <v>558</v>
       </c>
       <c r="E43" s="3" t="b">
         <v>1</v>
@@ -7400,17 +7403,17 @@
         <v>170</v>
       </c>
       <c r="C44" s="9" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="D44" s="9" t="s">
-        <v>561</v>
+        <v>562</v>
       </c>
       <c r="E44" s="3" t="s">
-        <v>344</v>
+        <v>345</v>
       </c>
       <c r="F44" s="3"/>
       <c r="G44" s="3" t="s">
-        <v>344</v>
+        <v>345</v>
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.15">
@@ -7424,14 +7427,14 @@
         <v>237</v>
       </c>
       <c r="D45" s="9" t="s">
-        <v>562</v>
+        <v>563</v>
       </c>
       <c r="E45" s="3" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="F45" s="3"/>
       <c r="G45" s="3" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
     </row>
     <row r="46" spans="1:7" s="2" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -7442,10 +7445,10 @@
         <v>170</v>
       </c>
       <c r="C46" s="9" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="D46" s="9" t="s">
-        <v>563</v>
+        <v>564</v>
       </c>
       <c r="E46" s="3" t="b">
         <v>1</v>
@@ -7466,10 +7469,10 @@
         <v>234</v>
       </c>
       <c r="D47" s="9" t="s">
-        <v>583</v>
+        <v>584</v>
       </c>
       <c r="E47" s="3" t="s">
-        <v>584</v>
+        <v>585</v>
       </c>
       <c r="F47" s="3"/>
       <c r="G47" s="3"/>
@@ -7482,7 +7485,7 @@
         <v>170</v>
       </c>
       <c r="C48" s="9" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="D48" s="9" t="s">
         <v>241</v>
@@ -7533,7 +7536,7 @@
         <v>170</v>
       </c>
       <c r="C51" s="9" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="D51" s="9" t="s">
         <v>244</v>
@@ -7552,7 +7555,7 @@
         <v>170</v>
       </c>
       <c r="C52" s="9" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="D52" s="9" t="s">
         <v>245</v>
@@ -7571,7 +7574,7 @@
         <v>170</v>
       </c>
       <c r="C53" s="9" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="D53" s="9" t="s">
         <v>246</v>
@@ -7590,7 +7593,7 @@
         <v>170</v>
       </c>
       <c r="C54" s="9" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="D54" s="9" t="s">
         <v>247</v>
@@ -7615,7 +7618,7 @@
         <v>238</v>
       </c>
       <c r="E55" s="3" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
       <c r="F55" s="3"/>
       <c r="G55" s="3"/>
@@ -7631,10 +7634,10 @@
         <v>235</v>
       </c>
       <c r="D56" s="9" t="s">
-        <v>348</v>
+        <v>349</v>
       </c>
       <c r="E56" s="3" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
       <c r="F56" s="3"/>
       <c r="G56" s="3"/>
@@ -7669,7 +7672,7 @@
         <v>236</v>
       </c>
       <c r="D58" s="9" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="E58" s="3">
         <v>1</v>
@@ -7685,13 +7688,13 @@
         <v>170</v>
       </c>
       <c r="C59" s="9" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="D59" s="9" t="s">
         <v>239</v>
       </c>
       <c r="E59" s="3" t="s">
-        <v>351</v>
+        <v>352</v>
       </c>
       <c r="F59" s="3"/>
       <c r="G59" s="3"/>
@@ -7704,13 +7707,13 @@
         <v>170</v>
       </c>
       <c r="C60" s="9" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="D60" s="9" t="s">
-        <v>352</v>
+        <v>353</v>
       </c>
       <c r="E60" s="3" t="s">
-        <v>353</v>
+        <v>354</v>
       </c>
       <c r="F60" s="3"/>
       <c r="G60" s="3"/>
@@ -7723,7 +7726,7 @@
         <v>170</v>
       </c>
       <c r="C61" s="9" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="D61" s="9" t="s">
         <v>240</v>
@@ -7742,10 +7745,10 @@
         <v>170</v>
       </c>
       <c r="C62" s="9" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="D62" s="9" t="s">
-        <v>354</v>
+        <v>355</v>
       </c>
       <c r="E62" s="3" t="b">
         <v>0</v>
@@ -7761,13 +7764,13 @@
         <v>170</v>
       </c>
       <c r="C63" s="9" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="D63" s="9" t="s">
-        <v>568</v>
+        <v>569</v>
       </c>
       <c r="E63" s="3" t="s">
-        <v>344</v>
+        <v>345</v>
       </c>
       <c r="F63" s="3"/>
       <c r="G63" s="3"/>
@@ -7783,10 +7786,10 @@
         <v>237</v>
       </c>
       <c r="D64" s="9" t="s">
-        <v>569</v>
+        <v>570</v>
       </c>
       <c r="E64" s="3" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="F64" s="3"/>
       <c r="G64" s="3"/>
@@ -7799,10 +7802,10 @@
         <v>170</v>
       </c>
       <c r="C65" s="9" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="D65" s="9" t="s">
-        <v>570</v>
+        <v>571</v>
       </c>
       <c r="E65" s="3" t="b">
         <v>0</v>
@@ -7818,13 +7821,13 @@
         <v>170</v>
       </c>
       <c r="C66" s="9" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="D66" s="9" t="s">
-        <v>571</v>
+        <v>572</v>
       </c>
       <c r="E66" s="3" t="s">
-        <v>344</v>
+        <v>345</v>
       </c>
       <c r="F66" s="3"/>
       <c r="G66" s="3"/>
@@ -7840,10 +7843,10 @@
         <v>237</v>
       </c>
       <c r="D67" s="9" t="s">
-        <v>572</v>
+        <v>573</v>
       </c>
       <c r="E67" s="3" t="s">
-        <v>567</v>
+        <v>568</v>
       </c>
       <c r="F67" s="3"/>
       <c r="G67" s="3"/>
@@ -7856,10 +7859,10 @@
         <v>170</v>
       </c>
       <c r="C68" s="9" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="D68" s="9" t="s">
-        <v>573</v>
+        <v>574</v>
       </c>
       <c r="E68" s="3" t="b">
         <v>0</v>
@@ -7875,13 +7878,13 @@
         <v>170</v>
       </c>
       <c r="C69" s="9" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="D69" s="9" t="s">
-        <v>574</v>
+        <v>575</v>
       </c>
       <c r="E69" s="3" t="s">
-        <v>344</v>
+        <v>345</v>
       </c>
       <c r="F69" s="3"/>
       <c r="G69" s="3"/>
@@ -7897,10 +7900,10 @@
         <v>237</v>
       </c>
       <c r="D70" s="9" t="s">
-        <v>575</v>
+        <v>576</v>
       </c>
       <c r="E70" s="3" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="F70" s="3"/>
       <c r="G70" s="3"/>
@@ -7913,10 +7916,10 @@
         <v>170</v>
       </c>
       <c r="C71" s="9" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="D71" s="9" t="s">
-        <v>576</v>
+        <v>577</v>
       </c>
       <c r="E71" s="3" t="b">
         <v>0</v>
@@ -7932,13 +7935,13 @@
         <v>170</v>
       </c>
       <c r="C72" s="9" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="D72" s="9" t="s">
-        <v>577</v>
+        <v>578</v>
       </c>
       <c r="E72" s="3" t="s">
-        <v>344</v>
+        <v>345</v>
       </c>
       <c r="F72" s="3"/>
       <c r="G72" s="3"/>
@@ -7954,10 +7957,10 @@
         <v>237</v>
       </c>
       <c r="D73" s="9" t="s">
-        <v>578</v>
+        <v>579</v>
       </c>
       <c r="E73" s="3" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="F73" s="3"/>
       <c r="G73" s="3"/>
@@ -7970,10 +7973,10 @@
         <v>170</v>
       </c>
       <c r="C74" s="9" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="D74" s="9" t="s">
-        <v>579</v>
+        <v>580</v>
       </c>
       <c r="E74" s="3" t="b">
         <v>1</v>
@@ -7989,13 +7992,13 @@
         <v>170</v>
       </c>
       <c r="C75" s="9" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="D75" s="9" t="s">
-        <v>580</v>
+        <v>581</v>
       </c>
       <c r="E75" s="3" t="s">
-        <v>344</v>
+        <v>345</v>
       </c>
       <c r="F75" s="3"/>
       <c r="G75" s="3"/>
@@ -8011,10 +8014,10 @@
         <v>237</v>
       </c>
       <c r="D76" s="9" t="s">
-        <v>581</v>
+        <v>582</v>
       </c>
       <c r="E76" s="3" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="F76" s="3"/>
       <c r="G76" s="3"/>
@@ -8027,10 +8030,10 @@
         <v>170</v>
       </c>
       <c r="C77" s="9" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="D77" s="9" t="s">
-        <v>582</v>
+        <v>583</v>
       </c>
       <c r="E77" s="3" t="b">
         <v>1</v>
@@ -8049,10 +8052,10 @@
         <v>234</v>
       </c>
       <c r="D78" s="9" t="s">
-        <v>355</v>
+        <v>356</v>
       </c>
       <c r="E78" s="3" t="s">
-        <v>356</v>
+        <v>357</v>
       </c>
       <c r="F78" s="3"/>
       <c r="G78" s="3"/>
@@ -8065,10 +8068,10 @@
         <v>170</v>
       </c>
       <c r="C79" s="9" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="D79" s="9" t="s">
-        <v>357</v>
+        <v>358</v>
       </c>
       <c r="E79" s="3"/>
       <c r="F79" s="3"/>
@@ -8085,7 +8088,7 @@
         <v>232</v>
       </c>
       <c r="D80" s="9" t="s">
-        <v>358</v>
+        <v>359</v>
       </c>
       <c r="E80" s="3"/>
       <c r="F80" s="3"/>
@@ -8102,7 +8105,7 @@
         <v>233</v>
       </c>
       <c r="D81" s="9" t="s">
-        <v>359</v>
+        <v>360</v>
       </c>
       <c r="E81" s="3"/>
       <c r="F81" s="3"/>
@@ -8116,10 +8119,10 @@
         <v>170</v>
       </c>
       <c r="C82" s="9" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="D82" s="9" t="s">
-        <v>360</v>
+        <v>361</v>
       </c>
       <c r="E82" s="3" t="b">
         <v>1</v>
@@ -8135,10 +8138,10 @@
         <v>170</v>
       </c>
       <c r="C83" s="9" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="D83" s="9" t="s">
-        <v>361</v>
+        <v>362</v>
       </c>
       <c r="E83" s="3" t="b">
         <v>0</v>
@@ -8154,10 +8157,10 @@
         <v>170</v>
       </c>
       <c r="C84" s="9" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="D84" s="9" t="s">
-        <v>362</v>
+        <v>363</v>
       </c>
       <c r="E84" s="3" t="b">
         <v>0</v>
@@ -8173,10 +8176,10 @@
         <v>170</v>
       </c>
       <c r="C85" s="9" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="D85" s="9" t="s">
-        <v>363</v>
+        <v>364</v>
       </c>
       <c r="E85" s="3" t="b">
         <v>1</v>
@@ -8195,10 +8198,10 @@
         <v>235</v>
       </c>
       <c r="D86" s="9" t="s">
-        <v>364</v>
+        <v>365</v>
       </c>
       <c r="E86" s="3" t="s">
-        <v>365</v>
+        <v>366</v>
       </c>
       <c r="F86" s="3"/>
       <c r="G86" s="3"/>
@@ -8214,10 +8217,10 @@
         <v>235</v>
       </c>
       <c r="D87" s="9" t="s">
-        <v>366</v>
+        <v>367</v>
       </c>
       <c r="E87" s="3" t="s">
-        <v>367</v>
+        <v>368</v>
       </c>
       <c r="F87" s="3"/>
       <c r="G87" s="3"/>
@@ -8233,7 +8236,7 @@
         <v>236</v>
       </c>
       <c r="D88" s="9" t="s">
-        <v>368</v>
+        <v>369</v>
       </c>
       <c r="E88" s="3">
         <v>0</v>
@@ -8252,7 +8255,7 @@
         <v>236</v>
       </c>
       <c r="D89" s="9" t="s">
-        <v>369</v>
+        <v>370</v>
       </c>
       <c r="E89" s="3">
         <v>1</v>
@@ -8268,13 +8271,13 @@
         <v>170</v>
       </c>
       <c r="C90" s="9" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="D90" s="9" t="s">
-        <v>370</v>
+        <v>371</v>
       </c>
       <c r="E90" s="3" t="s">
-        <v>371</v>
+        <v>372</v>
       </c>
       <c r="F90" s="3"/>
       <c r="G90" s="3"/>
@@ -8287,13 +8290,13 @@
         <v>170</v>
       </c>
       <c r="C91" s="9" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="D91" s="9" t="s">
-        <v>372</v>
+        <v>373</v>
       </c>
       <c r="E91" s="3" t="s">
-        <v>373</v>
+        <v>374</v>
       </c>
       <c r="F91" s="3"/>
       <c r="G91" s="3"/>
@@ -8306,10 +8309,10 @@
         <v>170</v>
       </c>
       <c r="C92" s="9" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="D92" s="9" t="s">
-        <v>374</v>
+        <v>375</v>
       </c>
       <c r="E92" s="3" t="b">
         <v>1</v>
@@ -8325,10 +8328,10 @@
         <v>170</v>
       </c>
       <c r="C93" s="9" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="D93" s="9" t="s">
-        <v>375</v>
+        <v>376</v>
       </c>
       <c r="E93" s="3" t="b">
         <v>0</v>
@@ -8344,10 +8347,10 @@
         <v>170</v>
       </c>
       <c r="C94" s="9" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="D94" s="9" t="s">
-        <v>376</v>
+        <v>377</v>
       </c>
       <c r="E94" s="3"/>
       <c r="F94" s="3"/>
@@ -8364,7 +8367,7 @@
         <v>237</v>
       </c>
       <c r="D95" s="9" t="s">
-        <v>377</v>
+        <v>378</v>
       </c>
       <c r="E95" s="3"/>
       <c r="F95" s="3"/>
@@ -8378,10 +8381,10 @@
         <v>170</v>
       </c>
       <c r="C96" s="9" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="D96" s="9" t="s">
-        <v>378</v>
+        <v>379</v>
       </c>
       <c r="E96" s="3" t="b">
         <v>0</v>
@@ -8400,10 +8403,10 @@
         <v>234</v>
       </c>
       <c r="D97" s="9" t="s">
-        <v>379</v>
+        <v>380</v>
       </c>
       <c r="E97" s="3" t="s">
-        <v>380</v>
+        <v>381</v>
       </c>
       <c r="F97" s="3"/>
       <c r="G97" s="3"/>
@@ -8416,10 +8419,10 @@
         <v>170</v>
       </c>
       <c r="C98" s="9" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="D98" s="9" t="s">
-        <v>381</v>
+        <v>382</v>
       </c>
       <c r="E98" s="3"/>
       <c r="F98" s="3"/>
@@ -8436,7 +8439,7 @@
         <v>232</v>
       </c>
       <c r="D99" s="9" t="s">
-        <v>382</v>
+        <v>383</v>
       </c>
       <c r="E99" s="3"/>
       <c r="F99" s="3"/>
@@ -8453,7 +8456,7 @@
         <v>233</v>
       </c>
       <c r="D100" s="9" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
       <c r="E100" s="3"/>
       <c r="F100" s="3"/>
@@ -8467,10 +8470,10 @@
         <v>170</v>
       </c>
       <c r="C101" s="9" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="D101" s="9" t="s">
-        <v>384</v>
+        <v>385</v>
       </c>
       <c r="E101" s="3" t="b">
         <v>1</v>
@@ -8486,10 +8489,10 @@
         <v>170</v>
       </c>
       <c r="C102" s="9" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="D102" s="9" t="s">
-        <v>385</v>
+        <v>386</v>
       </c>
       <c r="E102" s="3" t="b">
         <v>0</v>
@@ -8505,10 +8508,10 @@
         <v>170</v>
       </c>
       <c r="C103" s="9" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="D103" s="9" t="s">
-        <v>386</v>
+        <v>387</v>
       </c>
       <c r="E103" s="3" t="b">
         <v>0</v>
@@ -8524,10 +8527,10 @@
         <v>170</v>
       </c>
       <c r="C104" s="9" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="D104" s="9" t="s">
-        <v>387</v>
+        <v>388</v>
       </c>
       <c r="E104" s="3" t="b">
         <v>1</v>
@@ -8546,10 +8549,10 @@
         <v>235</v>
       </c>
       <c r="D105" s="9" t="s">
-        <v>388</v>
+        <v>389</v>
       </c>
       <c r="E105" s="3" t="s">
-        <v>389</v>
+        <v>390</v>
       </c>
       <c r="F105" s="3"/>
       <c r="G105" s="3"/>
@@ -8565,10 +8568,10 @@
         <v>235</v>
       </c>
       <c r="D106" s="9" t="s">
-        <v>390</v>
+        <v>391</v>
       </c>
       <c r="E106" s="3" t="s">
-        <v>391</v>
+        <v>392</v>
       </c>
       <c r="F106" s="3"/>
       <c r="G106" s="3"/>
@@ -8584,7 +8587,7 @@
         <v>236</v>
       </c>
       <c r="D107" s="9" t="s">
-        <v>392</v>
+        <v>393</v>
       </c>
       <c r="E107" s="3">
         <v>0</v>
@@ -8603,7 +8606,7 @@
         <v>236</v>
       </c>
       <c r="D108" s="9" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="E108" s="3">
         <v>1</v>
@@ -8619,10 +8622,10 @@
         <v>170</v>
       </c>
       <c r="C109" s="9" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="D109" s="9" t="s">
-        <v>394</v>
+        <v>395</v>
       </c>
       <c r="E109" s="3" t="b">
         <v>0</v>
@@ -8638,10 +8641,10 @@
         <v>170</v>
       </c>
       <c r="C110" s="9" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="D110" s="9" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
       <c r="E110" s="3" t="b">
         <v>1</v>
@@ -8657,10 +8660,10 @@
         <v>170</v>
       </c>
       <c r="C111" s="9" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="D111" s="9" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="E111" s="3" t="b">
         <v>1</v>
@@ -8676,10 +8679,10 @@
         <v>170</v>
       </c>
       <c r="C112" s="9" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="D112" s="9" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="E112" s="3" t="b">
         <v>0</v>
@@ -8698,10 +8701,10 @@
         <v>234</v>
       </c>
       <c r="D113" s="9" t="s">
-        <v>398</v>
+        <v>399</v>
       </c>
       <c r="E113" s="3" t="s">
-        <v>399</v>
+        <v>400</v>
       </c>
       <c r="F113" s="3"/>
       <c r="G113" s="3"/>
@@ -8714,10 +8717,10 @@
         <v>170</v>
       </c>
       <c r="C114" s="9" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="D114" s="9" t="s">
-        <v>400</v>
+        <v>401</v>
       </c>
       <c r="E114" s="3"/>
       <c r="F114" s="3"/>
@@ -8734,7 +8737,7 @@
         <v>232</v>
       </c>
       <c r="D115" s="9" t="s">
-        <v>401</v>
+        <v>402</v>
       </c>
       <c r="E115" s="3"/>
       <c r="F115" s="3"/>
@@ -8751,7 +8754,7 @@
         <v>233</v>
       </c>
       <c r="D116" s="9" t="s">
-        <v>402</v>
+        <v>403</v>
       </c>
       <c r="E116" s="3"/>
       <c r="F116" s="3"/>
@@ -8765,10 +8768,10 @@
         <v>170</v>
       </c>
       <c r="C117" s="9" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="D117" s="9" t="s">
-        <v>403</v>
+        <v>404</v>
       </c>
       <c r="E117" s="3" t="b">
         <v>1</v>
@@ -8784,10 +8787,10 @@
         <v>170</v>
       </c>
       <c r="C118" s="9" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="D118" s="9" t="s">
-        <v>404</v>
+        <v>405</v>
       </c>
       <c r="E118" s="3" t="b">
         <v>0</v>
@@ -8803,10 +8806,10 @@
         <v>170</v>
       </c>
       <c r="C119" s="9" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="D119" s="9" t="s">
-        <v>405</v>
+        <v>406</v>
       </c>
       <c r="E119" s="3" t="b">
         <v>0</v>
@@ -8822,10 +8825,10 @@
         <v>170</v>
       </c>
       <c r="C120" s="9" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="D120" s="9" t="s">
-        <v>406</v>
+        <v>407</v>
       </c>
       <c r="E120" s="3" t="b">
         <v>1</v>
@@ -8844,10 +8847,10 @@
         <v>235</v>
       </c>
       <c r="D121" s="9" t="s">
-        <v>407</v>
+        <v>408</v>
       </c>
       <c r="E121" s="3" t="s">
-        <v>408</v>
+        <v>409</v>
       </c>
       <c r="F121" s="3"/>
       <c r="G121" s="3"/>
@@ -8863,10 +8866,10 @@
         <v>235</v>
       </c>
       <c r="D122" s="9" t="s">
-        <v>409</v>
+        <v>410</v>
       </c>
       <c r="E122" s="3" t="s">
-        <v>410</v>
+        <v>411</v>
       </c>
       <c r="F122" s="3"/>
       <c r="G122" s="3"/>
@@ -8882,7 +8885,7 @@
         <v>236</v>
       </c>
       <c r="D123" s="9" t="s">
-        <v>411</v>
+        <v>412</v>
       </c>
       <c r="E123" s="3">
         <v>0</v>
@@ -8901,7 +8904,7 @@
         <v>236</v>
       </c>
       <c r="D124" s="9" t="s">
-        <v>412</v>
+        <v>413</v>
       </c>
       <c r="E124" s="3">
         <v>1</v>
@@ -8917,13 +8920,13 @@
         <v>170</v>
       </c>
       <c r="C125" s="9" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="D125" s="9" t="s">
-        <v>413</v>
+        <v>414</v>
       </c>
       <c r="E125" s="3" t="s">
-        <v>414</v>
+        <v>415</v>
       </c>
       <c r="F125" s="3"/>
       <c r="G125" s="3"/>
@@ -8936,13 +8939,13 @@
         <v>170</v>
       </c>
       <c r="C126" s="9" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="D126" s="9" t="s">
-        <v>415</v>
+        <v>416</v>
       </c>
       <c r="E126" s="3" t="s">
-        <v>416</v>
+        <v>417</v>
       </c>
       <c r="F126" s="3"/>
       <c r="G126" s="3"/>
@@ -8955,10 +8958,10 @@
         <v>170</v>
       </c>
       <c r="C127" s="9" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="D127" s="9" t="s">
-        <v>417</v>
+        <v>418</v>
       </c>
       <c r="E127" s="3" t="b">
         <v>1</v>
@@ -8974,10 +8977,10 @@
         <v>170</v>
       </c>
       <c r="C128" s="9" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="D128" s="9" t="s">
-        <v>418</v>
+        <v>419</v>
       </c>
       <c r="E128" s="3" t="b">
         <v>0</v>
@@ -8996,10 +8999,10 @@
         <v>234</v>
       </c>
       <c r="D129" s="9" t="s">
-        <v>419</v>
+        <v>420</v>
       </c>
       <c r="E129" s="3" t="s">
-        <v>420</v>
+        <v>421</v>
       </c>
       <c r="F129" s="3"/>
       <c r="G129" s="3"/>
@@ -9012,10 +9015,10 @@
         <v>170</v>
       </c>
       <c r="C130" s="9" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="D130" s="9" t="s">
-        <v>421</v>
+        <v>422</v>
       </c>
       <c r="E130" s="3"/>
       <c r="F130" s="3"/>
@@ -9032,7 +9035,7 @@
         <v>232</v>
       </c>
       <c r="D131" s="9" t="s">
-        <v>422</v>
+        <v>423</v>
       </c>
       <c r="E131" s="3"/>
       <c r="F131" s="3"/>
@@ -9049,7 +9052,7 @@
         <v>233</v>
       </c>
       <c r="D132" s="9" t="s">
-        <v>423</v>
+        <v>424</v>
       </c>
       <c r="E132" s="3"/>
       <c r="F132" s="3"/>
@@ -9063,10 +9066,10 @@
         <v>170</v>
       </c>
       <c r="C133" s="9" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="D133" s="9" t="s">
-        <v>424</v>
+        <v>425</v>
       </c>
       <c r="E133" s="3" t="b">
         <v>1</v>
@@ -9082,10 +9085,10 @@
         <v>170</v>
       </c>
       <c r="C134" s="9" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="D134" s="9" t="s">
-        <v>425</v>
+        <v>426</v>
       </c>
       <c r="E134" s="3" t="b">
         <v>0</v>
@@ -9101,10 +9104,10 @@
         <v>170</v>
       </c>
       <c r="C135" s="9" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="D135" s="9" t="s">
-        <v>426</v>
+        <v>427</v>
       </c>
       <c r="E135" s="3" t="b">
         <v>0</v>
@@ -9120,10 +9123,10 @@
         <v>170</v>
       </c>
       <c r="C136" s="9" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="D136" s="9" t="s">
-        <v>427</v>
+        <v>428</v>
       </c>
       <c r="E136" s="3" t="b">
         <v>1</v>
@@ -9142,10 +9145,10 @@
         <v>235</v>
       </c>
       <c r="D137" s="9" t="s">
-        <v>428</v>
+        <v>429</v>
       </c>
       <c r="E137" s="3" t="s">
-        <v>429</v>
+        <v>430</v>
       </c>
       <c r="F137" s="3"/>
       <c r="G137" s="3"/>
@@ -9161,10 +9164,10 @@
         <v>235</v>
       </c>
       <c r="D138" s="9" t="s">
-        <v>430</v>
+        <v>431</v>
       </c>
       <c r="E138" s="3" t="s">
-        <v>431</v>
+        <v>432</v>
       </c>
       <c r="F138" s="3"/>
       <c r="G138" s="3"/>
@@ -9180,7 +9183,7 @@
         <v>236</v>
       </c>
       <c r="D139" s="9" t="s">
-        <v>432</v>
+        <v>433</v>
       </c>
       <c r="E139" s="3">
         <v>0</v>
@@ -9199,7 +9202,7 @@
         <v>236</v>
       </c>
       <c r="D140" s="9" t="s">
-        <v>433</v>
+        <v>434</v>
       </c>
       <c r="E140" s="3">
         <v>1</v>
@@ -9215,13 +9218,13 @@
         <v>170</v>
       </c>
       <c r="C141" s="9" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="D141" s="9" t="s">
-        <v>434</v>
+        <v>435</v>
       </c>
       <c r="E141" s="3" t="s">
-        <v>435</v>
+        <v>436</v>
       </c>
       <c r="F141" s="3"/>
       <c r="G141" s="3"/>
@@ -9234,13 +9237,13 @@
         <v>170</v>
       </c>
       <c r="C142" s="9" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="D142" s="9" t="s">
-        <v>436</v>
+        <v>437</v>
       </c>
       <c r="E142" s="3" t="s">
-        <v>437</v>
+        <v>438</v>
       </c>
       <c r="F142" s="3"/>
       <c r="G142" s="3"/>
@@ -9253,10 +9256,10 @@
         <v>170</v>
       </c>
       <c r="C143" s="9" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="D143" s="9" t="s">
-        <v>438</v>
+        <v>439</v>
       </c>
       <c r="E143" s="3" t="b">
         <v>1</v>
@@ -9272,10 +9275,10 @@
         <v>170</v>
       </c>
       <c r="C144" s="9" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="D144" s="9" t="s">
-        <v>439</v>
+        <v>440</v>
       </c>
       <c r="E144" s="3" t="b">
         <v>0</v>
@@ -9294,10 +9297,10 @@
         <v>234</v>
       </c>
       <c r="D145" s="9" t="s">
-        <v>440</v>
+        <v>441</v>
       </c>
       <c r="E145" s="3" t="s">
-        <v>441</v>
+        <v>442</v>
       </c>
       <c r="F145" s="3"/>
       <c r="G145" s="3"/>
@@ -9310,10 +9313,10 @@
         <v>170</v>
       </c>
       <c r="C146" s="9" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="D146" s="9" t="s">
-        <v>442</v>
+        <v>443</v>
       </c>
       <c r="E146" s="3"/>
       <c r="F146" s="3"/>
@@ -9330,7 +9333,7 @@
         <v>232</v>
       </c>
       <c r="D147" s="9" t="s">
-        <v>443</v>
+        <v>444</v>
       </c>
       <c r="E147" s="3"/>
       <c r="F147" s="3"/>
@@ -9347,7 +9350,7 @@
         <v>233</v>
       </c>
       <c r="D148" s="9" t="s">
-        <v>444</v>
+        <v>445</v>
       </c>
       <c r="E148" s="3"/>
       <c r="F148" s="3"/>
@@ -9361,10 +9364,10 @@
         <v>170</v>
       </c>
       <c r="C149" s="9" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="D149" s="9" t="s">
-        <v>445</v>
+        <v>446</v>
       </c>
       <c r="E149" s="3" t="b">
         <v>1</v>
@@ -9380,10 +9383,10 @@
         <v>170</v>
       </c>
       <c r="C150" s="9" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="D150" s="9" t="s">
-        <v>446</v>
+        <v>447</v>
       </c>
       <c r="E150" s="3" t="b">
         <v>0</v>
@@ -9399,10 +9402,10 @@
         <v>170</v>
       </c>
       <c r="C151" s="9" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="D151" s="9" t="s">
-        <v>447</v>
+        <v>448</v>
       </c>
       <c r="E151" s="3" t="b">
         <v>0</v>
@@ -9418,10 +9421,10 @@
         <v>170</v>
       </c>
       <c r="C152" s="9" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="D152" s="9" t="s">
-        <v>448</v>
+        <v>449</v>
       </c>
       <c r="E152" s="3" t="b">
         <v>1</v>
@@ -9440,10 +9443,10 @@
         <v>235</v>
       </c>
       <c r="D153" s="9" t="s">
-        <v>449</v>
+        <v>450</v>
       </c>
       <c r="E153" s="3" t="s">
-        <v>450</v>
+        <v>451</v>
       </c>
       <c r="F153" s="3"/>
       <c r="G153" s="3"/>
@@ -9459,10 +9462,10 @@
         <v>235</v>
       </c>
       <c r="D154" s="9" t="s">
-        <v>451</v>
+        <v>452</v>
       </c>
       <c r="E154" s="3" t="s">
-        <v>452</v>
+        <v>453</v>
       </c>
       <c r="F154" s="3"/>
       <c r="G154" s="3"/>
@@ -9478,7 +9481,7 @@
         <v>236</v>
       </c>
       <c r="D155" s="9" t="s">
-        <v>453</v>
+        <v>454</v>
       </c>
       <c r="E155" s="3">
         <v>0</v>
@@ -9497,7 +9500,7 @@
         <v>236</v>
       </c>
       <c r="D156" s="9" t="s">
-        <v>454</v>
+        <v>455</v>
       </c>
       <c r="E156" s="3">
         <v>1</v>
@@ -9513,13 +9516,13 @@
         <v>170</v>
       </c>
       <c r="C157" s="9" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="D157" s="9" t="s">
-        <v>455</v>
+        <v>456</v>
       </c>
       <c r="E157" s="3" t="s">
-        <v>456</v>
+        <v>457</v>
       </c>
       <c r="F157" s="3"/>
       <c r="G157" s="3"/>
@@ -9532,13 +9535,13 @@
         <v>170</v>
       </c>
       <c r="C158" s="9" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="D158" s="9" t="s">
-        <v>457</v>
+        <v>458</v>
       </c>
       <c r="E158" s="3" t="s">
-        <v>458</v>
+        <v>459</v>
       </c>
       <c r="F158" s="3"/>
       <c r="G158" s="3"/>
@@ -9551,10 +9554,10 @@
         <v>170</v>
       </c>
       <c r="C159" s="9" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="D159" s="9" t="s">
-        <v>459</v>
+        <v>460</v>
       </c>
       <c r="E159" s="3" t="b">
         <v>1</v>
@@ -9570,10 +9573,10 @@
         <v>170</v>
       </c>
       <c r="C160" s="9" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="D160" s="9" t="s">
-        <v>460</v>
+        <v>461</v>
       </c>
       <c r="E160" s="3" t="b">
         <v>0</v>
@@ -9592,10 +9595,10 @@
         <v>234</v>
       </c>
       <c r="D161" s="9" t="s">
-        <v>461</v>
+        <v>462</v>
       </c>
       <c r="E161" s="3" t="s">
-        <v>462</v>
+        <v>463</v>
       </c>
       <c r="F161" s="3"/>
       <c r="G161" s="3"/>
@@ -9608,10 +9611,10 @@
         <v>170</v>
       </c>
       <c r="C162" s="9" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="D162" s="9" t="s">
-        <v>463</v>
+        <v>464</v>
       </c>
       <c r="E162" s="3"/>
       <c r="F162" s="3"/>
@@ -9628,7 +9631,7 @@
         <v>232</v>
       </c>
       <c r="D163" s="9" t="s">
-        <v>464</v>
+        <v>465</v>
       </c>
       <c r="E163" s="3"/>
       <c r="F163" s="3"/>
@@ -9645,7 +9648,7 @@
         <v>233</v>
       </c>
       <c r="D164" s="9" t="s">
-        <v>465</v>
+        <v>466</v>
       </c>
       <c r="E164" s="3"/>
       <c r="F164" s="3"/>
@@ -9659,10 +9662,10 @@
         <v>170</v>
       </c>
       <c r="C165" s="9" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="D165" s="9" t="s">
-        <v>466</v>
+        <v>467</v>
       </c>
       <c r="E165" s="3" t="b">
         <v>1</v>
@@ -9678,10 +9681,10 @@
         <v>170</v>
       </c>
       <c r="C166" s="9" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="D166" s="9" t="s">
-        <v>467</v>
+        <v>468</v>
       </c>
       <c r="E166" s="3" t="b">
         <v>0</v>
@@ -9697,10 +9700,10 @@
         <v>170</v>
       </c>
       <c r="C167" s="9" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="D167" s="9" t="s">
-        <v>468</v>
+        <v>469</v>
       </c>
       <c r="E167" s="3" t="b">
         <v>0</v>
@@ -9716,10 +9719,10 @@
         <v>170</v>
       </c>
       <c r="C168" s="9" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="D168" s="9" t="s">
-        <v>469</v>
+        <v>470</v>
       </c>
       <c r="E168" s="3" t="b">
         <v>1</v>
@@ -9738,10 +9741,10 @@
         <v>235</v>
       </c>
       <c r="D169" s="9" t="s">
-        <v>470</v>
+        <v>471</v>
       </c>
       <c r="E169" s="3" t="s">
-        <v>471</v>
+        <v>472</v>
       </c>
       <c r="F169" s="3"/>
       <c r="G169" s="3"/>
@@ -9757,10 +9760,10 @@
         <v>235</v>
       </c>
       <c r="D170" s="9" t="s">
-        <v>472</v>
+        <v>473</v>
       </c>
       <c r="E170" s="3" t="s">
-        <v>473</v>
+        <v>474</v>
       </c>
       <c r="F170" s="3"/>
       <c r="G170" s="3"/>
@@ -9776,7 +9779,7 @@
         <v>236</v>
       </c>
       <c r="D171" s="9" t="s">
-        <v>474</v>
+        <v>475</v>
       </c>
       <c r="E171" s="3">
         <v>0</v>
@@ -9795,7 +9798,7 @@
         <v>236</v>
       </c>
       <c r="D172" s="9" t="s">
-        <v>475</v>
+        <v>476</v>
       </c>
       <c r="E172" s="3">
         <v>1</v>
@@ -9811,13 +9814,13 @@
         <v>170</v>
       </c>
       <c r="C173" s="9" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="D173" s="9" t="s">
-        <v>476</v>
+        <v>477</v>
       </c>
       <c r="E173" s="3" t="s">
-        <v>414</v>
+        <v>415</v>
       </c>
       <c r="F173" s="3"/>
       <c r="G173" s="3"/>
@@ -9830,13 +9833,13 @@
         <v>170</v>
       </c>
       <c r="C174" s="9" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="D174" s="9" t="s">
-        <v>477</v>
+        <v>478</v>
       </c>
       <c r="E174" s="3" t="s">
-        <v>416</v>
+        <v>417</v>
       </c>
       <c r="F174" s="3"/>
       <c r="G174" s="3"/>
@@ -9849,10 +9852,10 @@
         <v>170</v>
       </c>
       <c r="C175" s="9" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="D175" s="9" t="s">
-        <v>478</v>
+        <v>479</v>
       </c>
       <c r="E175" s="3" t="b">
         <v>1</v>
@@ -9868,10 +9871,10 @@
         <v>170</v>
       </c>
       <c r="C176" s="9" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="D176" s="9" t="s">
-        <v>479</v>
+        <v>480</v>
       </c>
       <c r="E176" s="3" t="b">
         <v>0</v>
@@ -9890,10 +9893,10 @@
         <v>234</v>
       </c>
       <c r="D177" s="9" t="s">
-        <v>480</v>
+        <v>481</v>
       </c>
       <c r="E177" s="3" t="s">
-        <v>481</v>
+        <v>482</v>
       </c>
       <c r="F177" s="3"/>
       <c r="G177" s="3"/>
@@ -9906,10 +9909,10 @@
         <v>170</v>
       </c>
       <c r="C178" s="9" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="D178" s="9" t="s">
-        <v>482</v>
+        <v>483</v>
       </c>
       <c r="E178" s="3"/>
       <c r="F178" s="3"/>
@@ -9926,7 +9929,7 @@
         <v>232</v>
       </c>
       <c r="D179" s="9" t="s">
-        <v>483</v>
+        <v>484</v>
       </c>
       <c r="E179" s="3"/>
       <c r="F179" s="3"/>
@@ -9943,7 +9946,7 @@
         <v>233</v>
       </c>
       <c r="D180" s="9" t="s">
-        <v>484</v>
+        <v>485</v>
       </c>
       <c r="E180" s="3"/>
       <c r="F180" s="3"/>
@@ -9957,10 +9960,10 @@
         <v>170</v>
       </c>
       <c r="C181" s="9" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="D181" s="9" t="s">
-        <v>485</v>
+        <v>486</v>
       </c>
       <c r="E181" s="3" t="b">
         <v>1</v>
@@ -9976,10 +9979,10 @@
         <v>170</v>
       </c>
       <c r="C182" s="9" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="D182" s="9" t="s">
-        <v>486</v>
+        <v>487</v>
       </c>
       <c r="E182" s="3" t="b">
         <v>0</v>
@@ -9995,10 +9998,10 @@
         <v>170</v>
       </c>
       <c r="C183" s="9" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="D183" s="9" t="s">
-        <v>487</v>
+        <v>488</v>
       </c>
       <c r="E183" s="3" t="b">
         <v>0</v>
@@ -10014,10 +10017,10 @@
         <v>170</v>
       </c>
       <c r="C184" s="9" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="D184" s="9" t="s">
-        <v>488</v>
+        <v>489</v>
       </c>
       <c r="E184" s="3" t="b">
         <v>1</v>
@@ -10036,10 +10039,10 @@
         <v>235</v>
       </c>
       <c r="D185" s="9" t="s">
-        <v>489</v>
+        <v>490</v>
       </c>
       <c r="E185" s="3" t="s">
-        <v>490</v>
+        <v>491</v>
       </c>
       <c r="F185" s="3"/>
       <c r="G185" s="3"/>
@@ -10055,10 +10058,10 @@
         <v>235</v>
       </c>
       <c r="D186" s="9" t="s">
-        <v>491</v>
+        <v>492</v>
       </c>
       <c r="E186" s="3" t="s">
-        <v>492</v>
+        <v>493</v>
       </c>
       <c r="F186" s="3"/>
       <c r="G186" s="3"/>
@@ -10074,10 +10077,10 @@
         <v>235</v>
       </c>
       <c r="D187" s="9" t="s">
-        <v>493</v>
+        <v>494</v>
       </c>
       <c r="E187" s="3" t="s">
-        <v>494</v>
+        <v>495</v>
       </c>
       <c r="F187" s="3"/>
       <c r="G187" s="3"/>
@@ -10093,10 +10096,10 @@
         <v>235</v>
       </c>
       <c r="D188" s="9" t="s">
-        <v>495</v>
+        <v>496</v>
       </c>
       <c r="E188" s="3" t="s">
-        <v>496</v>
+        <v>497</v>
       </c>
       <c r="F188" s="3"/>
       <c r="G188" s="3"/>
@@ -10112,7 +10115,7 @@
         <v>236</v>
       </c>
       <c r="D189" s="9" t="s">
-        <v>497</v>
+        <v>498</v>
       </c>
       <c r="E189" s="3">
         <v>0</v>
@@ -10131,7 +10134,7 @@
         <v>236</v>
       </c>
       <c r="D190" s="9" t="s">
-        <v>498</v>
+        <v>499</v>
       </c>
       <c r="E190" s="3">
         <v>1</v>
@@ -10150,7 +10153,7 @@
         <v>236</v>
       </c>
       <c r="D191" s="9" t="s">
-        <v>499</v>
+        <v>500</v>
       </c>
       <c r="E191" s="3">
         <v>2</v>
@@ -10169,7 +10172,7 @@
         <v>236</v>
       </c>
       <c r="D192" s="9" t="s">
-        <v>500</v>
+        <v>501</v>
       </c>
       <c r="E192" s="3">
         <v>3</v>
@@ -10185,13 +10188,13 @@
         <v>170</v>
       </c>
       <c r="C193" s="9" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="D193" s="9" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="E193" s="3" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="F193" s="3"/>
       <c r="G193" s="3"/>
@@ -10204,13 +10207,13 @@
         <v>170</v>
       </c>
       <c r="C194" s="9" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="D194" s="9" t="s">
-        <v>502</v>
+        <v>503</v>
       </c>
       <c r="E194" s="3" t="s">
-        <v>503</v>
+        <v>504</v>
       </c>
       <c r="F194" s="3"/>
       <c r="G194" s="3"/>
@@ -10223,13 +10226,13 @@
         <v>170</v>
       </c>
       <c r="C195" s="9" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="D195" s="9" t="s">
-        <v>504</v>
+        <v>505</v>
       </c>
       <c r="E195" s="3" t="s">
-        <v>505</v>
+        <v>506</v>
       </c>
       <c r="F195" s="3"/>
       <c r="G195" s="3"/>
@@ -10242,13 +10245,13 @@
         <v>170</v>
       </c>
       <c r="C196" s="9" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="D196" s="9" t="s">
-        <v>506</v>
+        <v>507</v>
       </c>
       <c r="E196" s="3" t="s">
-        <v>507</v>
+        <v>508</v>
       </c>
       <c r="F196" s="3"/>
       <c r="G196" s="3"/>
@@ -10261,10 +10264,10 @@
         <v>170</v>
       </c>
       <c r="C197" s="9" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="D197" s="9" t="s">
-        <v>508</v>
+        <v>509</v>
       </c>
       <c r="E197" s="3" t="b">
         <v>1</v>
@@ -10280,10 +10283,10 @@
         <v>170</v>
       </c>
       <c r="C198" s="9" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="D198" s="9" t="s">
-        <v>509</v>
+        <v>510</v>
       </c>
       <c r="E198" s="3" t="b">
         <v>0</v>
@@ -10302,10 +10305,10 @@
         <v>234</v>
       </c>
       <c r="D199" s="9" t="s">
-        <v>510</v>
+        <v>511</v>
       </c>
       <c r="E199" s="3" t="s">
-        <v>511</v>
+        <v>512</v>
       </c>
       <c r="F199" s="3"/>
       <c r="G199" s="3"/>
@@ -10318,10 +10321,10 @@
         <v>170</v>
       </c>
       <c r="C200" s="9" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="D200" s="9" t="s">
-        <v>512</v>
+        <v>513</v>
       </c>
       <c r="E200" s="3"/>
       <c r="F200" s="3"/>
@@ -10338,7 +10341,7 @@
         <v>232</v>
       </c>
       <c r="D201" s="9" t="s">
-        <v>513</v>
+        <v>514</v>
       </c>
       <c r="E201" s="3"/>
       <c r="F201" s="3"/>
@@ -10355,7 +10358,7 @@
         <v>233</v>
       </c>
       <c r="D202" s="9" t="s">
-        <v>514</v>
+        <v>515</v>
       </c>
       <c r="E202" s="3"/>
       <c r="F202" s="3"/>
@@ -10369,10 +10372,10 @@
         <v>170</v>
       </c>
       <c r="C203" s="9" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="D203" s="9" t="s">
-        <v>515</v>
+        <v>516</v>
       </c>
       <c r="E203" s="3" t="b">
         <v>1</v>
@@ -10388,10 +10391,10 @@
         <v>170</v>
       </c>
       <c r="C204" s="9" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="D204" s="9" t="s">
-        <v>516</v>
+        <v>517</v>
       </c>
       <c r="E204" s="3" t="b">
         <v>0</v>
@@ -10407,10 +10410,10 @@
         <v>170</v>
       </c>
       <c r="C205" s="9" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="D205" s="9" t="s">
-        <v>517</v>
+        <v>518</v>
       </c>
       <c r="E205" s="3" t="b">
         <v>0</v>
@@ -10426,10 +10429,10 @@
         <v>170</v>
       </c>
       <c r="C206" s="9" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="D206" s="9" t="s">
-        <v>518</v>
+        <v>519</v>
       </c>
       <c r="E206" s="3" t="b">
         <v>1</v>
@@ -10448,10 +10451,10 @@
         <v>235</v>
       </c>
       <c r="D207" s="9" t="s">
-        <v>519</v>
+        <v>520</v>
       </c>
       <c r="E207" s="3" t="s">
-        <v>520</v>
+        <v>521</v>
       </c>
       <c r="F207" s="3"/>
       <c r="G207" s="3"/>
@@ -10467,10 +10470,10 @@
         <v>235</v>
       </c>
       <c r="D208" s="9" t="s">
-        <v>521</v>
+        <v>522</v>
       </c>
       <c r="E208" s="3" t="s">
-        <v>522</v>
+        <v>523</v>
       </c>
       <c r="F208" s="3"/>
       <c r="G208" s="3"/>
@@ -10486,7 +10489,7 @@
         <v>236</v>
       </c>
       <c r="D209" s="9" t="s">
-        <v>523</v>
+        <v>524</v>
       </c>
       <c r="E209" s="3">
         <v>0</v>
@@ -10505,7 +10508,7 @@
         <v>236</v>
       </c>
       <c r="D210" s="9" t="s">
-        <v>524</v>
+        <v>525</v>
       </c>
       <c r="E210" s="3">
         <v>1</v>
@@ -10521,10 +10524,10 @@
         <v>170</v>
       </c>
       <c r="C211" s="9" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="D211" s="9" t="s">
-        <v>525</v>
+        <v>526</v>
       </c>
       <c r="E211" s="3" t="b">
         <v>0</v>
@@ -10540,10 +10543,10 @@
         <v>170</v>
       </c>
       <c r="C212" s="9" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="D212" s="9" t="s">
-        <v>526</v>
+        <v>527</v>
       </c>
       <c r="E212" s="3" t="b">
         <v>1</v>
@@ -10559,10 +10562,10 @@
         <v>170</v>
       </c>
       <c r="C213" s="9" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="D213" s="9" t="s">
-        <v>527</v>
+        <v>528</v>
       </c>
       <c r="E213" s="3" t="b">
         <v>1</v>
@@ -10578,10 +10581,10 @@
         <v>170</v>
       </c>
       <c r="C214" s="9" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="D214" s="9" t="s">
-        <v>528</v>
+        <v>529</v>
       </c>
       <c r="E214" s="3" t="b">
         <v>0</v>
@@ -10600,10 +10603,10 @@
         <v>234</v>
       </c>
       <c r="D215" s="9" t="s">
-        <v>529</v>
+        <v>530</v>
       </c>
       <c r="E215" s="3" t="s">
-        <v>530</v>
+        <v>531</v>
       </c>
       <c r="F215" s="3"/>
       <c r="G215" s="3"/>
@@ -10616,10 +10619,10 @@
         <v>170</v>
       </c>
       <c r="C216" s="9" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="D216" s="9" t="s">
-        <v>531</v>
+        <v>532</v>
       </c>
       <c r="E216" s="3"/>
       <c r="F216" s="3"/>
@@ -10636,7 +10639,7 @@
         <v>232</v>
       </c>
       <c r="D217" s="9" t="s">
-        <v>532</v>
+        <v>533</v>
       </c>
       <c r="E217" s="3"/>
       <c r="F217" s="3"/>
@@ -10653,7 +10656,7 @@
         <v>233</v>
       </c>
       <c r="D218" s="9" t="s">
-        <v>533</v>
+        <v>534</v>
       </c>
       <c r="E218" s="3"/>
       <c r="F218" s="3"/>
@@ -10667,10 +10670,10 @@
         <v>170</v>
       </c>
       <c r="C219" s="9" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="D219" s="9" t="s">
-        <v>534</v>
+        <v>535</v>
       </c>
       <c r="E219" s="3" t="b">
         <v>1</v>
@@ -10686,10 +10689,10 @@
         <v>170</v>
       </c>
       <c r="C220" s="9" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="D220" s="9" t="s">
-        <v>535</v>
+        <v>536</v>
       </c>
       <c r="E220" s="3" t="b">
         <v>0</v>
@@ -10705,10 +10708,10 @@
         <v>170</v>
       </c>
       <c r="C221" s="9" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="D221" s="9" t="s">
-        <v>536</v>
+        <v>537</v>
       </c>
       <c r="E221" s="3" t="b">
         <v>0</v>
@@ -10724,10 +10727,10 @@
         <v>170</v>
       </c>
       <c r="C222" s="9" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="D222" s="9" t="s">
-        <v>537</v>
+        <v>538</v>
       </c>
       <c r="E222" s="3" t="b">
         <v>1</v>
@@ -10746,10 +10749,10 @@
         <v>235</v>
       </c>
       <c r="D223" s="9" t="s">
-        <v>538</v>
+        <v>539</v>
       </c>
       <c r="E223" s="3" t="s">
-        <v>539</v>
+        <v>540</v>
       </c>
       <c r="F223" s="3"/>
       <c r="G223" s="3"/>
@@ -10765,10 +10768,10 @@
         <v>235</v>
       </c>
       <c r="D224" s="9" t="s">
-        <v>540</v>
+        <v>541</v>
       </c>
       <c r="E224" s="3" t="s">
-        <v>541</v>
+        <v>542</v>
       </c>
       <c r="F224" s="3"/>
       <c r="G224" s="3"/>
@@ -10784,7 +10787,7 @@
         <v>236</v>
       </c>
       <c r="D225" s="9" t="s">
-        <v>542</v>
+        <v>543</v>
       </c>
       <c r="E225" s="3">
         <v>0</v>
@@ -10803,7 +10806,7 @@
         <v>236</v>
       </c>
       <c r="D226" s="9" t="s">
-        <v>543</v>
+        <v>544</v>
       </c>
       <c r="E226" s="3">
         <v>1</v>
@@ -10819,10 +10822,10 @@
         <v>170</v>
       </c>
       <c r="C227" s="9" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="D227" s="9" t="s">
-        <v>544</v>
+        <v>545</v>
       </c>
       <c r="E227" s="3" t="b">
         <v>0</v>
@@ -10838,10 +10841,10 @@
         <v>170</v>
       </c>
       <c r="C228" s="9" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="D228" s="9" t="s">
-        <v>545</v>
+        <v>546</v>
       </c>
       <c r="E228" s="3" t="b">
         <v>1</v>
@@ -10857,10 +10860,10 @@
         <v>170</v>
       </c>
       <c r="C229" s="9" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="D229" s="9" t="s">
-        <v>546</v>
+        <v>547</v>
       </c>
       <c r="E229" s="3" t="b">
         <v>1</v>
@@ -10876,10 +10879,10 @@
         <v>170</v>
       </c>
       <c r="C230" s="9" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="D230" s="9" t="s">
-        <v>547</v>
+        <v>548</v>
       </c>
       <c r="E230" s="3" t="b">
         <v>0</v>

</xml_diff>

<commit_message>
Updating scoring mapping logic. Adding unit test
</commit_message>
<xml_diff>
--- a/src/test/resources/SBAC-IAB-FIXED-G11M-Winter-2017-2018.xlsx
+++ b/src/test/resources/SBAC-IAB-FIXED-G11M-Winter-2017-2018.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="34240" yWindow="6100" windowWidth="28800" windowHeight="17560" tabRatio="644" activeTab="3"/>
+    <workbookView xWindow="34240" yWindow="6100" windowWidth="28800" windowHeight="17560" tabRatio="644" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Package" sheetId="16" r:id="rId1"/>
@@ -20,12 +20,11 @@
     <sheet name="Tools" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="152511"/>
-  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1621" uniqueCount="587">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1630" uniqueCount="591">
   <si>
     <t>ItemId</t>
   </si>
@@ -1842,6 +1841,18 @@
   </si>
   <si>
     <t>BlueprintElementId</t>
+  </si>
+  <si>
+    <t>TestPackage.Blueprint.BlueprintElement-type</t>
+  </si>
+  <si>
+    <t>The type of the Blueprint Element</t>
+  </si>
+  <si>
+    <t>BlueprintElementType</t>
+  </si>
+  <si>
+    <t>test</t>
   </si>
 </sst>
 </file>
@@ -3251,13 +3262,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I49"/>
+  <dimension ref="A1:I50"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="4" ySplit="2" topLeftCell="E3" activePane="bottomRight" state="frozenSplit"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="F26" sqref="F26"/>
+      <selection pane="bottomRight" activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="55" defaultRowHeight="11" x14ac:dyDescent="0.15"/>
@@ -3345,256 +3356,266 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A4" s="17" t="s">
-        <v>127</v>
+        <v>587</v>
       </c>
       <c r="B4" s="9" t="s">
         <v>109</v>
       </c>
       <c r="C4" s="17" t="s">
-        <v>276</v>
-      </c>
-      <c r="D4" s="17" t="s">
-        <v>52</v>
-      </c>
-      <c r="E4" s="16">
-        <v>10</v>
-      </c>
-      <c r="F4" s="16">
-        <v>20</v>
-      </c>
-      <c r="G4" s="16">
-        <v>30</v>
-      </c>
-      <c r="H4" s="16">
-        <v>40</v>
-      </c>
-      <c r="I4" s="16">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" ht="22" x14ac:dyDescent="0.15">
+        <v>588</v>
+      </c>
+      <c r="D4" s="9" t="s">
+        <v>589</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>590</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>590</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>590</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>590</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>590</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A5" s="17" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="B5" s="9" t="s">
         <v>109</v>
       </c>
       <c r="C5" s="17" t="s">
+        <v>276</v>
+      </c>
+      <c r="D5" s="17" t="s">
+        <v>52</v>
+      </c>
+      <c r="E5" s="16">
+        <v>10</v>
+      </c>
+      <c r="F5" s="16">
+        <v>20</v>
+      </c>
+      <c r="G5" s="16">
+        <v>30</v>
+      </c>
+      <c r="H5" s="16">
+        <v>40</v>
+      </c>
+      <c r="I5" s="16">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="22" x14ac:dyDescent="0.15">
+      <c r="A6" s="17" t="s">
+        <v>126</v>
+      </c>
+      <c r="B6" s="9" t="s">
+        <v>109</v>
+      </c>
+      <c r="C6" s="17" t="s">
         <v>277</v>
       </c>
-      <c r="D5" s="17" t="s">
+      <c r="D6" s="17" t="s">
         <v>51</v>
       </c>
-      <c r="E5" s="16" t="s">
+      <c r="E6" s="16" t="s">
         <v>191</v>
       </c>
-      <c r="F5" s="16" t="s">
+      <c r="F6" s="16" t="s">
         <v>75</v>
       </c>
-      <c r="G5" s="16" t="s">
+      <c r="G6" s="16" t="s">
         <v>72</v>
       </c>
-      <c r="H5" s="16" t="s">
+      <c r="H6" s="16" t="s">
         <v>93</v>
       </c>
-      <c r="I5" s="16" t="s">
+      <c r="I6" s="16" t="s">
         <v>105</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="A6" s="17" t="s">
-        <v>166</v>
-      </c>
-      <c r="B6" s="9" t="s">
-        <v>170</v>
-      </c>
-      <c r="C6" s="17" t="s">
-        <v>278</v>
-      </c>
-      <c r="D6" s="17" t="s">
-        <v>272</v>
-      </c>
-      <c r="E6" s="16"/>
-      <c r="F6" s="16" t="s">
-        <v>275</v>
-      </c>
-      <c r="G6" s="16"/>
-      <c r="H6" s="16" t="s">
-        <v>274</v>
-      </c>
-      <c r="I6" s="16" t="s">
-        <v>273</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A7" s="17" t="s">
-        <v>129</v>
+        <v>166</v>
       </c>
       <c r="B7" s="9" t="s">
         <v>170</v>
       </c>
       <c r="C7" s="17" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="D7" s="17" t="s">
-        <v>53</v>
+        <v>272</v>
       </c>
       <c r="E7" s="16"/>
       <c r="F7" s="16" t="s">
-        <v>73</v>
+        <v>275</v>
       </c>
       <c r="G7" s="16"/>
       <c r="H7" s="16" t="s">
-        <v>73</v>
+        <v>274</v>
       </c>
       <c r="I7" s="16" t="s">
-        <v>71</v>
+        <v>273</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A8" s="17" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="B8" s="9" t="s">
         <v>170</v>
       </c>
       <c r="C8" s="17" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="D8" s="17" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E8" s="16"/>
       <c r="F8" s="16" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="G8" s="16"/>
       <c r="H8" s="16" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="I8" s="16" t="s">
-        <v>106</v>
+        <v>71</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A9" s="17" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="B9" s="9" t="s">
         <v>170</v>
       </c>
       <c r="C9" s="17" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="D9" s="17" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E9" s="16"/>
-      <c r="F9" s="16"/>
+      <c r="F9" s="16" t="s">
+        <v>76</v>
+      </c>
       <c r="G9" s="16"/>
-      <c r="H9" s="16"/>
+      <c r="H9" s="16" t="s">
+        <v>74</v>
+      </c>
       <c r="I9" s="16" t="s">
-        <v>70</v>
+        <v>106</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A10" s="17" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B10" s="9" t="s">
         <v>170</v>
       </c>
       <c r="C10" s="17" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="D10" s="17" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E10" s="16"/>
       <c r="F10" s="16"/>
       <c r="G10" s="16"/>
       <c r="H10" s="16"/>
       <c r="I10" s="16" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A11" s="17" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B11" s="9" t="s">
         <v>170</v>
       </c>
       <c r="C11" s="17" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="D11" s="17" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E11" s="16"/>
       <c r="F11" s="16"/>
       <c r="G11" s="16"/>
       <c r="H11" s="16"/>
       <c r="I11" s="16" t="s">
-        <v>107</v>
+        <v>71</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A12" s="17" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="B12" s="9" t="s">
         <v>170</v>
       </c>
       <c r="C12" s="17" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="D12" s="17" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E12" s="16"/>
-      <c r="F12" s="16">
-        <v>-2.9563999999999999</v>
-      </c>
+      <c r="F12" s="16"/>
       <c r="G12" s="16"/>
-      <c r="H12" s="16">
-        <v>1.5</v>
-      </c>
+      <c r="H12" s="16"/>
       <c r="I12" s="16" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A13" s="17" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="B13" s="9" t="s">
         <v>170</v>
       </c>
       <c r="C13" s="17" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="D13" s="17" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E13" s="16"/>
-      <c r="F13" s="16"/>
+      <c r="F13" s="16">
+        <v>-2.9563999999999999</v>
+      </c>
       <c r="G13" s="16"/>
-      <c r="H13" s="16"/>
-      <c r="I13" s="16"/>
+      <c r="H13" s="16">
+        <v>1.5</v>
+      </c>
+      <c r="I13" s="16" t="s">
+        <v>108</v>
+      </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A14" s="17" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="B14" s="9" t="s">
         <v>170</v>
       </c>
       <c r="C14" s="17" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="D14" s="17" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E14" s="16"/>
       <c r="F14" s="16"/>
@@ -3604,16 +3625,16 @@
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A15" s="17" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="B15" s="9" t="s">
         <v>170</v>
       </c>
       <c r="C15" s="17" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="D15" s="17" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E15" s="16"/>
       <c r="F15" s="16"/>
@@ -3623,16 +3644,16 @@
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A16" s="17" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="B16" s="9" t="s">
         <v>170</v>
       </c>
       <c r="C16" s="17" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="D16" s="17" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E16" s="16"/>
       <c r="F16" s="16"/>
@@ -3642,81 +3663,81 @@
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A17" s="17" t="s">
+        <v>130</v>
+      </c>
+      <c r="B17" s="9" t="s">
+        <v>170</v>
+      </c>
+      <c r="C17" s="17" t="s">
+        <v>284</v>
+      </c>
+      <c r="D17" s="17" t="s">
+        <v>62</v>
+      </c>
+      <c r="E17" s="16"/>
+      <c r="F17" s="16"/>
+      <c r="G17" s="16"/>
+      <c r="H17" s="16"/>
+      <c r="I17" s="16"/>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A18" s="17" t="s">
         <v>129</v>
       </c>
-      <c r="B17" s="9" t="s">
-        <v>170</v>
-      </c>
-      <c r="C17" s="17" t="s">
+      <c r="B18" s="9" t="s">
+        <v>170</v>
+      </c>
+      <c r="C18" s="17" t="s">
         <v>279</v>
       </c>
-      <c r="D17" s="17" t="s">
+      <c r="D18" s="17" t="s">
         <v>63</v>
-      </c>
-      <c r="E17" s="16"/>
-      <c r="F17" s="16" t="s">
-        <v>73</v>
-      </c>
-      <c r="G17" s="16"/>
-      <c r="H17" s="16" t="s">
-        <v>69</v>
-      </c>
-      <c r="I17" s="16"/>
-    </row>
-    <row r="18" spans="1:9" ht="22" x14ac:dyDescent="0.15">
-      <c r="A18" s="17" t="s">
-        <v>128</v>
-      </c>
-      <c r="B18" s="9" t="s">
-        <v>170</v>
-      </c>
-      <c r="C18" s="17" t="s">
-        <v>280</v>
-      </c>
-      <c r="D18" s="17" t="s">
-        <v>64</v>
       </c>
       <c r="E18" s="16"/>
       <c r="F18" s="16" t="s">
-        <v>91</v>
+        <v>73</v>
       </c>
       <c r="G18" s="16"/>
       <c r="H18" s="16" t="s">
+        <v>69</v>
+      </c>
+      <c r="I18" s="16"/>
+    </row>
+    <row r="19" spans="1:9" ht="22" x14ac:dyDescent="0.15">
+      <c r="A19" s="17" t="s">
+        <v>128</v>
+      </c>
+      <c r="B19" s="9" t="s">
+        <v>170</v>
+      </c>
+      <c r="C19" s="17" t="s">
+        <v>280</v>
+      </c>
+      <c r="D19" s="17" t="s">
+        <v>64</v>
+      </c>
+      <c r="E19" s="16"/>
+      <c r="F19" s="16" t="s">
+        <v>91</v>
+      </c>
+      <c r="G19" s="16"/>
+      <c r="H19" s="16" t="s">
         <v>94</v>
       </c>
-      <c r="I18" s="16"/>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="A19" s="9" t="s">
-        <v>131</v>
-      </c>
-      <c r="B19" s="9" t="s">
-        <v>170</v>
-      </c>
-      <c r="C19" s="17" t="s">
-        <v>281</v>
-      </c>
-      <c r="D19" s="17" t="s">
-        <v>65</v>
-      </c>
-      <c r="E19" s="16"/>
-      <c r="F19" s="16"/>
-      <c r="G19" s="16"/>
-      <c r="H19" s="16"/>
       <c r="I19" s="16"/>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A20" s="9" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B20" s="9" t="s">
         <v>170</v>
       </c>
       <c r="C20" s="17" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="D20" s="17" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E20" s="16"/>
       <c r="F20" s="16"/>
@@ -3726,16 +3747,16 @@
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A21" s="9" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B21" s="9" t="s">
         <v>170</v>
       </c>
       <c r="C21" s="17" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="D21" s="17" t="s">
-        <v>86</v>
+        <v>66</v>
       </c>
       <c r="E21" s="16"/>
       <c r="F21" s="16"/>
@@ -3745,58 +3766,58 @@
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A22" s="9" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="B22" s="9" t="s">
         <v>170</v>
       </c>
       <c r="C22" s="17" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="D22" s="17" t="s">
-        <v>67</v>
+        <v>86</v>
       </c>
       <c r="E22" s="16"/>
-      <c r="F22" s="16">
-        <v>4.3803999999999998</v>
-      </c>
+      <c r="F22" s="16"/>
       <c r="G22" s="16"/>
-      <c r="H22" s="16">
-        <v>3</v>
-      </c>
+      <c r="H22" s="16"/>
       <c r="I22" s="16"/>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A23" s="9" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="B23" s="9" t="s">
         <v>170</v>
       </c>
       <c r="C23" s="17" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="D23" s="17" t="s">
-        <v>77</v>
+        <v>67</v>
       </c>
       <c r="E23" s="16"/>
-      <c r="F23" s="16"/>
+      <c r="F23" s="16">
+        <v>4.3803999999999998</v>
+      </c>
       <c r="G23" s="16"/>
-      <c r="H23" s="16"/>
+      <c r="H23" s="16">
+        <v>3</v>
+      </c>
       <c r="I23" s="16"/>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A24" s="9" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="B24" s="9" t="s">
         <v>170</v>
       </c>
       <c r="C24" s="17" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="D24" s="17" t="s">
-        <v>68</v>
+        <v>77</v>
       </c>
       <c r="E24" s="16"/>
       <c r="F24" s="16"/>
@@ -3806,16 +3827,16 @@
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A25" s="9" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="B25" s="9" t="s">
         <v>170</v>
       </c>
       <c r="C25" s="17" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="D25" s="17" t="s">
-        <v>78</v>
+        <v>68</v>
       </c>
       <c r="E25" s="16"/>
       <c r="F25" s="16"/>
@@ -3825,16 +3846,16 @@
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A26" s="9" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="B26" s="9" t="s">
         <v>170</v>
       </c>
       <c r="C26" s="17" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="D26" s="17" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E26" s="16"/>
       <c r="F26" s="16"/>
@@ -3844,81 +3865,81 @@
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A27" s="9" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="B27" s="9" t="s">
         <v>170</v>
       </c>
       <c r="C27" s="17" t="s">
-        <v>279</v>
+        <v>284</v>
       </c>
       <c r="D27" s="17" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E27" s="16"/>
-      <c r="F27" s="16" t="s">
-        <v>73</v>
-      </c>
+      <c r="F27" s="16"/>
       <c r="G27" s="16"/>
-      <c r="H27" s="16" t="s">
-        <v>73</v>
-      </c>
+      <c r="H27" s="16"/>
       <c r="I27" s="16"/>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A28" s="9" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="B28" s="9" t="s">
         <v>170</v>
       </c>
       <c r="C28" s="17" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="D28" s="17" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E28" s="16"/>
       <c r="F28" s="16" t="s">
-        <v>92</v>
+        <v>73</v>
       </c>
       <c r="G28" s="16"/>
       <c r="H28" s="16" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="I28" s="16"/>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A29" s="9" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="B29" s="9" t="s">
         <v>170</v>
       </c>
       <c r="C29" s="17" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="D29" s="17" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E29" s="16"/>
-      <c r="F29" s="16"/>
+      <c r="F29" s="16" t="s">
+        <v>92</v>
+      </c>
       <c r="G29" s="16"/>
-      <c r="H29" s="16"/>
+      <c r="H29" s="16" t="s">
+        <v>76</v>
+      </c>
       <c r="I29" s="16"/>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A30" s="9" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B30" s="9" t="s">
         <v>170</v>
       </c>
       <c r="C30" s="17" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="D30" s="17" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E30" s="16"/>
       <c r="F30" s="16"/>
@@ -3928,16 +3949,16 @@
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A31" s="9" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B31" s="9" t="s">
         <v>170</v>
       </c>
       <c r="C31" s="17" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="D31" s="17" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="E31" s="16"/>
       <c r="F31" s="16"/>
@@ -3947,58 +3968,58 @@
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A32" s="9" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="B32" s="9" t="s">
         <v>170</v>
       </c>
       <c r="C32" s="17" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="D32" s="17" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="E32" s="16"/>
-      <c r="F32" s="16">
-        <v>2.5</v>
-      </c>
+      <c r="F32" s="16"/>
       <c r="G32" s="16"/>
-      <c r="H32" s="16">
-        <v>-2.9563999999999999</v>
-      </c>
+      <c r="H32" s="16"/>
       <c r="I32" s="16"/>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A33" s="9" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="B33" s="9" t="s">
         <v>170</v>
       </c>
       <c r="C33" s="17" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="D33" s="17" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="E33" s="16"/>
-      <c r="F33" s="16"/>
+      <c r="F33" s="16">
+        <v>2.5</v>
+      </c>
       <c r="G33" s="16"/>
-      <c r="H33" s="16"/>
+      <c r="H33" s="16">
+        <v>-2.9563999999999999</v>
+      </c>
       <c r="I33" s="16"/>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A34" s="9" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="B34" s="9" t="s">
         <v>170</v>
       </c>
       <c r="C34" s="17" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="D34" s="17" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="E34" s="16"/>
       <c r="F34" s="16"/>
@@ -4008,16 +4029,16 @@
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A35" s="9" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="B35" s="9" t="s">
         <v>170</v>
       </c>
       <c r="C35" s="17" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="D35" s="17" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="E35" s="16"/>
       <c r="F35" s="16"/>
@@ -4027,16 +4048,16 @@
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A36" s="9" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="B36" s="9" t="s">
         <v>170</v>
       </c>
       <c r="C36" s="17" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="D36" s="17" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="E36" s="16"/>
       <c r="F36" s="16"/>
@@ -4046,77 +4067,77 @@
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A37" s="9" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="B37" s="9" t="s">
         <v>170</v>
       </c>
       <c r="C37" s="17" t="s">
-        <v>279</v>
+        <v>284</v>
       </c>
       <c r="D37" s="17" t="s">
-        <v>95</v>
+        <v>85</v>
       </c>
       <c r="E37" s="16"/>
       <c r="F37" s="16"/>
       <c r="G37" s="16"/>
-      <c r="H37" s="16" t="s">
-        <v>73</v>
-      </c>
+      <c r="H37" s="16"/>
       <c r="I37" s="16"/>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A38" s="9" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="B38" s="9" t="s">
         <v>170</v>
       </c>
       <c r="C38" s="17" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="D38" s="17" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E38" s="16"/>
       <c r="F38" s="16"/>
       <c r="G38" s="16"/>
       <c r="H38" s="16" t="s">
-        <v>91</v>
+        <v>73</v>
       </c>
       <c r="I38" s="16"/>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A39" s="9" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="B39" s="9" t="s">
         <v>170</v>
       </c>
       <c r="C39" s="17" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="D39" s="17" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E39" s="16"/>
       <c r="F39" s="16"/>
       <c r="G39" s="16"/>
-      <c r="H39" s="16"/>
+      <c r="H39" s="16" t="s">
+        <v>91</v>
+      </c>
       <c r="I39" s="16"/>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A40" s="9" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B40" s="9" t="s">
         <v>170</v>
       </c>
       <c r="C40" s="17" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="D40" s="17" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E40" s="16"/>
       <c r="F40" s="16"/>
@@ -4126,16 +4147,16 @@
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A41" s="9" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B41" s="9" t="s">
         <v>170</v>
       </c>
       <c r="C41" s="17" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="D41" s="17" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E41" s="16"/>
       <c r="F41" s="16"/>
@@ -4145,56 +4166,56 @@
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A42" s="9" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="B42" s="9" t="s">
         <v>170</v>
       </c>
       <c r="C42" s="17" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="D42" s="17" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="E42" s="16"/>
       <c r="F42" s="16"/>
       <c r="G42" s="16"/>
-      <c r="H42" s="16">
-        <v>4.3803999999999998</v>
-      </c>
+      <c r="H42" s="16"/>
       <c r="I42" s="16"/>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A43" s="9" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="B43" s="9" t="s">
         <v>170</v>
       </c>
       <c r="C43" s="17" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="D43" s="17" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E43" s="16"/>
       <c r="F43" s="16"/>
       <c r="G43" s="16"/>
-      <c r="H43" s="16"/>
+      <c r="H43" s="16">
+        <v>4.3803999999999998</v>
+      </c>
       <c r="I43" s="16"/>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A44" s="9" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="B44" s="9" t="s">
         <v>170</v>
       </c>
       <c r="C44" s="17" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="D44" s="17" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E44" s="16"/>
       <c r="F44" s="16"/>
@@ -4204,16 +4225,16 @@
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A45" s="9" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="B45" s="9" t="s">
         <v>170</v>
       </c>
       <c r="C45" s="17" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="D45" s="17" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E45" s="16"/>
       <c r="F45" s="16"/>
@@ -4223,16 +4244,16 @@
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A46" s="9" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="B46" s="9" t="s">
         <v>170</v>
       </c>
       <c r="C46" s="17" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="D46" s="17" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E46" s="16"/>
       <c r="F46" s="16"/>
@@ -4240,16 +4261,35 @@
       <c r="H46" s="16"/>
       <c r="I46" s="16"/>
     </row>
-    <row r="48" spans="1:9" ht="12" thickBot="1" x14ac:dyDescent="0.2"/>
-    <row r="49" spans="1:1" ht="59" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="22" t="s">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A47" s="9" t="s">
+        <v>130</v>
+      </c>
+      <c r="B47" s="9" t="s">
+        <v>170</v>
+      </c>
+      <c r="C47" s="17" t="s">
+        <v>284</v>
+      </c>
+      <c r="D47" s="17" t="s">
+        <v>104</v>
+      </c>
+      <c r="E47" s="16"/>
+      <c r="F47" s="16"/>
+      <c r="G47" s="16"/>
+      <c r="H47" s="16"/>
+      <c r="I47" s="16"/>
+    </row>
+    <row r="49" spans="1:1" ht="12" thickBot="1" x14ac:dyDescent="0.2"/>
+    <row r="50" spans="1:1" ht="59" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A50" s="22" t="s">
         <v>305</v>
       </c>
     </row>
   </sheetData>
-  <sortState columnSort="1" ref="E1:I49">
+  <sortState columnSort="1" ref="E1:I50">
     <sortCondition ref="E3:I3"/>
-    <sortCondition ref="E4:I4"/>
+    <sortCondition ref="E5:I5"/>
   </sortState>
   <mergeCells count="3">
     <mergeCell ref="A1:B1"/>
@@ -4359,11 +4399,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F13"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="4" ySplit="2" topLeftCell="E3" activePane="bottomRight" state="frozenSplit"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="E4" sqref="E4:F4"/>
+      <selection pane="bottomRight" activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="38.1640625" defaultRowHeight="11" x14ac:dyDescent="0.15"/>

</xml_diff>

<commit_message>
adjusted test input spreadsheet scoring info
Changed scoring rule name from "SBACAttemptedness" to "SBACIABAttemptedness"
Changed scoring rule measure from empty string to "Attempted"
</commit_message>
<xml_diff>
--- a/src/test/resources/SBAC-IAB-FIXED-G11M-Winter-2017-2018.xlsx
+++ b/src/test/resources/SBAC-IAB-FIXED-G11M-Winter-2017-2018.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10116"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10709"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/emunoz/trunk/sbrepo/repositories/TDS_FixedFormPackager/src/test/resources/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/miketrupkin/tds-project/fixed-form-packager/TDS_FixedFormPackager/src/test/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FCA0E8D-E6AD-D244-A001-0E75846BF330}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4800" yWindow="440" windowWidth="28800" windowHeight="16640" tabRatio="644" activeTab="5"/>
+    <workbookView xWindow="4800" yWindow="440" windowWidth="28800" windowHeight="16640" tabRatio="644" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Package" sheetId="16" r:id="rId1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1630" uniqueCount="590">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1631" uniqueCount="591">
   <si>
     <t>ItemId</t>
   </si>
@@ -597,9 +598,6 @@
   </si>
   <si>
     <t>MATH</t>
-  </si>
-  <si>
-    <t>SBACAttemptedness</t>
   </si>
   <si>
     <t>Input Description</t>
@@ -1851,11 +1849,17 @@
   <si>
     <t>test</t>
   </si>
+  <si>
+    <t>SBACIABAttemptedness</t>
+  </si>
+  <si>
+    <t>Attempted</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.000000E+00"/>
     <numFmt numFmtId="165" formatCode="0.0"/>
@@ -2960,7 +2964,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2986,11 +2990,11 @@
       </c>
       <c r="B1" s="25"/>
       <c r="C1" s="25" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="D1" s="25"/>
       <c r="E1" s="7" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.15">
@@ -3001,10 +3005,10 @@
         <v>186</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="E2" s="7" t="s">
         <v>187</v>
@@ -3018,13 +3022,13 @@
         <v>109</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="D3" s="9" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -3035,7 +3039,7 @@
         <v>109</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D4" s="9" t="s">
         <v>167</v>
@@ -3052,7 +3056,7 @@
         <v>109</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="D5" s="9" t="s">
         <v>168</v>
@@ -3069,7 +3073,7 @@
         <v>109</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D6" s="9" t="s">
         <v>183</v>
@@ -3086,7 +3090,7 @@
         <v>109</v>
       </c>
       <c r="C7" s="9" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="D7" s="9" t="s">
         <v>39</v>
@@ -3103,7 +3107,7 @@
         <v>109</v>
       </c>
       <c r="C8" s="9" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="D8" s="9" t="s">
         <v>40</v>
@@ -3120,7 +3124,7 @@
         <v>109</v>
       </c>
       <c r="C9" s="9" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="D9" s="9" t="s">
         <v>41</v>
@@ -3137,7 +3141,7 @@
         <v>109</v>
       </c>
       <c r="C10" s="9" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="D10" s="9" t="s">
         <v>42</v>
@@ -3154,13 +3158,13 @@
         <v>110</v>
       </c>
       <c r="C11" s="9" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="D11" s="9" t="s">
         <v>43</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.15">
@@ -3171,7 +3175,7 @@
         <v>109</v>
       </c>
       <c r="C12" s="9" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D12" s="9" t="s">
         <v>44</v>
@@ -3188,7 +3192,7 @@
         <v>109</v>
       </c>
       <c r="C13" s="9" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D13" s="9" t="s">
         <v>45</v>
@@ -3205,7 +3209,7 @@
         <v>109</v>
       </c>
       <c r="C14" s="9" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="D14" s="9" t="s">
         <v>46</v>
@@ -3222,7 +3226,7 @@
         <v>109</v>
       </c>
       <c r="C15" s="9" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="D15" s="9" t="s">
         <v>47</v>
@@ -3239,7 +3243,7 @@
         <v>109</v>
       </c>
       <c r="C16" s="9" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="D16" s="9" t="s">
         <v>48</v>
@@ -3258,14 +3262,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:I50"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="4" ySplit="2" topLeftCell="E3" activePane="bottomRight" state="frozenSplit"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="E3" sqref="E3"/>
+      <selection pane="bottomRight" activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="55" defaultRowHeight="11" x14ac:dyDescent="0.15"/>
@@ -3284,7 +3288,7 @@
       </c>
       <c r="B1" s="25"/>
       <c r="C1" s="25" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="D1" s="25"/>
       <c r="E1" s="26"/>
@@ -3301,10 +3305,10 @@
         <v>186</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="E2" s="20" t="s">
         <v>187</v>
@@ -3330,54 +3334,54 @@
         <v>109</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="D3" s="9" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A4" s="17" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
       <c r="B4" s="9" t="s">
         <v>109</v>
       </c>
       <c r="C4" s="17" t="s">
+        <v>586</v>
+      </c>
+      <c r="D4" s="9" t="s">
         <v>587</v>
       </c>
-      <c r="D4" s="9" t="s">
+      <c r="E4" s="1" t="s">
         <v>588</v>
       </c>
-      <c r="E4" s="1" t="s">
-        <v>589</v>
-      </c>
       <c r="F4" s="1" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.15">
@@ -3388,7 +3392,7 @@
         <v>109</v>
       </c>
       <c r="C5" s="17" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="D5" s="17" t="s">
         <v>52</v>
@@ -3417,13 +3421,13 @@
         <v>109</v>
       </c>
       <c r="C6" s="17" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="D6" s="17" t="s">
         <v>51</v>
       </c>
       <c r="E6" s="16" t="s">
-        <v>191</v>
+        <v>589</v>
       </c>
       <c r="F6" s="16" t="s">
         <v>75</v>
@@ -3446,21 +3450,23 @@
         <v>170</v>
       </c>
       <c r="C7" s="17" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="D7" s="17" t="s">
-        <v>272</v>
-      </c>
-      <c r="E7" s="16"/>
+        <v>271</v>
+      </c>
+      <c r="E7" s="16" t="s">
+        <v>590</v>
+      </c>
       <c r="F7" s="16" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="G7" s="16"/>
       <c r="H7" s="16" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="I7" s="16" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.15">
@@ -3471,7 +3477,7 @@
         <v>170</v>
       </c>
       <c r="C8" s="17" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="D8" s="17" t="s">
         <v>53</v>
@@ -3496,7 +3502,7 @@
         <v>170</v>
       </c>
       <c r="C9" s="17" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="D9" s="17" t="s">
         <v>54</v>
@@ -3521,7 +3527,7 @@
         <v>170</v>
       </c>
       <c r="C10" s="17" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="D10" s="17" t="s">
         <v>55</v>
@@ -3542,7 +3548,7 @@
         <v>170</v>
       </c>
       <c r="C11" s="17" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="D11" s="17" t="s">
         <v>56</v>
@@ -3563,7 +3569,7 @@
         <v>170</v>
       </c>
       <c r="C12" s="17" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="D12" s="17" t="s">
         <v>57</v>
@@ -3584,7 +3590,7 @@
         <v>170</v>
       </c>
       <c r="C13" s="17" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="D13" s="17" t="s">
         <v>58</v>
@@ -3609,7 +3615,7 @@
         <v>170</v>
       </c>
       <c r="C14" s="17" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="D14" s="17" t="s">
         <v>59</v>
@@ -3628,7 +3634,7 @@
         <v>170</v>
       </c>
       <c r="C15" s="17" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="D15" s="17" t="s">
         <v>60</v>
@@ -3647,7 +3653,7 @@
         <v>170</v>
       </c>
       <c r="C16" s="17" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="D16" s="17" t="s">
         <v>61</v>
@@ -3666,7 +3672,7 @@
         <v>170</v>
       </c>
       <c r="C17" s="17" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="D17" s="17" t="s">
         <v>62</v>
@@ -3685,7 +3691,7 @@
         <v>170</v>
       </c>
       <c r="C18" s="17" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="D18" s="17" t="s">
         <v>63</v>
@@ -3708,7 +3714,7 @@
         <v>170</v>
       </c>
       <c r="C19" s="17" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="D19" s="17" t="s">
         <v>64</v>
@@ -3731,7 +3737,7 @@
         <v>170</v>
       </c>
       <c r="C20" s="17" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="D20" s="17" t="s">
         <v>65</v>
@@ -3750,7 +3756,7 @@
         <v>170</v>
       </c>
       <c r="C21" s="17" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="D21" s="17" t="s">
         <v>66</v>
@@ -3769,7 +3775,7 @@
         <v>170</v>
       </c>
       <c r="C22" s="17" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="D22" s="17" t="s">
         <v>86</v>
@@ -3788,7 +3794,7 @@
         <v>170</v>
       </c>
       <c r="C23" s="17" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="D23" s="17" t="s">
         <v>67</v>
@@ -3811,7 +3817,7 @@
         <v>170</v>
       </c>
       <c r="C24" s="17" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="D24" s="17" t="s">
         <v>77</v>
@@ -3830,7 +3836,7 @@
         <v>170</v>
       </c>
       <c r="C25" s="17" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="D25" s="17" t="s">
         <v>68</v>
@@ -3849,7 +3855,7 @@
         <v>170</v>
       </c>
       <c r="C26" s="17" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="D26" s="17" t="s">
         <v>78</v>
@@ -3868,7 +3874,7 @@
         <v>170</v>
       </c>
       <c r="C27" s="17" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="D27" s="17" t="s">
         <v>79</v>
@@ -3887,7 +3893,7 @@
         <v>170</v>
       </c>
       <c r="C28" s="17" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="D28" s="17" t="s">
         <v>80</v>
@@ -3910,7 +3916,7 @@
         <v>170</v>
       </c>
       <c r="C29" s="17" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="D29" s="17" t="s">
         <v>81</v>
@@ -3933,7 +3939,7 @@
         <v>170</v>
       </c>
       <c r="C30" s="17" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="D30" s="17" t="s">
         <v>82</v>
@@ -3952,7 +3958,7 @@
         <v>170</v>
       </c>
       <c r="C31" s="17" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="D31" s="17" t="s">
         <v>83</v>
@@ -3971,7 +3977,7 @@
         <v>170</v>
       </c>
       <c r="C32" s="17" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="D32" s="17" t="s">
         <v>87</v>
@@ -3990,7 +3996,7 @@
         <v>170</v>
       </c>
       <c r="C33" s="17" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="D33" s="17" t="s">
         <v>84</v>
@@ -4013,7 +4019,7 @@
         <v>170</v>
       </c>
       <c r="C34" s="17" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="D34" s="17" t="s">
         <v>89</v>
@@ -4032,7 +4038,7 @@
         <v>170</v>
       </c>
       <c r="C35" s="17" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="D35" s="17" t="s">
         <v>88</v>
@@ -4051,7 +4057,7 @@
         <v>170</v>
       </c>
       <c r="C36" s="17" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="D36" s="17" t="s">
         <v>90</v>
@@ -4070,7 +4076,7 @@
         <v>170</v>
       </c>
       <c r="C37" s="17" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="D37" s="17" t="s">
         <v>85</v>
@@ -4089,7 +4095,7 @@
         <v>170</v>
       </c>
       <c r="C38" s="17" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="D38" s="17" t="s">
         <v>95</v>
@@ -4110,7 +4116,7 @@
         <v>170</v>
       </c>
       <c r="C39" s="17" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="D39" s="17" t="s">
         <v>96</v>
@@ -4131,7 +4137,7 @@
         <v>170</v>
       </c>
       <c r="C40" s="17" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="D40" s="17" t="s">
         <v>97</v>
@@ -4150,7 +4156,7 @@
         <v>170</v>
       </c>
       <c r="C41" s="17" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="D41" s="17" t="s">
         <v>98</v>
@@ -4169,7 +4175,7 @@
         <v>170</v>
       </c>
       <c r="C42" s="17" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="D42" s="17" t="s">
         <v>99</v>
@@ -4188,7 +4194,7 @@
         <v>170</v>
       </c>
       <c r="C43" s="17" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="D43" s="17" t="s">
         <v>100</v>
@@ -4209,7 +4215,7 @@
         <v>170</v>
       </c>
       <c r="C44" s="17" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="D44" s="17" t="s">
         <v>101</v>
@@ -4228,7 +4234,7 @@
         <v>170</v>
       </c>
       <c r="C45" s="17" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="D45" s="17" t="s">
         <v>102</v>
@@ -4247,7 +4253,7 @@
         <v>170</v>
       </c>
       <c r="C46" s="17" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="D46" s="17" t="s">
         <v>103</v>
@@ -4266,7 +4272,7 @@
         <v>170</v>
       </c>
       <c r="C47" s="17" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="D47" s="17" t="s">
         <v>104</v>
@@ -4280,7 +4286,7 @@
     <row r="49" spans="1:1" ht="12" thickBot="1" x14ac:dyDescent="0.2"/>
     <row r="50" spans="1:1" ht="59" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A50" s="22" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
   </sheetData>
@@ -4299,7 +4305,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
@@ -4325,11 +4331,11 @@
       </c>
       <c r="B1" s="25"/>
       <c r="C1" s="25" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="D1" s="25"/>
       <c r="E1" s="19" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.15">
@@ -4340,10 +4346,10 @@
         <v>186</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="E2" s="7" t="s">
         <v>187</v>
@@ -4357,13 +4363,13 @@
         <v>109</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="D3" s="9" t="s">
         <v>182</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.15">
@@ -4374,13 +4380,13 @@
         <v>109</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="D4" s="9" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
     </row>
   </sheetData>
@@ -4394,7 +4400,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
@@ -4421,11 +4427,11 @@
       </c>
       <c r="B1" s="25"/>
       <c r="C1" s="25" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="D1" s="25"/>
       <c r="E1" s="25" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="F1" s="25"/>
     </row>
@@ -4437,10 +4443,10 @@
         <v>186</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="E2" s="7" t="s">
         <v>187</v>
@@ -4457,16 +4463,16 @@
         <v>109</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="D3" s="9" t="s">
         <v>1</v>
       </c>
       <c r="E3" s="3" t="s">
+        <v>298</v>
+      </c>
+      <c r="F3" s="3" t="s">
         <v>299</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>300</v>
       </c>
     </row>
     <row r="4" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.15">
@@ -4477,16 +4483,16 @@
         <v>109</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="D4" s="9" t="s">
         <v>182</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="5" spans="1:6" s="2" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -4497,7 +4503,7 @@
         <v>109</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="D5" s="9" t="s">
         <v>2</v>
@@ -4517,16 +4523,16 @@
         <v>170</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="D6" s="9" t="s">
         <v>179</v>
       </c>
       <c r="E6" s="3" t="s">
+        <v>298</v>
+      </c>
+      <c r="F6" s="3" t="s">
         <v>299</v>
-      </c>
-      <c r="F6" s="3" t="s">
-        <v>300</v>
       </c>
     </row>
     <row r="7" spans="1:6" s="2" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -4537,7 +4543,7 @@
         <v>170</v>
       </c>
       <c r="C7" s="9" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="D7" s="9" t="s">
         <v>180</v>
@@ -4557,7 +4563,7 @@
         <v>170</v>
       </c>
       <c r="C8" s="9" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="D8" s="9" t="s">
         <v>181</v>
@@ -4577,10 +4583,10 @@
         <v>109</v>
       </c>
       <c r="C9" s="9" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="D9" s="9" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="E9" s="3" t="b">
         <v>1</v>
@@ -4597,10 +4603,10 @@
         <v>170</v>
       </c>
       <c r="C10" s="9" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="D10" s="9" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="E10" s="3" t="b">
         <v>1</v>
@@ -4617,10 +4623,10 @@
         <v>170</v>
       </c>
       <c r="C11" s="9" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="D11" s="9" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="E11" s="3" t="b">
         <v>1</v>
@@ -4637,7 +4643,7 @@
         <v>109</v>
       </c>
       <c r="C12" s="9" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="D12" s="9" t="s">
         <v>189</v>
@@ -4657,10 +4663,10 @@
         <v>109</v>
       </c>
       <c r="C13" s="9" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="D13" s="9" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="E13" s="8">
         <v>2514.9</v>
@@ -4681,7 +4687,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:S56"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
@@ -4707,16 +4713,16 @@
       </c>
       <c r="B1" s="25"/>
       <c r="C1" s="25" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="D1" s="25"/>
       <c r="E1" s="27" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="F1" s="28"/>
       <c r="G1" s="29"/>
       <c r="H1" s="30" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="I1" s="31"/>
       <c r="J1" s="31"/>
@@ -4738,10 +4744,10 @@
         <v>186</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="E2" s="10" t="s">
         <v>187</v>
@@ -4797,173 +4803,173 @@
         <v>109</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="D3" s="9" t="s">
         <v>1</v>
       </c>
       <c r="E3" s="3" t="s">
+        <v>298</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>298</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>298</v>
+      </c>
+      <c r="H3" s="3" t="s">
         <v>299</v>
       </c>
-      <c r="F3" s="3" t="s">
+      <c r="I3" s="3" t="s">
         <v>299</v>
       </c>
-      <c r="G3" s="3" t="s">
+      <c r="J3" s="3" t="s">
         <v>299</v>
       </c>
-      <c r="H3" s="3" t="s">
-        <v>300</v>
-      </c>
-      <c r="I3" s="3" t="s">
-        <v>300</v>
-      </c>
-      <c r="J3" s="3" t="s">
-        <v>300</v>
-      </c>
       <c r="K3" s="3" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="L3" s="3" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="M3" s="3" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="N3" s="3" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="O3" s="3" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="P3" s="3" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="Q3" s="3" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="R3" s="3" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="S3" s="3" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
     </row>
     <row r="4" spans="1:19" ht="22" x14ac:dyDescent="0.15">
       <c r="A4" s="9" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="B4" s="9" t="s">
         <v>109</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="D4" s="9" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="E4" s="3" t="s">
+        <v>298</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>298</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>298</v>
+      </c>
+      <c r="H4" s="3" t="s">
         <v>299</v>
       </c>
-      <c r="F4" s="3" t="s">
+      <c r="I4" s="3" t="s">
         <v>299</v>
       </c>
-      <c r="G4" s="3" t="s">
+      <c r="J4" s="3" t="s">
         <v>299</v>
       </c>
-      <c r="H4" s="3" t="s">
-        <v>300</v>
-      </c>
-      <c r="I4" s="3" t="s">
-        <v>300</v>
-      </c>
-      <c r="J4" s="3" t="s">
-        <v>300</v>
-      </c>
       <c r="K4" s="3" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="L4" s="3" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="M4" s="3" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="N4" s="3" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="O4" s="3" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="P4" s="3" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="Q4" s="3" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="R4" s="3" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="S4" s="3" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A5" s="9" t="s">
+        <v>250</v>
+      </c>
+      <c r="B5" s="9" t="s">
+        <v>170</v>
+      </c>
+      <c r="C5" s="9" t="s">
+        <v>294</v>
+      </c>
+      <c r="D5" s="9" t="s">
         <v>251</v>
       </c>
-      <c r="B5" s="9" t="s">
-        <v>170</v>
-      </c>
-      <c r="C5" s="9" t="s">
-        <v>295</v>
-      </c>
-      <c r="D5" s="9" t="s">
+      <c r="E5" s="12" t="s">
         <v>252</v>
       </c>
-      <c r="E5" s="12" t="s">
-        <v>253</v>
-      </c>
       <c r="F5" s="12" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="G5" s="12" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="H5" s="12" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="I5" s="12" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="J5" s="12" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="K5" s="12" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="L5" s="12" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="M5" s="12" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="N5" s="12" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="O5" s="12" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="P5" s="12" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="Q5" s="12" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="R5" s="12" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="S5" s="12" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.15">
@@ -4972,10 +4978,10 @@
         <v>109</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="D6" s="9" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="E6" s="5">
         <v>1</v>
@@ -5031,10 +5037,10 @@
         <v>109</v>
       </c>
       <c r="C7" s="9" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="D7" s="9" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="E7" s="5">
         <v>1</v>
@@ -5090,7 +5096,7 @@
         <v>109</v>
       </c>
       <c r="C8" s="9" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="D8" s="9" t="s">
         <v>0</v>
@@ -5143,16 +5149,16 @@
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A9" s="9" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="B9" s="9" t="s">
         <v>109</v>
       </c>
       <c r="C9" s="9" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="D9" s="9" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="E9" s="1" t="b">
         <v>1</v>
@@ -5202,16 +5208,16 @@
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A10" s="9" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="B10" s="9" t="s">
         <v>170</v>
       </c>
       <c r="C10" s="9" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="D10" s="9" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E10" s="1" t="b">
         <v>1</v>
@@ -5261,16 +5267,16 @@
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A11" s="9" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="B11" s="9" t="s">
         <v>170</v>
       </c>
       <c r="C11" s="9" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="D11" s="9" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="E11" s="1" t="b">
         <v>1</v>
@@ -5320,16 +5326,16 @@
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A12" s="9" t="s">
+        <v>547</v>
+      </c>
+      <c r="B12" s="9" t="s">
+        <v>170</v>
+      </c>
+      <c r="C12" s="9" t="s">
+        <v>549</v>
+      </c>
+      <c r="D12" s="9" t="s">
         <v>548</v>
-      </c>
-      <c r="B12" s="9" t="s">
-        <v>170</v>
-      </c>
-      <c r="C12" s="9" t="s">
-        <v>550</v>
-      </c>
-      <c r="D12" s="9" t="s">
-        <v>549</v>
       </c>
       <c r="E12" s="1"/>
       <c r="F12" s="1"/>
@@ -5355,7 +5361,7 @@
         <v>170</v>
       </c>
       <c r="C13" s="9" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="D13" s="9" t="s">
         <v>171</v>
@@ -6550,10 +6556,10 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:I230"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <pane xSplit="4" ySplit="2" topLeftCell="E12" activePane="bottomRight" state="frozenSplit"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
@@ -6577,17 +6583,17 @@
       </c>
       <c r="B1" s="25"/>
       <c r="C1" s="25" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="D1" s="25"/>
       <c r="E1" s="13" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="F1" s="13" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="G1" s="13" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.15">
@@ -6598,10 +6604,10 @@
         <v>186</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="E2" s="7" t="s">
         <v>187</v>
@@ -6621,19 +6627,19 @@
         <v>109</v>
       </c>
       <c r="C3" s="9" t="s">
+        <v>289</v>
+      </c>
+      <c r="D3" s="9" t="s">
         <v>290</v>
       </c>
-      <c r="D3" s="9" t="s">
-        <v>291</v>
-      </c>
       <c r="E3" s="1" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="F3" s="3" t="s">
+        <v>298</v>
+      </c>
+      <c r="G3" s="3" t="s">
         <v>299</v>
-      </c>
-      <c r="G3" s="3" t="s">
-        <v>300</v>
       </c>
     </row>
     <row r="4" spans="1:9" s="2" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -6644,17 +6650,17 @@
         <v>109</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="D4" s="9" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="F4" s="3"/>
       <c r="G4" s="3" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="5" spans="1:9" s="2" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -6665,10 +6671,10 @@
         <v>170</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="D5" s="9" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="E5" s="3"/>
       <c r="F5" s="3"/>
@@ -6682,10 +6688,10 @@
         <v>170</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="D6" s="9" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="E6" s="3"/>
       <c r="F6" s="3"/>
@@ -6699,10 +6705,10 @@
         <v>170</v>
       </c>
       <c r="C7" s="9" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="D7" s="9" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="E7" s="3"/>
       <c r="F7" s="3"/>
@@ -6718,10 +6724,10 @@
         <v>170</v>
       </c>
       <c r="C8" s="9" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="D8" s="9" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="E8" s="3" t="b">
         <v>1</v>
@@ -6739,10 +6745,10 @@
         <v>170</v>
       </c>
       <c r="C9" s="9" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="D9" s="9" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="E9" s="3" t="b">
         <v>0</v>
@@ -6760,10 +6766,10 @@
         <v>170</v>
       </c>
       <c r="C10" s="9" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="D10" s="9" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="E10" s="3" t="b">
         <v>0</v>
@@ -6781,10 +6787,10 @@
         <v>170</v>
       </c>
       <c r="C11" s="9" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="D11" s="9" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="E11" s="3" t="b">
         <v>1</v>
@@ -6802,17 +6808,17 @@
         <v>109</v>
       </c>
       <c r="C12" s="9" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="D12" s="9" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="F12" s="3"/>
       <c r="G12" s="3" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="H12" s="23"/>
       <c r="I12" s="24"/>
@@ -6825,17 +6831,17 @@
         <v>109</v>
       </c>
       <c r="C13" s="9" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="D13" s="9" t="s">
+        <v>316</v>
+      </c>
+      <c r="E13" s="3" t="s">
         <v>317</v>
-      </c>
-      <c r="E13" s="3" t="s">
-        <v>318</v>
       </c>
       <c r="F13" s="3"/>
       <c r="G13" s="3" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="H13" s="23"/>
       <c r="I13" s="24"/>
@@ -6848,15 +6854,15 @@
         <v>109</v>
       </c>
       <c r="C14" s="9" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="D14" s="9" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="E14" s="3"/>
       <c r="F14" s="3"/>
       <c r="G14" s="3" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="H14" s="23"/>
       <c r="I14" s="24"/>
@@ -6869,15 +6875,15 @@
         <v>109</v>
       </c>
       <c r="C15" s="9" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="D15" s="9" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="E15" s="3"/>
       <c r="F15" s="3"/>
       <c r="G15" s="3" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="H15" s="23"/>
       <c r="I15" s="24"/>
@@ -6890,15 +6896,15 @@
         <v>109</v>
       </c>
       <c r="C16" s="9" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="D16" s="9" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="E16" s="3"/>
       <c r="F16" s="3"/>
       <c r="G16" s="3" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="H16" s="23"/>
       <c r="I16" s="24"/>
@@ -6911,10 +6917,10 @@
         <v>109</v>
       </c>
       <c r="C17" s="9" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="D17" s="9" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="E17" s="3">
         <v>0</v>
@@ -6932,10 +6938,10 @@
         <v>109</v>
       </c>
       <c r="C18" s="9" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="D18" s="9" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="E18" s="3">
         <v>1</v>
@@ -6953,10 +6959,10 @@
         <v>109</v>
       </c>
       <c r="C19" s="9" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="D19" s="9" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="E19" s="3"/>
       <c r="F19" s="3"/>
@@ -6972,10 +6978,10 @@
         <v>109</v>
       </c>
       <c r="C20" s="9" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="D20" s="9" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="E20" s="3"/>
       <c r="F20" s="3"/>
@@ -6991,10 +6997,10 @@
         <v>109</v>
       </c>
       <c r="C21" s="9" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="D21" s="9" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="E21" s="3"/>
       <c r="F21" s="3"/>
@@ -7010,17 +7016,17 @@
         <v>170</v>
       </c>
       <c r="C22" s="9" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="D22" s="9" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="E22" s="3" t="b">
         <v>0</v>
       </c>
       <c r="F22" s="3"/>
       <c r="G22" s="3" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.15">
@@ -7031,17 +7037,17 @@
         <v>170</v>
       </c>
       <c r="C23" s="9" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="D23" s="9" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="E23" s="3" t="b">
         <v>1</v>
       </c>
       <c r="F23" s="3"/>
       <c r="G23" s="3" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.15">
@@ -7052,15 +7058,15 @@
         <v>170</v>
       </c>
       <c r="C24" s="9" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="D24" s="9" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="E24" s="3"/>
       <c r="F24" s="3"/>
       <c r="G24" s="3" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.15">
@@ -7071,15 +7077,15 @@
         <v>170</v>
       </c>
       <c r="C25" s="9" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="D25" s="9" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="E25" s="3"/>
       <c r="F25" s="3"/>
       <c r="G25" s="3" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.15">
@@ -7090,15 +7096,15 @@
         <v>170</v>
       </c>
       <c r="C26" s="9" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="D26" s="9" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="E26" s="3"/>
       <c r="F26" s="3"/>
       <c r="G26" s="3" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.15">
@@ -7109,10 +7115,10 @@
         <v>170</v>
       </c>
       <c r="C27" s="9" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="D27" s="9" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="E27" s="3" t="b">
         <v>1</v>
@@ -7130,10 +7136,10 @@
         <v>170</v>
       </c>
       <c r="C28" s="9" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="D28" s="9" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="E28" s="3" t="b">
         <v>0</v>
@@ -7151,10 +7157,10 @@
         <v>170</v>
       </c>
       <c r="C29" s="9" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="D29" s="9" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="E29" s="3"/>
       <c r="F29" s="3"/>
@@ -7170,10 +7176,10 @@
         <v>170</v>
       </c>
       <c r="C30" s="9" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="D30" s="9" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="E30" s="3"/>
       <c r="F30" s="3"/>
@@ -7189,10 +7195,10 @@
         <v>170</v>
       </c>
       <c r="C31" s="9" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="D31" s="9" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="E31" s="3"/>
       <c r="F31" s="3"/>
@@ -7208,13 +7214,13 @@
         <v>170</v>
       </c>
       <c r="C32" s="9" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="D32" s="9" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
       <c r="E32" s="3" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="F32" s="3"/>
       <c r="G32" s="3"/>
@@ -7227,29 +7233,29 @@
         <v>170</v>
       </c>
       <c r="C33" s="9" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="D33" s="9" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="E33" s="3" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="F33" s="3"/>
       <c r="G33" s="3"/>
     </row>
     <row r="34" spans="1:7" s="2" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A34" s="18" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B34" s="18" t="s">
         <v>170</v>
       </c>
       <c r="C34" s="9" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="D34" s="9" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="E34" s="3" t="b">
         <v>0</v>
@@ -7265,13 +7271,13 @@
         <v>170</v>
       </c>
       <c r="C35" s="9" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="D35" s="9" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
       <c r="E35" s="3" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="F35" s="3"/>
       <c r="G35" s="3"/>
@@ -7284,29 +7290,29 @@
         <v>170</v>
       </c>
       <c r="C36" s="9" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="D36" s="9" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
       <c r="E36" s="3" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
       <c r="F36" s="3"/>
       <c r="G36" s="3"/>
     </row>
     <row r="37" spans="1:7" s="2" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A37" s="18" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B37" s="18" t="s">
         <v>170</v>
       </c>
       <c r="C37" s="9" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="D37" s="9" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
       <c r="E37" s="3" t="b">
         <v>0</v>
@@ -7322,13 +7328,13 @@
         <v>170</v>
       </c>
       <c r="C38" s="9" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="D38" s="9" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
       <c r="E38" s="3" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="F38" s="3"/>
       <c r="G38" s="3"/>
@@ -7341,29 +7347,29 @@
         <v>170</v>
       </c>
       <c r="C39" s="9" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="D39" s="9" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="E39" s="3" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="F39" s="3"/>
       <c r="G39" s="3"/>
     </row>
     <row r="40" spans="1:7" s="2" customFormat="1" ht="13" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A40" s="18" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B40" s="18" t="s">
         <v>170</v>
       </c>
       <c r="C40" s="9" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="D40" s="9" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
       <c r="E40" s="3" t="b">
         <v>0</v>
@@ -7379,17 +7385,17 @@
         <v>170</v>
       </c>
       <c r="C41" s="9" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="D41" s="9" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="E41" s="3" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="F41" s="3"/>
       <c r="G41" s="3" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.15">
@@ -7400,31 +7406,31 @@
         <v>170</v>
       </c>
       <c r="C42" s="9" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="D42" s="9" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="E42" s="3" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="F42" s="3"/>
       <c r="G42" s="3" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
     </row>
     <row r="43" spans="1:7" s="2" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A43" s="18" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B43" s="18" t="s">
         <v>170</v>
       </c>
       <c r="C43" s="9" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="D43" s="9" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="E43" s="3" t="b">
         <v>1</v>
@@ -7442,17 +7448,17 @@
         <v>170</v>
       </c>
       <c r="C44" s="9" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="D44" s="9" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
       <c r="E44" s="3" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="F44" s="3"/>
       <c r="G44" s="3" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.15">
@@ -7463,31 +7469,31 @@
         <v>170</v>
       </c>
       <c r="C45" s="9" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="D45" s="9" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
       <c r="E45" s="3" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="F45" s="3"/>
       <c r="G45" s="3" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
     </row>
     <row r="46" spans="1:7" s="2" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A46" s="18" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B46" s="18" t="s">
         <v>170</v>
       </c>
       <c r="C46" s="9" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="D46" s="9" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="E46" s="3" t="b">
         <v>1</v>
@@ -7505,13 +7511,13 @@
         <v>109</v>
       </c>
       <c r="C47" s="9" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="D47" s="9" t="s">
+        <v>582</v>
+      </c>
+      <c r="E47" s="3" t="s">
         <v>583</v>
-      </c>
-      <c r="E47" s="3" t="s">
-        <v>584</v>
       </c>
       <c r="F47" s="3"/>
       <c r="G47" s="3"/>
@@ -7524,10 +7530,10 @@
         <v>170</v>
       </c>
       <c r="C48" s="9" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="D48" s="9" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="E48" s="3"/>
       <c r="F48" s="3"/>
@@ -7541,10 +7547,10 @@
         <v>170</v>
       </c>
       <c r="C49" s="9" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="D49" s="9" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="E49" s="3"/>
       <c r="F49" s="3"/>
@@ -7558,10 +7564,10 @@
         <v>170</v>
       </c>
       <c r="C50" s="9" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="D50" s="9" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="E50" s="3"/>
       <c r="F50" s="3"/>
@@ -7575,10 +7581,10 @@
         <v>170</v>
       </c>
       <c r="C51" s="9" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="D51" s="9" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="E51" s="3" t="b">
         <v>1</v>
@@ -7594,10 +7600,10 @@
         <v>170</v>
       </c>
       <c r="C52" s="9" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="D52" s="9" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="E52" s="3" t="b">
         <v>0</v>
@@ -7613,10 +7619,10 @@
         <v>170</v>
       </c>
       <c r="C53" s="9" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="D53" s="9" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="E53" s="3" t="b">
         <v>0</v>
@@ -7632,10 +7638,10 @@
         <v>170</v>
       </c>
       <c r="C54" s="9" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="D54" s="9" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="E54" s="3" t="b">
         <v>1</v>
@@ -7651,13 +7657,13 @@
         <v>109</v>
       </c>
       <c r="C55" s="9" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="D55" s="9" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="E55" s="3" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="F55" s="3"/>
       <c r="G55" s="3"/>
@@ -7670,13 +7676,13 @@
         <v>109</v>
       </c>
       <c r="C56" s="9" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="D56" s="9" t="s">
+        <v>347</v>
+      </c>
+      <c r="E56" s="3" t="s">
         <v>348</v>
-      </c>
-      <c r="E56" s="3" t="s">
-        <v>349</v>
       </c>
       <c r="F56" s="3"/>
       <c r="G56" s="3"/>
@@ -7689,10 +7695,10 @@
         <v>109</v>
       </c>
       <c r="C57" s="9" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="D57" s="9" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="E57" s="3">
         <v>0</v>
@@ -7708,10 +7714,10 @@
         <v>109</v>
       </c>
       <c r="C58" s="9" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="D58" s="9" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="E58" s="3">
         <v>1</v>
@@ -7727,13 +7733,13 @@
         <v>170</v>
       </c>
       <c r="C59" s="9" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="D59" s="9" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="E59" s="3" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="F59" s="3"/>
       <c r="G59" s="3"/>
@@ -7746,13 +7752,13 @@
         <v>170</v>
       </c>
       <c r="C60" s="9" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="D60" s="9" t="s">
+        <v>351</v>
+      </c>
+      <c r="E60" s="3" t="s">
         <v>352</v>
-      </c>
-      <c r="E60" s="3" t="s">
-        <v>353</v>
       </c>
       <c r="F60" s="3"/>
       <c r="G60" s="3"/>
@@ -7765,10 +7771,10 @@
         <v>170</v>
       </c>
       <c r="C61" s="9" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="D61" s="9" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="E61" s="3" t="b">
         <v>1</v>
@@ -7784,10 +7790,10 @@
         <v>170</v>
       </c>
       <c r="C62" s="9" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="D62" s="9" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="E62" s="3" t="b">
         <v>0</v>
@@ -7803,13 +7809,13 @@
         <v>170</v>
       </c>
       <c r="C63" s="9" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="D63" s="9" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
       <c r="E63" s="3" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="F63" s="3"/>
       <c r="G63" s="3"/>
@@ -7822,29 +7828,29 @@
         <v>170</v>
       </c>
       <c r="C64" s="9" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="D64" s="9" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="E64" s="3" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="F64" s="3"/>
       <c r="G64" s="3"/>
     </row>
     <row r="65" spans="1:7" s="2" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A65" s="18" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B65" s="18" t="s">
         <v>170</v>
       </c>
       <c r="C65" s="9" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="D65" s="9" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
       <c r="E65" s="3" t="b">
         <v>0</v>
@@ -7860,13 +7866,13 @@
         <v>170</v>
       </c>
       <c r="C66" s="9" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="D66" s="9" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
       <c r="E66" s="3" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="F66" s="3"/>
       <c r="G66" s="3"/>
@@ -7879,29 +7885,29 @@
         <v>170</v>
       </c>
       <c r="C67" s="9" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="D67" s="9" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
       <c r="E67" s="3" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
       <c r="F67" s="3"/>
       <c r="G67" s="3"/>
     </row>
     <row r="68" spans="1:7" s="2" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A68" s="18" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B68" s="18" t="s">
         <v>170</v>
       </c>
       <c r="C68" s="9" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="D68" s="9" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
       <c r="E68" s="3" t="b">
         <v>0</v>
@@ -7917,13 +7923,13 @@
         <v>170</v>
       </c>
       <c r="C69" s="9" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="D69" s="9" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="E69" s="3" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="F69" s="3"/>
       <c r="G69" s="3"/>
@@ -7936,29 +7942,29 @@
         <v>170</v>
       </c>
       <c r="C70" s="9" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="D70" s="9" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="E70" s="3" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="F70" s="3"/>
       <c r="G70" s="3"/>
     </row>
     <row r="71" spans="1:7" s="2" customFormat="1" ht="13" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A71" s="18" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B71" s="18" t="s">
         <v>170</v>
       </c>
       <c r="C71" s="9" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="D71" s="9" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
       <c r="E71" s="3" t="b">
         <v>0</v>
@@ -7974,13 +7980,13 @@
         <v>170</v>
       </c>
       <c r="C72" s="9" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="D72" s="9" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="E72" s="3" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="F72" s="3"/>
       <c r="G72" s="3"/>
@@ -7993,29 +7999,29 @@
         <v>170</v>
       </c>
       <c r="C73" s="9" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="D73" s="9" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
       <c r="E73" s="3" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="F73" s="3"/>
       <c r="G73" s="3"/>
     </row>
     <row r="74" spans="1:7" s="2" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A74" s="18" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B74" s="18" t="s">
         <v>170</v>
       </c>
       <c r="C74" s="9" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="D74" s="9" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
       <c r="E74" s="3" t="b">
         <v>1</v>
@@ -8031,13 +8037,13 @@
         <v>170</v>
       </c>
       <c r="C75" s="9" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="D75" s="9" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
       <c r="E75" s="3" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="F75" s="3"/>
       <c r="G75" s="3"/>
@@ -8050,29 +8056,29 @@
         <v>170</v>
       </c>
       <c r="C76" s="9" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="D76" s="9" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="E76" s="3" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="F76" s="3"/>
       <c r="G76" s="3"/>
     </row>
     <row r="77" spans="1:7" s="2" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A77" s="18" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B77" s="18" t="s">
         <v>170</v>
       </c>
       <c r="C77" s="9" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="D77" s="9" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="E77" s="3" t="b">
         <v>1</v>
@@ -8088,13 +8094,13 @@
         <v>109</v>
       </c>
       <c r="C78" s="9" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="D78" s="9" t="s">
+        <v>354</v>
+      </c>
+      <c r="E78" s="3" t="s">
         <v>355</v>
-      </c>
-      <c r="E78" s="3" t="s">
-        <v>356</v>
       </c>
       <c r="F78" s="3"/>
       <c r="G78" s="3"/>
@@ -8107,10 +8113,10 @@
         <v>170</v>
       </c>
       <c r="C79" s="9" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="D79" s="9" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="E79" s="3"/>
       <c r="F79" s="3"/>
@@ -8124,10 +8130,10 @@
         <v>170</v>
       </c>
       <c r="C80" s="9" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="D80" s="9" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="E80" s="3"/>
       <c r="F80" s="3"/>
@@ -8141,10 +8147,10 @@
         <v>170</v>
       </c>
       <c r="C81" s="9" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="D81" s="9" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="E81" s="3"/>
       <c r="F81" s="3"/>
@@ -8158,10 +8164,10 @@
         <v>170</v>
       </c>
       <c r="C82" s="9" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="D82" s="9" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="E82" s="3" t="b">
         <v>1</v>
@@ -8177,10 +8183,10 @@
         <v>170</v>
       </c>
       <c r="C83" s="9" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="D83" s="9" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="E83" s="3" t="b">
         <v>0</v>
@@ -8196,10 +8202,10 @@
         <v>170</v>
       </c>
       <c r="C84" s="9" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="D84" s="9" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="E84" s="3" t="b">
         <v>0</v>
@@ -8215,10 +8221,10 @@
         <v>170</v>
       </c>
       <c r="C85" s="9" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="D85" s="9" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="E85" s="3" t="b">
         <v>1</v>
@@ -8234,13 +8240,13 @@
         <v>109</v>
       </c>
       <c r="C86" s="9" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="D86" s="9" t="s">
+        <v>363</v>
+      </c>
+      <c r="E86" s="3" t="s">
         <v>364</v>
-      </c>
-      <c r="E86" s="3" t="s">
-        <v>365</v>
       </c>
       <c r="F86" s="3"/>
       <c r="G86" s="3"/>
@@ -8253,13 +8259,13 @@
         <v>109</v>
       </c>
       <c r="C87" s="9" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="D87" s="9" t="s">
+        <v>365</v>
+      </c>
+      <c r="E87" s="3" t="s">
         <v>366</v>
-      </c>
-      <c r="E87" s="3" t="s">
-        <v>367</v>
       </c>
       <c r="F87" s="3"/>
       <c r="G87" s="3"/>
@@ -8272,10 +8278,10 @@
         <v>109</v>
       </c>
       <c r="C88" s="9" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="D88" s="9" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="E88" s="3">
         <v>0</v>
@@ -8291,10 +8297,10 @@
         <v>109</v>
       </c>
       <c r="C89" s="9" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="D89" s="9" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="E89" s="3">
         <v>1</v>
@@ -8310,13 +8316,13 @@
         <v>170</v>
       </c>
       <c r="C90" s="9" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="D90" s="9" t="s">
+        <v>369</v>
+      </c>
+      <c r="E90" s="3" t="s">
         <v>370</v>
-      </c>
-      <c r="E90" s="3" t="s">
-        <v>371</v>
       </c>
       <c r="F90" s="3"/>
       <c r="G90" s="3"/>
@@ -8329,13 +8335,13 @@
         <v>170</v>
       </c>
       <c r="C91" s="9" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="D91" s="9" t="s">
+        <v>371</v>
+      </c>
+      <c r="E91" s="3" t="s">
         <v>372</v>
-      </c>
-      <c r="E91" s="3" t="s">
-        <v>373</v>
       </c>
       <c r="F91" s="3"/>
       <c r="G91" s="3"/>
@@ -8348,10 +8354,10 @@
         <v>170</v>
       </c>
       <c r="C92" s="9" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="D92" s="9" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="E92" s="3" t="b">
         <v>1</v>
@@ -8367,10 +8373,10 @@
         <v>170</v>
       </c>
       <c r="C93" s="9" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="D93" s="9" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="E93" s="3" t="b">
         <v>0</v>
@@ -8386,10 +8392,10 @@
         <v>170</v>
       </c>
       <c r="C94" s="9" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="D94" s="9" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="E94" s="3"/>
       <c r="F94" s="3"/>
@@ -8403,10 +8409,10 @@
         <v>170</v>
       </c>
       <c r="C95" s="9" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="D95" s="9" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="E95" s="3"/>
       <c r="F95" s="3"/>
@@ -8414,16 +8420,16 @@
     </row>
     <row r="96" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A96" s="18" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B96" s="18" t="s">
         <v>170</v>
       </c>
       <c r="C96" s="9" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="D96" s="9" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="E96" s="3" t="b">
         <v>0</v>
@@ -8439,13 +8445,13 @@
         <v>109</v>
       </c>
       <c r="C97" s="9" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="D97" s="9" t="s">
+        <v>378</v>
+      </c>
+      <c r="E97" s="3" t="s">
         <v>379</v>
-      </c>
-      <c r="E97" s="3" t="s">
-        <v>380</v>
       </c>
       <c r="F97" s="3"/>
       <c r="G97" s="3"/>
@@ -8458,10 +8464,10 @@
         <v>170</v>
       </c>
       <c r="C98" s="9" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="D98" s="9" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="E98" s="3"/>
       <c r="F98" s="3"/>
@@ -8475,10 +8481,10 @@
         <v>170</v>
       </c>
       <c r="C99" s="9" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="D99" s="9" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="E99" s="3"/>
       <c r="F99" s="3"/>
@@ -8492,10 +8498,10 @@
         <v>170</v>
       </c>
       <c r="C100" s="9" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="D100" s="9" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="E100" s="3"/>
       <c r="F100" s="3"/>
@@ -8509,10 +8515,10 @@
         <v>170</v>
       </c>
       <c r="C101" s="9" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="D101" s="9" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="E101" s="3" t="b">
         <v>1</v>
@@ -8528,10 +8534,10 @@
         <v>170</v>
       </c>
       <c r="C102" s="9" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="D102" s="9" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="E102" s="3" t="b">
         <v>0</v>
@@ -8547,10 +8553,10 @@
         <v>170</v>
       </c>
       <c r="C103" s="9" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="D103" s="9" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="E103" s="3" t="b">
         <v>0</v>
@@ -8566,10 +8572,10 @@
         <v>170</v>
       </c>
       <c r="C104" s="9" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="D104" s="9" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="E104" s="3" t="b">
         <v>1</v>
@@ -8585,13 +8591,13 @@
         <v>109</v>
       </c>
       <c r="C105" s="9" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="D105" s="9" t="s">
+        <v>387</v>
+      </c>
+      <c r="E105" s="3" t="s">
         <v>388</v>
-      </c>
-      <c r="E105" s="3" t="s">
-        <v>389</v>
       </c>
       <c r="F105" s="3"/>
       <c r="G105" s="3"/>
@@ -8604,13 +8610,13 @@
         <v>109</v>
       </c>
       <c r="C106" s="9" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="D106" s="9" t="s">
+        <v>389</v>
+      </c>
+      <c r="E106" s="3" t="s">
         <v>390</v>
-      </c>
-      <c r="E106" s="3" t="s">
-        <v>391</v>
       </c>
       <c r="F106" s="3"/>
       <c r="G106" s="3"/>
@@ -8623,10 +8629,10 @@
         <v>109</v>
       </c>
       <c r="C107" s="9" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="D107" s="9" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="E107" s="3">
         <v>0</v>
@@ -8642,10 +8648,10 @@
         <v>109</v>
       </c>
       <c r="C108" s="9" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="D108" s="9" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="E108" s="3">
         <v>1</v>
@@ -8661,10 +8667,10 @@
         <v>170</v>
       </c>
       <c r="C109" s="9" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="D109" s="9" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="E109" s="3" t="b">
         <v>0</v>
@@ -8680,10 +8686,10 @@
         <v>170</v>
       </c>
       <c r="C110" s="9" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="D110" s="9" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="E110" s="3" t="b">
         <v>1</v>
@@ -8699,10 +8705,10 @@
         <v>170</v>
       </c>
       <c r="C111" s="9" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="D111" s="9" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="E111" s="3" t="b">
         <v>1</v>
@@ -8718,10 +8724,10 @@
         <v>170</v>
       </c>
       <c r="C112" s="9" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="D112" s="9" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="E112" s="3" t="b">
         <v>0</v>
@@ -8737,13 +8743,13 @@
         <v>109</v>
       </c>
       <c r="C113" s="9" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="D113" s="9" t="s">
+        <v>397</v>
+      </c>
+      <c r="E113" s="3" t="s">
         <v>398</v>
-      </c>
-      <c r="E113" s="3" t="s">
-        <v>399</v>
       </c>
       <c r="F113" s="3"/>
       <c r="G113" s="3"/>
@@ -8756,10 +8762,10 @@
         <v>170</v>
       </c>
       <c r="C114" s="9" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="D114" s="9" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="E114" s="3"/>
       <c r="F114" s="3"/>
@@ -8773,10 +8779,10 @@
         <v>170</v>
       </c>
       <c r="C115" s="9" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="D115" s="9" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="E115" s="3"/>
       <c r="F115" s="3"/>
@@ -8790,10 +8796,10 @@
         <v>170</v>
       </c>
       <c r="C116" s="9" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="D116" s="9" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="E116" s="3"/>
       <c r="F116" s="3"/>
@@ -8807,10 +8813,10 @@
         <v>170</v>
       </c>
       <c r="C117" s="9" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="D117" s="9" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="E117" s="3" t="b">
         <v>1</v>
@@ -8826,10 +8832,10 @@
         <v>170</v>
       </c>
       <c r="C118" s="9" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="D118" s="9" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="E118" s="3" t="b">
         <v>0</v>
@@ -8845,10 +8851,10 @@
         <v>170</v>
       </c>
       <c r="C119" s="9" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="D119" s="9" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="E119" s="3" t="b">
         <v>0</v>
@@ -8864,10 +8870,10 @@
         <v>170</v>
       </c>
       <c r="C120" s="9" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="D120" s="9" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="E120" s="3" t="b">
         <v>1</v>
@@ -8883,13 +8889,13 @@
         <v>109</v>
       </c>
       <c r="C121" s="9" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="D121" s="9" t="s">
+        <v>406</v>
+      </c>
+      <c r="E121" s="3" t="s">
         <v>407</v>
-      </c>
-      <c r="E121" s="3" t="s">
-        <v>408</v>
       </c>
       <c r="F121" s="3"/>
       <c r="G121" s="3"/>
@@ -8902,13 +8908,13 @@
         <v>109</v>
       </c>
       <c r="C122" s="9" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="D122" s="9" t="s">
+        <v>408</v>
+      </c>
+      <c r="E122" s="3" t="s">
         <v>409</v>
-      </c>
-      <c r="E122" s="3" t="s">
-        <v>410</v>
       </c>
       <c r="F122" s="3"/>
       <c r="G122" s="3"/>
@@ -8921,10 +8927,10 @@
         <v>109</v>
       </c>
       <c r="C123" s="9" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="D123" s="9" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="E123" s="3">
         <v>0</v>
@@ -8940,10 +8946,10 @@
         <v>109</v>
       </c>
       <c r="C124" s="9" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="D124" s="9" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="E124" s="3">
         <v>1</v>
@@ -8959,13 +8965,13 @@
         <v>170</v>
       </c>
       <c r="C125" s="9" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="D125" s="9" t="s">
+        <v>412</v>
+      </c>
+      <c r="E125" s="3" t="s">
         <v>413</v>
-      </c>
-      <c r="E125" s="3" t="s">
-        <v>414</v>
       </c>
       <c r="F125" s="3"/>
       <c r="G125" s="3"/>
@@ -8978,13 +8984,13 @@
         <v>170</v>
       </c>
       <c r="C126" s="9" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="D126" s="9" t="s">
+        <v>414</v>
+      </c>
+      <c r="E126" s="3" t="s">
         <v>415</v>
-      </c>
-      <c r="E126" s="3" t="s">
-        <v>416</v>
       </c>
       <c r="F126" s="3"/>
       <c r="G126" s="3"/>
@@ -8997,10 +9003,10 @@
         <v>170</v>
       </c>
       <c r="C127" s="9" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="D127" s="9" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="E127" s="3" t="b">
         <v>1</v>
@@ -9016,10 +9022,10 @@
         <v>170</v>
       </c>
       <c r="C128" s="9" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="D128" s="9" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="E128" s="3" t="b">
         <v>0</v>
@@ -9035,13 +9041,13 @@
         <v>109</v>
       </c>
       <c r="C129" s="9" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="D129" s="9" t="s">
+        <v>418</v>
+      </c>
+      <c r="E129" s="3" t="s">
         <v>419</v>
-      </c>
-      <c r="E129" s="3" t="s">
-        <v>420</v>
       </c>
       <c r="F129" s="3"/>
       <c r="G129" s="3"/>
@@ -9054,10 +9060,10 @@
         <v>170</v>
       </c>
       <c r="C130" s="9" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="D130" s="9" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="E130" s="3"/>
       <c r="F130" s="3"/>
@@ -9071,10 +9077,10 @@
         <v>170</v>
       </c>
       <c r="C131" s="9" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="D131" s="9" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="E131" s="3"/>
       <c r="F131" s="3"/>
@@ -9088,10 +9094,10 @@
         <v>170</v>
       </c>
       <c r="C132" s="9" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="D132" s="9" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="E132" s="3"/>
       <c r="F132" s="3"/>
@@ -9105,10 +9111,10 @@
         <v>170</v>
       </c>
       <c r="C133" s="9" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="D133" s="9" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="E133" s="3" t="b">
         <v>1</v>
@@ -9124,10 +9130,10 @@
         <v>170</v>
       </c>
       <c r="C134" s="9" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="D134" s="9" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="E134" s="3" t="b">
         <v>0</v>
@@ -9143,10 +9149,10 @@
         <v>170</v>
       </c>
       <c r="C135" s="9" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="D135" s="9" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="E135" s="3" t="b">
         <v>0</v>
@@ -9162,10 +9168,10 @@
         <v>170</v>
       </c>
       <c r="C136" s="9" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="D136" s="9" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="E136" s="3" t="b">
         <v>1</v>
@@ -9181,13 +9187,13 @@
         <v>109</v>
       </c>
       <c r="C137" s="9" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="D137" s="9" t="s">
+        <v>427</v>
+      </c>
+      <c r="E137" s="3" t="s">
         <v>428</v>
-      </c>
-      <c r="E137" s="3" t="s">
-        <v>429</v>
       </c>
       <c r="F137" s="3"/>
       <c r="G137" s="3"/>
@@ -9200,13 +9206,13 @@
         <v>109</v>
       </c>
       <c r="C138" s="9" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="D138" s="9" t="s">
+        <v>429</v>
+      </c>
+      <c r="E138" s="3" t="s">
         <v>430</v>
-      </c>
-      <c r="E138" s="3" t="s">
-        <v>431</v>
       </c>
       <c r="F138" s="3"/>
       <c r="G138" s="3"/>
@@ -9219,10 +9225,10 @@
         <v>109</v>
       </c>
       <c r="C139" s="9" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="D139" s="9" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="E139" s="3">
         <v>0</v>
@@ -9238,10 +9244,10 @@
         <v>109</v>
       </c>
       <c r="C140" s="9" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="D140" s="9" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="E140" s="3">
         <v>1</v>
@@ -9257,13 +9263,13 @@
         <v>170</v>
       </c>
       <c r="C141" s="9" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="D141" s="9" t="s">
+        <v>433</v>
+      </c>
+      <c r="E141" s="3" t="s">
         <v>434</v>
-      </c>
-      <c r="E141" s="3" t="s">
-        <v>435</v>
       </c>
       <c r="F141" s="3"/>
       <c r="G141" s="3"/>
@@ -9276,13 +9282,13 @@
         <v>170</v>
       </c>
       <c r="C142" s="9" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="D142" s="9" t="s">
+        <v>435</v>
+      </c>
+      <c r="E142" s="3" t="s">
         <v>436</v>
-      </c>
-      <c r="E142" s="3" t="s">
-        <v>437</v>
       </c>
       <c r="F142" s="3"/>
       <c r="G142" s="3"/>
@@ -9295,10 +9301,10 @@
         <v>170</v>
       </c>
       <c r="C143" s="9" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="D143" s="9" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="E143" s="3" t="b">
         <v>1</v>
@@ -9314,10 +9320,10 @@
         <v>170</v>
       </c>
       <c r="C144" s="9" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="D144" s="9" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="E144" s="3" t="b">
         <v>0</v>
@@ -9333,13 +9339,13 @@
         <v>109</v>
       </c>
       <c r="C145" s="9" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="D145" s="9" t="s">
+        <v>439</v>
+      </c>
+      <c r="E145" s="3" t="s">
         <v>440</v>
-      </c>
-      <c r="E145" s="3" t="s">
-        <v>441</v>
       </c>
       <c r="F145" s="3"/>
       <c r="G145" s="3"/>
@@ -9352,10 +9358,10 @@
         <v>170</v>
       </c>
       <c r="C146" s="9" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="D146" s="9" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="E146" s="3"/>
       <c r="F146" s="3"/>
@@ -9369,10 +9375,10 @@
         <v>170</v>
       </c>
       <c r="C147" s="9" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="D147" s="9" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="E147" s="3"/>
       <c r="F147" s="3"/>
@@ -9386,10 +9392,10 @@
         <v>170</v>
       </c>
       <c r="C148" s="9" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="D148" s="9" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="E148" s="3"/>
       <c r="F148" s="3"/>
@@ -9403,10 +9409,10 @@
         <v>170</v>
       </c>
       <c r="C149" s="9" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="D149" s="9" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="E149" s="3" t="b">
         <v>1</v>
@@ -9422,10 +9428,10 @@
         <v>170</v>
       </c>
       <c r="C150" s="9" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="D150" s="9" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="E150" s="3" t="b">
         <v>0</v>
@@ -9441,10 +9447,10 @@
         <v>170</v>
       </c>
       <c r="C151" s="9" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="D151" s="9" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="E151" s="3" t="b">
         <v>0</v>
@@ -9460,10 +9466,10 @@
         <v>170</v>
       </c>
       <c r="C152" s="9" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="D152" s="9" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="E152" s="3" t="b">
         <v>1</v>
@@ -9479,13 +9485,13 @@
         <v>109</v>
       </c>
       <c r="C153" s="9" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="D153" s="9" t="s">
+        <v>448</v>
+      </c>
+      <c r="E153" s="3" t="s">
         <v>449</v>
-      </c>
-      <c r="E153" s="3" t="s">
-        <v>450</v>
       </c>
       <c r="F153" s="3"/>
       <c r="G153" s="3"/>
@@ -9498,13 +9504,13 @@
         <v>109</v>
       </c>
       <c r="C154" s="9" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="D154" s="9" t="s">
+        <v>450</v>
+      </c>
+      <c r="E154" s="3" t="s">
         <v>451</v>
-      </c>
-      <c r="E154" s="3" t="s">
-        <v>452</v>
       </c>
       <c r="F154" s="3"/>
       <c r="G154" s="3"/>
@@ -9517,10 +9523,10 @@
         <v>109</v>
       </c>
       <c r="C155" s="9" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="D155" s="9" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="E155" s="3">
         <v>0</v>
@@ -9536,10 +9542,10 @@
         <v>109</v>
       </c>
       <c r="C156" s="9" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="D156" s="9" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="E156" s="3">
         <v>1</v>
@@ -9555,13 +9561,13 @@
         <v>170</v>
       </c>
       <c r="C157" s="9" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="D157" s="9" t="s">
+        <v>454</v>
+      </c>
+      <c r="E157" s="3" t="s">
         <v>455</v>
-      </c>
-      <c r="E157" s="3" t="s">
-        <v>456</v>
       </c>
       <c r="F157" s="3"/>
       <c r="G157" s="3"/>
@@ -9574,13 +9580,13 @@
         <v>170</v>
       </c>
       <c r="C158" s="9" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="D158" s="9" t="s">
+        <v>456</v>
+      </c>
+      <c r="E158" s="3" t="s">
         <v>457</v>
-      </c>
-      <c r="E158" s="3" t="s">
-        <v>458</v>
       </c>
       <c r="F158" s="3"/>
       <c r="G158" s="3"/>
@@ -9593,10 +9599,10 @@
         <v>170</v>
       </c>
       <c r="C159" s="9" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="D159" s="9" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="E159" s="3" t="b">
         <v>1</v>
@@ -9612,10 +9618,10 @@
         <v>170</v>
       </c>
       <c r="C160" s="9" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="D160" s="9" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="E160" s="3" t="b">
         <v>0</v>
@@ -9631,13 +9637,13 @@
         <v>109</v>
       </c>
       <c r="C161" s="9" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="D161" s="9" t="s">
+        <v>460</v>
+      </c>
+      <c r="E161" s="3" t="s">
         <v>461</v>
-      </c>
-      <c r="E161" s="3" t="s">
-        <v>462</v>
       </c>
       <c r="F161" s="3"/>
       <c r="G161" s="3"/>
@@ -9650,10 +9656,10 @@
         <v>170</v>
       </c>
       <c r="C162" s="9" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="D162" s="9" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="E162" s="3"/>
       <c r="F162" s="3"/>
@@ -9667,10 +9673,10 @@
         <v>170</v>
       </c>
       <c r="C163" s="9" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="D163" s="9" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="E163" s="3"/>
       <c r="F163" s="3"/>
@@ -9684,10 +9690,10 @@
         <v>170</v>
       </c>
       <c r="C164" s="9" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="D164" s="9" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="E164" s="3"/>
       <c r="F164" s="3"/>
@@ -9701,10 +9707,10 @@
         <v>170</v>
       </c>
       <c r="C165" s="9" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="D165" s="9" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="E165" s="3" t="b">
         <v>1</v>
@@ -9720,10 +9726,10 @@
         <v>170</v>
       </c>
       <c r="C166" s="9" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="D166" s="9" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="E166" s="3" t="b">
         <v>0</v>
@@ -9739,10 +9745,10 @@
         <v>170</v>
       </c>
       <c r="C167" s="9" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="D167" s="9" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="E167" s="3" t="b">
         <v>0</v>
@@ -9758,10 +9764,10 @@
         <v>170</v>
       </c>
       <c r="C168" s="9" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="D168" s="9" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="E168" s="3" t="b">
         <v>1</v>
@@ -9777,13 +9783,13 @@
         <v>109</v>
       </c>
       <c r="C169" s="9" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="D169" s="9" t="s">
+        <v>469</v>
+      </c>
+      <c r="E169" s="3" t="s">
         <v>470</v>
-      </c>
-      <c r="E169" s="3" t="s">
-        <v>471</v>
       </c>
       <c r="F169" s="3"/>
       <c r="G169" s="3"/>
@@ -9796,13 +9802,13 @@
         <v>109</v>
       </c>
       <c r="C170" s="9" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="D170" s="9" t="s">
+        <v>471</v>
+      </c>
+      <c r="E170" s="3" t="s">
         <v>472</v>
-      </c>
-      <c r="E170" s="3" t="s">
-        <v>473</v>
       </c>
       <c r="F170" s="3"/>
       <c r="G170" s="3"/>
@@ -9815,10 +9821,10 @@
         <v>109</v>
       </c>
       <c r="C171" s="9" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="D171" s="9" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="E171" s="3">
         <v>0</v>
@@ -9834,10 +9840,10 @@
         <v>109</v>
       </c>
       <c r="C172" s="9" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="D172" s="9" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="E172" s="3">
         <v>1</v>
@@ -9853,13 +9859,13 @@
         <v>170</v>
       </c>
       <c r="C173" s="9" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="D173" s="9" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="E173" s="3" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="F173" s="3"/>
       <c r="G173" s="3"/>
@@ -9872,13 +9878,13 @@
         <v>170</v>
       </c>
       <c r="C174" s="9" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="D174" s="9" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="E174" s="3" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="F174" s="3"/>
       <c r="G174" s="3"/>
@@ -9891,10 +9897,10 @@
         <v>170</v>
       </c>
       <c r="C175" s="9" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="D175" s="9" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="E175" s="3" t="b">
         <v>1</v>
@@ -9910,10 +9916,10 @@
         <v>170</v>
       </c>
       <c r="C176" s="9" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="D176" s="9" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="E176" s="3" t="b">
         <v>0</v>
@@ -9929,13 +9935,13 @@
         <v>109</v>
       </c>
       <c r="C177" s="9" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="D177" s="9" t="s">
+        <v>479</v>
+      </c>
+      <c r="E177" s="3" t="s">
         <v>480</v>
-      </c>
-      <c r="E177" s="3" t="s">
-        <v>481</v>
       </c>
       <c r="F177" s="3"/>
       <c r="G177" s="3"/>
@@ -9948,10 +9954,10 @@
         <v>170</v>
       </c>
       <c r="C178" s="9" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="D178" s="9" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="E178" s="3"/>
       <c r="F178" s="3"/>
@@ -9965,10 +9971,10 @@
         <v>170</v>
       </c>
       <c r="C179" s="9" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="D179" s="9" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="E179" s="3"/>
       <c r="F179" s="3"/>
@@ -9982,10 +9988,10 @@
         <v>170</v>
       </c>
       <c r="C180" s="9" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="D180" s="9" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="E180" s="3"/>
       <c r="F180" s="3"/>
@@ -9999,10 +10005,10 @@
         <v>170</v>
       </c>
       <c r="C181" s="9" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="D181" s="9" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="E181" s="3" t="b">
         <v>1</v>
@@ -10018,10 +10024,10 @@
         <v>170</v>
       </c>
       <c r="C182" s="9" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="D182" s="9" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="E182" s="3" t="b">
         <v>0</v>
@@ -10037,10 +10043,10 @@
         <v>170</v>
       </c>
       <c r="C183" s="9" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="D183" s="9" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="E183" s="3" t="b">
         <v>0</v>
@@ -10056,10 +10062,10 @@
         <v>170</v>
       </c>
       <c r="C184" s="9" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="D184" s="9" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="E184" s="3" t="b">
         <v>1</v>
@@ -10075,13 +10081,13 @@
         <v>109</v>
       </c>
       <c r="C185" s="9" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="D185" s="9" t="s">
+        <v>488</v>
+      </c>
+      <c r="E185" s="3" t="s">
         <v>489</v>
-      </c>
-      <c r="E185" s="3" t="s">
-        <v>490</v>
       </c>
       <c r="F185" s="3"/>
       <c r="G185" s="3"/>
@@ -10094,13 +10100,13 @@
         <v>109</v>
       </c>
       <c r="C186" s="9" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="D186" s="9" t="s">
+        <v>490</v>
+      </c>
+      <c r="E186" s="3" t="s">
         <v>491</v>
-      </c>
-      <c r="E186" s="3" t="s">
-        <v>492</v>
       </c>
       <c r="F186" s="3"/>
       <c r="G186" s="3"/>
@@ -10113,13 +10119,13 @@
         <v>109</v>
       </c>
       <c r="C187" s="9" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="D187" s="9" t="s">
+        <v>492</v>
+      </c>
+      <c r="E187" s="3" t="s">
         <v>493</v>
-      </c>
-      <c r="E187" s="3" t="s">
-        <v>494</v>
       </c>
       <c r="F187" s="3"/>
       <c r="G187" s="3"/>
@@ -10132,13 +10138,13 @@
         <v>109</v>
       </c>
       <c r="C188" s="9" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="D188" s="9" t="s">
+        <v>494</v>
+      </c>
+      <c r="E188" s="3" t="s">
         <v>495</v>
-      </c>
-      <c r="E188" s="3" t="s">
-        <v>496</v>
       </c>
       <c r="F188" s="3"/>
       <c r="G188" s="3"/>
@@ -10151,10 +10157,10 @@
         <v>109</v>
       </c>
       <c r="C189" s="9" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="D189" s="9" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="E189" s="3">
         <v>0</v>
@@ -10170,10 +10176,10 @@
         <v>109</v>
       </c>
       <c r="C190" s="9" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="D190" s="9" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="E190" s="3">
         <v>1</v>
@@ -10189,10 +10195,10 @@
         <v>109</v>
       </c>
       <c r="C191" s="9" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="D191" s="9" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="E191" s="3">
         <v>2</v>
@@ -10208,10 +10214,10 @@
         <v>109</v>
       </c>
       <c r="C192" s="9" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="D192" s="9" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="E192" s="3">
         <v>3</v>
@@ -10227,13 +10233,13 @@
         <v>170</v>
       </c>
       <c r="C193" s="9" t="s">
+        <v>329</v>
+      </c>
+      <c r="D193" s="9" t="s">
+        <v>500</v>
+      </c>
+      <c r="E193" s="3" t="s">
         <v>330</v>
-      </c>
-      <c r="D193" s="9" t="s">
-        <v>501</v>
-      </c>
-      <c r="E193" s="3" t="s">
-        <v>331</v>
       </c>
       <c r="F193" s="3"/>
       <c r="G193" s="3"/>
@@ -10246,13 +10252,13 @@
         <v>170</v>
       </c>
       <c r="C194" s="9" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="D194" s="9" t="s">
+        <v>501</v>
+      </c>
+      <c r="E194" s="3" t="s">
         <v>502</v>
-      </c>
-      <c r="E194" s="3" t="s">
-        <v>503</v>
       </c>
       <c r="F194" s="3"/>
       <c r="G194" s="3"/>
@@ -10265,13 +10271,13 @@
         <v>170</v>
       </c>
       <c r="C195" s="9" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="D195" s="9" t="s">
+        <v>503</v>
+      </c>
+      <c r="E195" s="3" t="s">
         <v>504</v>
-      </c>
-      <c r="E195" s="3" t="s">
-        <v>505</v>
       </c>
       <c r="F195" s="3"/>
       <c r="G195" s="3"/>
@@ -10284,13 +10290,13 @@
         <v>170</v>
       </c>
       <c r="C196" s="9" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="D196" s="9" t="s">
+        <v>505</v>
+      </c>
+      <c r="E196" s="3" t="s">
         <v>506</v>
-      </c>
-      <c r="E196" s="3" t="s">
-        <v>507</v>
       </c>
       <c r="F196" s="3"/>
       <c r="G196" s="3"/>
@@ -10303,10 +10309,10 @@
         <v>170</v>
       </c>
       <c r="C197" s="9" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="D197" s="9" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="E197" s="3" t="b">
         <v>1</v>
@@ -10322,10 +10328,10 @@
         <v>170</v>
       </c>
       <c r="C198" s="9" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="D198" s="9" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="E198" s="3" t="b">
         <v>0</v>
@@ -10341,13 +10347,13 @@
         <v>109</v>
       </c>
       <c r="C199" s="9" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="D199" s="9" t="s">
+        <v>509</v>
+      </c>
+      <c r="E199" s="3" t="s">
         <v>510</v>
-      </c>
-      <c r="E199" s="3" t="s">
-        <v>511</v>
       </c>
       <c r="F199" s="3"/>
       <c r="G199" s="3"/>
@@ -10360,10 +10366,10 @@
         <v>170</v>
       </c>
       <c r="C200" s="9" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="D200" s="9" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="E200" s="3"/>
       <c r="F200" s="3"/>
@@ -10377,10 +10383,10 @@
         <v>170</v>
       </c>
       <c r="C201" s="9" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="D201" s="9" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="E201" s="3"/>
       <c r="F201" s="3"/>
@@ -10394,10 +10400,10 @@
         <v>170</v>
       </c>
       <c r="C202" s="9" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="D202" s="9" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="E202" s="3"/>
       <c r="F202" s="3"/>
@@ -10411,10 +10417,10 @@
         <v>170</v>
       </c>
       <c r="C203" s="9" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="D203" s="9" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="E203" s="3" t="b">
         <v>1</v>
@@ -10430,10 +10436,10 @@
         <v>170</v>
       </c>
       <c r="C204" s="9" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="D204" s="9" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="E204" s="3" t="b">
         <v>0</v>
@@ -10449,10 +10455,10 @@
         <v>170</v>
       </c>
       <c r="C205" s="9" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="D205" s="9" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="E205" s="3" t="b">
         <v>0</v>
@@ -10468,10 +10474,10 @@
         <v>170</v>
       </c>
       <c r="C206" s="9" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="D206" s="9" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="E206" s="3" t="b">
         <v>1</v>
@@ -10487,13 +10493,13 @@
         <v>109</v>
       </c>
       <c r="C207" s="9" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="D207" s="9" t="s">
+        <v>518</v>
+      </c>
+      <c r="E207" s="3" t="s">
         <v>519</v>
-      </c>
-      <c r="E207" s="3" t="s">
-        <v>520</v>
       </c>
       <c r="F207" s="3"/>
       <c r="G207" s="3"/>
@@ -10506,13 +10512,13 @@
         <v>109</v>
       </c>
       <c r="C208" s="9" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="D208" s="9" t="s">
+        <v>520</v>
+      </c>
+      <c r="E208" s="3" t="s">
         <v>521</v>
-      </c>
-      <c r="E208" s="3" t="s">
-        <v>522</v>
       </c>
       <c r="F208" s="3"/>
       <c r="G208" s="3"/>
@@ -10525,10 +10531,10 @@
         <v>109</v>
       </c>
       <c r="C209" s="9" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="D209" s="9" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="E209" s="3">
         <v>0</v>
@@ -10544,10 +10550,10 @@
         <v>109</v>
       </c>
       <c r="C210" s="9" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="D210" s="9" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="E210" s="3">
         <v>1</v>
@@ -10563,10 +10569,10 @@
         <v>170</v>
       </c>
       <c r="C211" s="9" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="D211" s="9" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="E211" s="3" t="b">
         <v>0</v>
@@ -10582,10 +10588,10 @@
         <v>170</v>
       </c>
       <c r="C212" s="9" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="D212" s="9" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="E212" s="3" t="b">
         <v>1</v>
@@ -10601,10 +10607,10 @@
         <v>170</v>
       </c>
       <c r="C213" s="9" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="D213" s="9" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="E213" s="3" t="b">
         <v>1</v>
@@ -10620,10 +10626,10 @@
         <v>170</v>
       </c>
       <c r="C214" s="9" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="D214" s="9" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="E214" s="3" t="b">
         <v>0</v>
@@ -10639,13 +10645,13 @@
         <v>109</v>
       </c>
       <c r="C215" s="9" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="D215" s="9" t="s">
+        <v>528</v>
+      </c>
+      <c r="E215" s="3" t="s">
         <v>529</v>
-      </c>
-      <c r="E215" s="3" t="s">
-        <v>530</v>
       </c>
       <c r="F215" s="3"/>
       <c r="G215" s="3"/>
@@ -10658,10 +10664,10 @@
         <v>170</v>
       </c>
       <c r="C216" s="9" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="D216" s="9" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="E216" s="3"/>
       <c r="F216" s="3"/>
@@ -10675,10 +10681,10 @@
         <v>170</v>
       </c>
       <c r="C217" s="9" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="D217" s="9" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="E217" s="3"/>
       <c r="F217" s="3"/>
@@ -10692,10 +10698,10 @@
         <v>170</v>
       </c>
       <c r="C218" s="9" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="D218" s="9" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
       <c r="E218" s="3"/>
       <c r="F218" s="3"/>
@@ -10709,10 +10715,10 @@
         <v>170</v>
       </c>
       <c r="C219" s="9" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="D219" s="9" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
       <c r="E219" s="3" t="b">
         <v>1</v>
@@ -10728,10 +10734,10 @@
         <v>170</v>
       </c>
       <c r="C220" s="9" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="D220" s="9" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="E220" s="3" t="b">
         <v>0</v>
@@ -10747,10 +10753,10 @@
         <v>170</v>
       </c>
       <c r="C221" s="9" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="D221" s="9" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="E221" s="3" t="b">
         <v>0</v>
@@ -10766,10 +10772,10 @@
         <v>170</v>
       </c>
       <c r="C222" s="9" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="D222" s="9" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="E222" s="3" t="b">
         <v>1</v>
@@ -10785,13 +10791,13 @@
         <v>109</v>
       </c>
       <c r="C223" s="9" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="D223" s="9" t="s">
+        <v>537</v>
+      </c>
+      <c r="E223" s="3" t="s">
         <v>538</v>
-      </c>
-      <c r="E223" s="3" t="s">
-        <v>539</v>
       </c>
       <c r="F223" s="3"/>
       <c r="G223" s="3"/>
@@ -10804,13 +10810,13 @@
         <v>109</v>
       </c>
       <c r="C224" s="9" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="D224" s="9" t="s">
+        <v>539</v>
+      </c>
+      <c r="E224" s="3" t="s">
         <v>540</v>
-      </c>
-      <c r="E224" s="3" t="s">
-        <v>541</v>
       </c>
       <c r="F224" s="3"/>
       <c r="G224" s="3"/>
@@ -10823,10 +10829,10 @@
         <v>109</v>
       </c>
       <c r="C225" s="9" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="D225" s="9" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="E225" s="3">
         <v>0</v>
@@ -10842,10 +10848,10 @@
         <v>109</v>
       </c>
       <c r="C226" s="9" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="D226" s="9" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
       <c r="E226" s="3">
         <v>1</v>
@@ -10861,10 +10867,10 @@
         <v>170</v>
       </c>
       <c r="C227" s="9" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="D227" s="9" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="E227" s="3" t="b">
         <v>0</v>
@@ -10880,10 +10886,10 @@
         <v>170</v>
       </c>
       <c r="C228" s="9" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="D228" s="9" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="E228" s="3" t="b">
         <v>1</v>
@@ -10899,10 +10905,10 @@
         <v>170</v>
       </c>
       <c r="C229" s="9" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="D229" s="9" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="E229" s="3" t="b">
         <v>1</v>
@@ -10918,10 +10924,10 @@
         <v>170</v>
       </c>
       <c r="C230" s="9" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="D230" s="9" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="E230" s="3" t="b">
         <v>0</v>

</xml_diff>

<commit_message>
Correct casing issue with boolean values read from xlsx
</commit_message>
<xml_diff>
--- a/src/test/resources/SBAC-IAB-FIXED-G11M-Winter-2017-2018.xlsx
+++ b/src/test/resources/SBAC-IAB-FIXED-G11M-Winter-2017-2018.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10715"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gstoike\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jeffjohnson/dev/sbac/git/tds/repositories/TDS_FixedFormPackager/src/test/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{3B509A98-1BCB-43FF-B4B8-AF49BF9B13CF}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE29AC85-BCDA-454E-9BE0-C42D4BF70D28}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13425" tabRatio="644" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="34400" windowHeight="28360" tabRatio="644" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Package" sheetId="16" r:id="rId1"/>
@@ -2965,17 +2965,17 @@
       <selection pane="bottomRight" activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="11" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="53.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="30.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="20.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="9.140625" style="2"/>
+    <col min="1" max="1" width="53.83203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.1640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="30.83203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.1640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="9.1640625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="25" t="s">
         <v>184</v>
       </c>
@@ -2988,7 +2988,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A2" s="7" t="s">
         <v>185</v>
       </c>
@@ -3005,7 +3005,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A3" s="9" t="s">
         <v>111</v>
       </c>
@@ -3022,7 +3022,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="18" t="s">
         <v>145</v>
       </c>
@@ -3039,7 +3039,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="18" t="s">
         <v>146</v>
       </c>
@@ -3056,7 +3056,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="9" t="s">
         <v>147</v>
       </c>
@@ -3073,7 +3073,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A7" s="9" t="s">
         <v>114</v>
       </c>
@@ -3090,7 +3090,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A8" s="9" t="s">
         <v>115</v>
       </c>
@@ -3107,7 +3107,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A9" s="9" t="s">
         <v>116</v>
       </c>
@@ -3124,7 +3124,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A10" s="9" t="s">
         <v>117</v>
       </c>
@@ -3141,7 +3141,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A11" s="9" t="s">
         <v>110</v>
       </c>
@@ -3158,7 +3158,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A12" s="9" t="s">
         <v>112</v>
       </c>
@@ -3175,7 +3175,7 @@
         <v>2280</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A13" s="9" t="s">
         <v>113</v>
       </c>
@@ -3192,7 +3192,7 @@
         <v>2543</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A14" s="9" t="s">
         <v>113</v>
       </c>
@@ -3209,7 +3209,7 @@
         <v>2628</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A15" s="9" t="s">
         <v>113</v>
       </c>
@@ -3226,7 +3226,7 @@
         <v>2718</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A16" s="9" t="s">
         <v>113</v>
       </c>
@@ -3263,18 +3263,18 @@
       <selection pane="bottomRight" activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="55" defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="55" defaultRowHeight="11" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="61.28515625" style="14" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.140625" style="14" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="26.140625" style="14" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="26.85546875" style="14" bestFit="1" customWidth="1"/>
-    <col min="5" max="8" width="20.140625" style="15" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="20.28515625" style="15" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="61.33203125" style="14" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.1640625" style="14" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="26.1640625" style="14" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="26.83203125" style="14" bestFit="1" customWidth="1"/>
+    <col min="5" max="8" width="20.1640625" style="15" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="20.33203125" style="15" bestFit="1" customWidth="1"/>
     <col min="10" max="16384" width="55" style="14"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A1" s="25" t="s">
         <v>184</v>
       </c>
@@ -3289,7 +3289,7 @@
       <c r="H1" s="26"/>
       <c r="I1" s="26"/>
     </row>
-    <row r="2" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" ht="12" x14ac:dyDescent="0.15">
       <c r="A2" s="7" t="s">
         <v>185</v>
       </c>
@@ -3318,7 +3318,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9" ht="12" x14ac:dyDescent="0.15">
       <c r="A3" s="17" t="s">
         <v>577</v>
       </c>
@@ -3347,7 +3347,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9" ht="12" x14ac:dyDescent="0.15">
       <c r="A4" s="17" t="s">
         <v>578</v>
       </c>
@@ -3376,7 +3376,7 @@
         <v>576</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9" ht="12" x14ac:dyDescent="0.15">
       <c r="A5" s="17" t="s">
         <v>127</v>
       </c>
@@ -3405,7 +3405,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="22.5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:9" ht="12" x14ac:dyDescent="0.15">
       <c r="A6" s="17" t="s">
         <v>126</v>
       </c>
@@ -3434,7 +3434,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:9" ht="12" x14ac:dyDescent="0.15">
       <c r="A7" s="17" t="s">
         <v>166</v>
       </c>
@@ -3461,7 +3461,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:9" ht="12" x14ac:dyDescent="0.15">
       <c r="A8" s="17" t="s">
         <v>129</v>
       </c>
@@ -3486,7 +3486,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:9" ht="12" x14ac:dyDescent="0.15">
       <c r="A9" s="17" t="s">
         <v>128</v>
       </c>
@@ -3511,7 +3511,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:9" ht="12" x14ac:dyDescent="0.15">
       <c r="A10" s="17" t="s">
         <v>131</v>
       </c>
@@ -3532,7 +3532,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:9" ht="12" x14ac:dyDescent="0.15">
       <c r="A11" s="17" t="s">
         <v>132</v>
       </c>
@@ -3553,7 +3553,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="12" spans="1:9" ht="22.5" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:9" ht="12" x14ac:dyDescent="0.15">
       <c r="A12" s="17" t="s">
         <v>133</v>
       </c>
@@ -3574,7 +3574,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="13" spans="1:9" ht="22.5" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:9" ht="12" x14ac:dyDescent="0.15">
       <c r="A13" s="17" t="s">
         <v>130</v>
       </c>
@@ -3599,7 +3599,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="14" spans="1:9" ht="22.5" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:9" ht="12" x14ac:dyDescent="0.15">
       <c r="A14" s="17" t="s">
         <v>133</v>
       </c>
@@ -3618,7 +3618,7 @@
       <c r="H14" s="16"/>
       <c r="I14" s="16"/>
     </row>
-    <row r="15" spans="1:9" ht="22.5" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:9" ht="12" x14ac:dyDescent="0.15">
       <c r="A15" s="17" t="s">
         <v>130</v>
       </c>
@@ -3637,7 +3637,7 @@
       <c r="H15" s="16"/>
       <c r="I15" s="16"/>
     </row>
-    <row r="16" spans="1:9" ht="22.5" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:9" ht="12" x14ac:dyDescent="0.15">
       <c r="A16" s="17" t="s">
         <v>133</v>
       </c>
@@ -3656,7 +3656,7 @@
       <c r="H16" s="16"/>
       <c r="I16" s="16"/>
     </row>
-    <row r="17" spans="1:9" ht="22.5" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:9" ht="12" x14ac:dyDescent="0.15">
       <c r="A17" s="17" t="s">
         <v>130</v>
       </c>
@@ -3675,7 +3675,7 @@
       <c r="H17" s="16"/>
       <c r="I17" s="16"/>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:9" ht="12" x14ac:dyDescent="0.15">
       <c r="A18" s="17" t="s">
         <v>129</v>
       </c>
@@ -3698,7 +3698,7 @@
       </c>
       <c r="I18" s="16"/>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:9" ht="12" x14ac:dyDescent="0.15">
       <c r="A19" s="17" t="s">
         <v>128</v>
       </c>
@@ -3721,7 +3721,7 @@
       </c>
       <c r="I19" s="16"/>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:9" ht="12" x14ac:dyDescent="0.15">
       <c r="A20" s="9" t="s">
         <v>131</v>
       </c>
@@ -3740,7 +3740,7 @@
       <c r="H20" s="16"/>
       <c r="I20" s="16"/>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:9" ht="12" x14ac:dyDescent="0.15">
       <c r="A21" s="9" t="s">
         <v>132</v>
       </c>
@@ -3759,7 +3759,7 @@
       <c r="H21" s="16"/>
       <c r="I21" s="16"/>
     </row>
-    <row r="22" spans="1:9" ht="22.5" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:9" ht="12" x14ac:dyDescent="0.15">
       <c r="A22" s="9" t="s">
         <v>133</v>
       </c>
@@ -3778,7 +3778,7 @@
       <c r="H22" s="16"/>
       <c r="I22" s="16"/>
     </row>
-    <row r="23" spans="1:9" ht="22.5" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:9" ht="12" x14ac:dyDescent="0.15">
       <c r="A23" s="9" t="s">
         <v>130</v>
       </c>
@@ -3801,7 +3801,7 @@
       </c>
       <c r="I23" s="16"/>
     </row>
-    <row r="24" spans="1:9" ht="22.5" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:9" ht="12" x14ac:dyDescent="0.15">
       <c r="A24" s="9" t="s">
         <v>133</v>
       </c>
@@ -3820,7 +3820,7 @@
       <c r="H24" s="16"/>
       <c r="I24" s="16"/>
     </row>
-    <row r="25" spans="1:9" ht="22.5" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:9" ht="12" x14ac:dyDescent="0.15">
       <c r="A25" s="9" t="s">
         <v>130</v>
       </c>
@@ -3839,7 +3839,7 @@
       <c r="H25" s="16"/>
       <c r="I25" s="16"/>
     </row>
-    <row r="26" spans="1:9" ht="22.5" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:9" ht="12" x14ac:dyDescent="0.15">
       <c r="A26" s="9" t="s">
         <v>133</v>
       </c>
@@ -3858,7 +3858,7 @@
       <c r="H26" s="16"/>
       <c r="I26" s="16"/>
     </row>
-    <row r="27" spans="1:9" ht="22.5" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:9" ht="12" x14ac:dyDescent="0.15">
       <c r="A27" s="9" t="s">
         <v>130</v>
       </c>
@@ -3877,7 +3877,7 @@
       <c r="H27" s="16"/>
       <c r="I27" s="16"/>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:9" ht="12" x14ac:dyDescent="0.15">
       <c r="A28" s="9" t="s">
         <v>129</v>
       </c>
@@ -3900,7 +3900,7 @@
       </c>
       <c r="I28" s="16"/>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:9" ht="12" x14ac:dyDescent="0.15">
       <c r="A29" s="9" t="s">
         <v>128</v>
       </c>
@@ -3923,7 +3923,7 @@
       </c>
       <c r="I29" s="16"/>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:9" ht="12" x14ac:dyDescent="0.15">
       <c r="A30" s="9" t="s">
         <v>131</v>
       </c>
@@ -3942,7 +3942,7 @@
       <c r="H30" s="16"/>
       <c r="I30" s="16"/>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:9" ht="12" x14ac:dyDescent="0.15">
       <c r="A31" s="9" t="s">
         <v>132</v>
       </c>
@@ -3961,7 +3961,7 @@
       <c r="H31" s="16"/>
       <c r="I31" s="16"/>
     </row>
-    <row r="32" spans="1:9" ht="22.5" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:9" ht="12" x14ac:dyDescent="0.15">
       <c r="A32" s="9" t="s">
         <v>133</v>
       </c>
@@ -3980,7 +3980,7 @@
       <c r="H32" s="16"/>
       <c r="I32" s="16"/>
     </row>
-    <row r="33" spans="1:9" ht="22.5" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:9" ht="12" x14ac:dyDescent="0.15">
       <c r="A33" s="9" t="s">
         <v>130</v>
       </c>
@@ -4003,7 +4003,7 @@
       </c>
       <c r="I33" s="16"/>
     </row>
-    <row r="34" spans="1:9" ht="22.5" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:9" ht="12" x14ac:dyDescent="0.15">
       <c r="A34" s="9" t="s">
         <v>133</v>
       </c>
@@ -4022,7 +4022,7 @@
       <c r="H34" s="16"/>
       <c r="I34" s="16"/>
     </row>
-    <row r="35" spans="1:9" ht="22.5" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:9" ht="12" x14ac:dyDescent="0.15">
       <c r="A35" s="9" t="s">
         <v>130</v>
       </c>
@@ -4041,7 +4041,7 @@
       <c r="H35" s="16"/>
       <c r="I35" s="16"/>
     </row>
-    <row r="36" spans="1:9" ht="22.5" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:9" ht="12" x14ac:dyDescent="0.15">
       <c r="A36" s="9" t="s">
         <v>133</v>
       </c>
@@ -4060,7 +4060,7 @@
       <c r="H36" s="16"/>
       <c r="I36" s="16"/>
     </row>
-    <row r="37" spans="1:9" ht="22.5" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:9" ht="12" x14ac:dyDescent="0.15">
       <c r="A37" s="9" t="s">
         <v>130</v>
       </c>
@@ -4079,7 +4079,7 @@
       <c r="H37" s="16"/>
       <c r="I37" s="16"/>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:9" ht="12" x14ac:dyDescent="0.15">
       <c r="A38" s="9" t="s">
         <v>129</v>
       </c>
@@ -4100,7 +4100,7 @@
       </c>
       <c r="I38" s="16"/>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:9" ht="12" x14ac:dyDescent="0.15">
       <c r="A39" s="9" t="s">
         <v>128</v>
       </c>
@@ -4121,7 +4121,7 @@
       </c>
       <c r="I39" s="16"/>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:9" ht="12" x14ac:dyDescent="0.15">
       <c r="A40" s="9" t="s">
         <v>131</v>
       </c>
@@ -4140,7 +4140,7 @@
       <c r="H40" s="16"/>
       <c r="I40" s="16"/>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:9" ht="12" x14ac:dyDescent="0.15">
       <c r="A41" s="9" t="s">
         <v>132</v>
       </c>
@@ -4159,7 +4159,7 @@
       <c r="H41" s="16"/>
       <c r="I41" s="16"/>
     </row>
-    <row r="42" spans="1:9" ht="22.5" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:9" ht="12" x14ac:dyDescent="0.15">
       <c r="A42" s="9" t="s">
         <v>133</v>
       </c>
@@ -4178,7 +4178,7 @@
       <c r="H42" s="16"/>
       <c r="I42" s="16"/>
     </row>
-    <row r="43" spans="1:9" ht="22.5" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:9" ht="12" x14ac:dyDescent="0.15">
       <c r="A43" s="9" t="s">
         <v>130</v>
       </c>
@@ -4199,7 +4199,7 @@
       </c>
       <c r="I43" s="16"/>
     </row>
-    <row r="44" spans="1:9" ht="22.5" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:9" ht="12" x14ac:dyDescent="0.15">
       <c r="A44" s="9" t="s">
         <v>133</v>
       </c>
@@ -4218,7 +4218,7 @@
       <c r="H44" s="16"/>
       <c r="I44" s="16"/>
     </row>
-    <row r="45" spans="1:9" ht="22.5" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:9" ht="12" x14ac:dyDescent="0.15">
       <c r="A45" s="9" t="s">
         <v>130</v>
       </c>
@@ -4237,7 +4237,7 @@
       <c r="H45" s="16"/>
       <c r="I45" s="16"/>
     </row>
-    <row r="46" spans="1:9" ht="22.5" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:9" ht="12" x14ac:dyDescent="0.15">
       <c r="A46" s="9" t="s">
         <v>133</v>
       </c>
@@ -4256,7 +4256,7 @@
       <c r="H46" s="16"/>
       <c r="I46" s="16"/>
     </row>
-    <row r="47" spans="1:9" ht="22.5" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:9" ht="12" x14ac:dyDescent="0.15">
       <c r="A47" s="9" t="s">
         <v>130</v>
       </c>
@@ -4275,14 +4275,14 @@
       <c r="H47" s="16"/>
       <c r="I47" s="16"/>
     </row>
-    <row r="49" spans="1:1" ht="12" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="50" spans="1:1" ht="54" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:1" ht="12" thickBot="1" x14ac:dyDescent="0.2"/>
+    <row r="50" spans="1:1" ht="63" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A50" s="22" t="s">
         <v>301</v>
       </c>
     </row>
   </sheetData>
-  <sortState columnSort="1" ref="E1:I50">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" columnSort="1" ref="E1:I50">
     <sortCondition ref="E3:I3"/>
     <sortCondition ref="E5:I5"/>
   </sortState>
@@ -4307,17 +4307,17 @@
       <selection pane="bottomRight" activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="11" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="16.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="41.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="33.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="9.140625" style="2"/>
+    <col min="1" max="1" width="16.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.1640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="41.5" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.5" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="33.1640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="9.1640625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A1" s="25" t="s">
         <v>184</v>
       </c>
@@ -4330,7 +4330,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A2" s="7" t="s">
         <v>185</v>
       </c>
@@ -4347,7 +4347,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A3" s="9" t="s">
         <v>149</v>
       </c>
@@ -4364,7 +4364,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A4" s="9" t="s">
         <v>148</v>
       </c>
@@ -4402,18 +4402,18 @@
       <selection pane="bottomRight" activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="38.140625" defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="38.1640625" defaultRowHeight="11" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="79.42578125" style="11" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.140625" style="11" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="36.140625" style="11" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="21.42578125" style="11" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="54.7109375" style="11" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="52.7109375" style="11" bestFit="1" customWidth="1"/>
-    <col min="7" max="16384" width="38.140625" style="11"/>
+    <col min="1" max="1" width="79.5" style="11" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.1640625" style="11" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="36.1640625" style="11" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.5" style="11" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="54.6640625" style="11" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="52.6640625" style="11" bestFit="1" customWidth="1"/>
+    <col min="7" max="16384" width="38.1640625" style="11"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A1" s="25" t="s">
         <v>184</v>
       </c>
@@ -4427,7 +4427,7 @@
       </c>
       <c r="F1" s="25"/>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A2" s="7" t="s">
         <v>185</v>
       </c>
@@ -4447,7 +4447,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="3" spans="1:6" s="2" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" s="2" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="9" t="s">
         <v>120</v>
       </c>
@@ -4467,7 +4467,7 @@
         <v>583</v>
       </c>
     </row>
-    <row r="4" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A4" s="9" t="s">
         <v>149</v>
       </c>
@@ -4487,7 +4487,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="5" spans="1:6" s="2" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" s="2" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="9" t="s">
         <v>119</v>
       </c>
@@ -4507,7 +4507,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:6" s="2" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" s="2" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="18" t="s">
         <v>142</v>
       </c>
@@ -4527,7 +4527,7 @@
         <v>584</v>
       </c>
     </row>
-    <row r="7" spans="1:6" s="2" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6" s="2" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="18" t="s">
         <v>143</v>
       </c>
@@ -4547,7 +4547,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:6" s="2" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6" s="2" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="18" t="s">
         <v>144</v>
       </c>
@@ -4567,7 +4567,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:6" s="2" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:6" s="2" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="9" t="s">
         <v>164</v>
       </c>
@@ -4587,7 +4587,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:6" s="2" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:6" s="2" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="9" t="s">
         <v>164</v>
       </c>
@@ -4607,7 +4607,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:6" s="2" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:6" s="2" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="9" t="s">
         <v>164</v>
       </c>
@@ -4627,7 +4627,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:6" s="2" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:6" s="2" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="9" t="s">
         <v>165</v>
       </c>
@@ -4647,7 +4647,7 @@
         <v>79.3</v>
       </c>
     </row>
-    <row r="13" spans="1:6" s="2" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:6" s="2" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="9" t="s">
         <v>165</v>
       </c>
@@ -4682,23 +4682,23 @@
   <dimension ref="A1:S56"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="4" ySplit="2" topLeftCell="L3" activePane="bottomRight" state="frozenSplit"/>
+      <pane xSplit="4" ySplit="2" topLeftCell="E3" activePane="bottomRight" state="frozenSplit"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="R24" sqref="R24"/>
+      <selection pane="bottomRight" activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="32.85546875" defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="32.83203125" defaultRowHeight="11" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="55" style="21" customWidth="1"/>
-    <col min="2" max="2" width="7.140625" style="21" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="41.85546875" style="21" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.42578125" style="21" bestFit="1" customWidth="1"/>
-    <col min="5" max="19" width="17.42578125" style="21" customWidth="1"/>
-    <col min="20" max="16384" width="32.85546875" style="21"/>
+    <col min="2" max="2" width="7.1640625" style="21" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="41.83203125" style="21" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.5" style="21" bestFit="1" customWidth="1"/>
+    <col min="5" max="19" width="17.5" style="21" customWidth="1"/>
+    <col min="20" max="16384" width="32.83203125" style="21"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A1" s="25" t="s">
         <v>184</v>
       </c>
@@ -4727,7 +4727,7 @@
       <c r="R1" s="31"/>
       <c r="S1" s="32"/>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A2" s="7" t="s">
         <v>185</v>
       </c>
@@ -4786,7 +4786,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="3" spans="1:19" ht="33.75" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:19" ht="36" x14ac:dyDescent="0.15">
       <c r="A3" s="9" t="s">
         <v>120</v>
       </c>
@@ -4845,7 +4845,7 @@
         <v>583</v>
       </c>
     </row>
-    <row r="4" spans="1:19" ht="22.5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:19" ht="24" x14ac:dyDescent="0.15">
       <c r="A4" s="9" t="s">
         <v>248</v>
       </c>
@@ -4904,7 +4904,7 @@
         <v>587</v>
       </c>
     </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:19" ht="12" x14ac:dyDescent="0.15">
       <c r="A5" s="9" t="s">
         <v>250</v>
       </c>
@@ -4963,7 +4963,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A6" s="9"/>
       <c r="B6" s="9" t="s">
         <v>109</v>
@@ -5020,7 +5020,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A7" s="9" t="s">
         <v>169</v>
       </c>
@@ -5079,7 +5079,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A8" s="9" t="s">
         <v>118</v>
       </c>
@@ -5138,7 +5138,7 @@
         <v>30309</v>
       </c>
     </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A9" s="9" t="s">
         <v>253</v>
       </c>
@@ -5197,7 +5197,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A10" s="9" t="s">
         <v>253</v>
       </c>
@@ -5256,7 +5256,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A11" s="9" t="s">
         <v>253</v>
       </c>
@@ -5315,7 +5315,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A12" s="9" t="s">
         <v>536</v>
       </c>
@@ -5328,7 +5328,9 @@
       <c r="D12" s="9" t="s">
         <v>537</v>
       </c>
-      <c r="E12" s="1"/>
+      <c r="E12" s="1" t="b">
+        <v>1</v>
+      </c>
       <c r="F12" s="1"/>
       <c r="G12" s="1"/>
       <c r="H12" s="1"/>
@@ -5344,7 +5346,7 @@
       <c r="R12" s="1"/>
       <c r="S12" s="1"/>
     </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A13" s="18" t="s">
         <v>141</v>
       </c>
@@ -5357,7 +5359,9 @@
       <c r="D13" s="9" t="s">
         <v>171</v>
       </c>
-      <c r="E13" s="4"/>
+      <c r="E13" s="4" t="b">
+        <v>1</v>
+      </c>
       <c r="F13" s="4"/>
       <c r="G13" s="4"/>
       <c r="H13" s="4"/>
@@ -5373,7 +5377,7 @@
       <c r="R13" s="4"/>
       <c r="S13" s="4"/>
     </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A14" s="18" t="s">
         <v>140</v>
       </c>
@@ -5400,7 +5404,7 @@
       <c r="R14" s="4"/>
       <c r="S14" s="4"/>
     </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A15" s="18" t="s">
         <v>134</v>
       </c>
@@ -5427,7 +5431,7 @@
       <c r="R15" s="4"/>
       <c r="S15" s="4"/>
     </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A16" s="18" t="s">
         <v>135</v>
       </c>
@@ -5454,7 +5458,7 @@
       <c r="R16" s="4"/>
       <c r="S16" s="4"/>
     </row>
-    <row r="17" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A17" s="18" t="s">
         <v>136</v>
       </c>
@@ -5481,7 +5485,7 @@
       <c r="R17" s="4"/>
       <c r="S17" s="4"/>
     </row>
-    <row r="18" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A18" s="18" t="s">
         <v>137</v>
       </c>
@@ -5508,7 +5512,7 @@
       <c r="R18" s="4"/>
       <c r="S18" s="4"/>
     </row>
-    <row r="19" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A19" s="18" t="s">
         <v>138</v>
       </c>
@@ -5535,7 +5539,7 @@
       <c r="R19" s="4"/>
       <c r="S19" s="4"/>
     </row>
-    <row r="20" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A20" s="18" t="s">
         <v>139</v>
       </c>
@@ -5562,7 +5566,7 @@
       <c r="R20" s="4"/>
       <c r="S20" s="4"/>
     </row>
-    <row r="21" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A21" s="9" t="s">
         <v>121</v>
       </c>
@@ -5589,7 +5593,7 @@
       <c r="R21" s="1"/>
       <c r="S21" s="1"/>
     </row>
-    <row r="22" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A22" s="9" t="s">
         <v>122</v>
       </c>
@@ -5616,7 +5620,7 @@
       <c r="R22" s="1"/>
       <c r="S22" s="1"/>
     </row>
-    <row r="23" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A23" s="9" t="s">
         <v>123</v>
       </c>
@@ -5643,7 +5647,7 @@
       <c r="R23" s="1"/>
       <c r="S23" s="1"/>
     </row>
-    <row r="24" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A24" s="9" t="s">
         <v>124</v>
       </c>
@@ -5670,7 +5674,7 @@
       <c r="R24" s="4"/>
       <c r="S24" s="4"/>
     </row>
-    <row r="25" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A25" s="9" t="s">
         <v>125</v>
       </c>
@@ -5697,7 +5701,7 @@
       <c r="R25" s="4"/>
       <c r="S25" s="4"/>
     </row>
-    <row r="26" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A26" s="9" t="s">
         <v>125</v>
       </c>
@@ -5724,7 +5728,7 @@
       <c r="R26" s="4"/>
       <c r="S26" s="4"/>
     </row>
-    <row r="27" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A27" s="9" t="s">
         <v>125</v>
       </c>
@@ -5751,7 +5755,7 @@
       <c r="R27" s="4"/>
       <c r="S27" s="4"/>
     </row>
-    <row r="28" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A28" s="9" t="s">
         <v>125</v>
       </c>
@@ -5778,7 +5782,7 @@
       <c r="R28" s="4"/>
       <c r="S28" s="4"/>
     </row>
-    <row r="29" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A29" s="9" t="s">
         <v>125</v>
       </c>
@@ -5805,7 +5809,7 @@
       <c r="R29" s="4"/>
       <c r="S29" s="4"/>
     </row>
-    <row r="30" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A30" s="9" t="s">
         <v>125</v>
       </c>
@@ -5832,7 +5836,7 @@
       <c r="R30" s="4"/>
       <c r="S30" s="4"/>
     </row>
-    <row r="31" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A31" s="9" t="s">
         <v>125</v>
       </c>
@@ -5859,7 +5863,7 @@
       <c r="R31" s="4"/>
       <c r="S31" s="4"/>
     </row>
-    <row r="32" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A32" s="9" t="s">
         <v>125</v>
       </c>
@@ -5886,7 +5890,7 @@
       <c r="R32" s="4"/>
       <c r="S32" s="4"/>
     </row>
-    <row r="33" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A33" s="9" t="s">
         <v>121</v>
       </c>
@@ -5913,7 +5917,7 @@
       <c r="R33" s="1"/>
       <c r="S33" s="1"/>
     </row>
-    <row r="34" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A34" s="9" t="s">
         <v>122</v>
       </c>
@@ -5940,7 +5944,7 @@
       <c r="R34" s="1"/>
       <c r="S34" s="1"/>
     </row>
-    <row r="35" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A35" s="9" t="s">
         <v>123</v>
       </c>
@@ -5967,7 +5971,7 @@
       <c r="R35" s="1"/>
       <c r="S35" s="1"/>
     </row>
-    <row r="36" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A36" s="9" t="s">
         <v>124</v>
       </c>
@@ -5994,7 +5998,7 @@
       <c r="R36" s="4"/>
       <c r="S36" s="4"/>
     </row>
-    <row r="37" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A37" s="9" t="s">
         <v>125</v>
       </c>
@@ -6021,7 +6025,7 @@
       <c r="R37" s="4"/>
       <c r="S37" s="4"/>
     </row>
-    <row r="38" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A38" s="9" t="s">
         <v>125</v>
       </c>
@@ -6048,7 +6052,7 @@
       <c r="R38" s="4"/>
       <c r="S38" s="4"/>
     </row>
-    <row r="39" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A39" s="9" t="s">
         <v>125</v>
       </c>
@@ -6075,7 +6079,7 @@
       <c r="R39" s="4"/>
       <c r="S39" s="4"/>
     </row>
-    <row r="40" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A40" s="9" t="s">
         <v>125</v>
       </c>
@@ -6102,7 +6106,7 @@
       <c r="R40" s="4"/>
       <c r="S40" s="4"/>
     </row>
-    <row r="41" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A41" s="9" t="s">
         <v>125</v>
       </c>
@@ -6129,7 +6133,7 @@
       <c r="R41" s="4"/>
       <c r="S41" s="4"/>
     </row>
-    <row r="42" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A42" s="9" t="s">
         <v>125</v>
       </c>
@@ -6156,7 +6160,7 @@
       <c r="R42" s="4"/>
       <c r="S42" s="4"/>
     </row>
-    <row r="43" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A43" s="9" t="s">
         <v>125</v>
       </c>
@@ -6183,7 +6187,7 @@
       <c r="R43" s="4"/>
       <c r="S43" s="4"/>
     </row>
-    <row r="44" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A44" s="9" t="s">
         <v>125</v>
       </c>
@@ -6210,7 +6214,7 @@
       <c r="R44" s="4"/>
       <c r="S44" s="4"/>
     </row>
-    <row r="45" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A45" s="9" t="s">
         <v>121</v>
       </c>
@@ -6237,7 +6241,7 @@
       <c r="R45" s="1"/>
       <c r="S45" s="1"/>
     </row>
-    <row r="46" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A46" s="9" t="s">
         <v>122</v>
       </c>
@@ -6264,7 +6268,7 @@
       <c r="R46" s="1"/>
       <c r="S46" s="1"/>
     </row>
-    <row r="47" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A47" s="9" t="s">
         <v>123</v>
       </c>
@@ -6291,7 +6295,7 @@
       <c r="R47" s="1"/>
       <c r="S47" s="1"/>
     </row>
-    <row r="48" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A48" s="9" t="s">
         <v>124</v>
       </c>
@@ -6318,7 +6322,7 @@
       <c r="R48" s="4"/>
       <c r="S48" s="4"/>
     </row>
-    <row r="49" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A49" s="9" t="s">
         <v>125</v>
       </c>
@@ -6345,7 +6349,7 @@
       <c r="R49" s="4"/>
       <c r="S49" s="4"/>
     </row>
-    <row r="50" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A50" s="9" t="s">
         <v>125</v>
       </c>
@@ -6372,7 +6376,7 @@
       <c r="R50" s="4"/>
       <c r="S50" s="4"/>
     </row>
-    <row r="51" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A51" s="9" t="s">
         <v>125</v>
       </c>
@@ -6399,7 +6403,7 @@
       <c r="R51" s="4"/>
       <c r="S51" s="4"/>
     </row>
-    <row r="52" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A52" s="9" t="s">
         <v>125</v>
       </c>
@@ -6426,7 +6430,7 @@
       <c r="R52" s="4"/>
       <c r="S52" s="4"/>
     </row>
-    <row r="53" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A53" s="9" t="s">
         <v>125</v>
       </c>
@@ -6453,7 +6457,7 @@
       <c r="R53" s="4"/>
       <c r="S53" s="4"/>
     </row>
-    <row r="54" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A54" s="9" t="s">
         <v>125</v>
       </c>
@@ -6480,7 +6484,7 @@
       <c r="R54" s="4"/>
       <c r="S54" s="4"/>
     </row>
-    <row r="55" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A55" s="9" t="s">
         <v>125</v>
       </c>
@@ -6507,7 +6511,7 @@
       <c r="R55" s="4"/>
       <c r="S55" s="4"/>
     </row>
-    <row r="56" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A56" s="9" t="s">
         <v>125</v>
       </c>
@@ -6557,18 +6561,18 @@
       <selection pane="bottomRight" activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="49.85546875" defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="49.83203125" defaultRowHeight="11" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="59" style="11" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.140625" style="11" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.1640625" style="11" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="46" style="11" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="26.42578125" style="11" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="38.28515625" style="11" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="39.42578125" style="11" bestFit="1" customWidth="1"/>
-    <col min="8" max="16384" width="49.85546875" style="11"/>
+    <col min="4" max="4" width="26.5" style="11" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="38.33203125" style="11" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="39.5" style="11" bestFit="1" customWidth="1"/>
+    <col min="8" max="16384" width="49.83203125" style="11"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A1" s="25" t="s">
         <v>184</v>
       </c>
@@ -6587,7 +6591,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A2" s="7" t="s">
         <v>185</v>
       </c>
@@ -6610,7 +6614,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="3" spans="1:9" s="2" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9" s="2" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="9" t="s">
         <v>120</v>
       </c>
@@ -6633,7 +6637,7 @@
         <v>583</v>
       </c>
     </row>
-    <row r="4" spans="1:9" s="2" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9" s="2" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="18" t="s">
         <v>154</v>
       </c>
@@ -6654,7 +6658,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="5" spans="1:9" s="2" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9" s="2" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="18" t="s">
         <v>150</v>
       </c>
@@ -6671,7 +6675,7 @@
       <c r="F5" s="3"/>
       <c r="G5" s="3"/>
     </row>
-    <row r="6" spans="1:9" s="2" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:9" s="2" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="18" t="s">
         <v>151</v>
       </c>
@@ -6688,7 +6692,7 @@
       <c r="F6" s="3"/>
       <c r="G6" s="3"/>
     </row>
-    <row r="7" spans="1:9" s="2" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:9" s="2" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="18" t="s">
         <v>152</v>
       </c>
@@ -6707,7 +6711,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:9" s="2" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:9" s="2" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="18" t="s">
         <v>153</v>
       </c>
@@ -6728,7 +6732,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:9" s="2" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:9" s="2" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="18" t="s">
         <v>155</v>
       </c>
@@ -6749,7 +6753,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:9" s="2" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:9" s="2" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="18" t="s">
         <v>156</v>
       </c>
@@ -6770,7 +6774,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:9" s="2" customFormat="1" ht="12" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" s="2" customFormat="1" ht="12" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A11" s="18" t="s">
         <v>157</v>
       </c>
@@ -6791,7 +6795,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A12" s="18" t="s">
         <v>161</v>
       </c>
@@ -6814,7 +6818,7 @@
       <c r="H12" s="23"/>
       <c r="I12" s="24"/>
     </row>
-    <row r="13" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A13" s="18" t="s">
         <v>161</v>
       </c>
@@ -6837,7 +6841,7 @@
       <c r="H13" s="23"/>
       <c r="I13" s="24"/>
     </row>
-    <row r="14" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A14" s="18" t="s">
         <v>161</v>
       </c>
@@ -6858,7 +6862,7 @@
       <c r="H14" s="23"/>
       <c r="I14" s="24"/>
     </row>
-    <row r="15" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A15" s="18" t="s">
         <v>161</v>
       </c>
@@ -6879,7 +6883,7 @@
       <c r="H15" s="23"/>
       <c r="I15" s="24"/>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A16" s="18" t="s">
         <v>158</v>
       </c>
@@ -6900,7 +6904,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A17" s="18" t="s">
         <v>158</v>
       </c>
@@ -6921,7 +6925,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A18" s="18" t="s">
         <v>158</v>
       </c>
@@ -6940,7 +6944,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A19" s="18" t="s">
         <v>158</v>
       </c>
@@ -6959,7 +6963,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:7" ht="12" x14ac:dyDescent="0.15">
       <c r="A20" s="18" t="s">
         <v>159</v>
       </c>
@@ -6980,7 +6984,7 @@
         <v>325</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:7" ht="12" x14ac:dyDescent="0.15">
       <c r="A21" s="18" t="s">
         <v>159</v>
       </c>
@@ -7001,7 +7005,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:7" ht="12" x14ac:dyDescent="0.15">
       <c r="A22" s="18" t="s">
         <v>159</v>
       </c>
@@ -7020,7 +7024,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:7" ht="12" x14ac:dyDescent="0.15">
       <c r="A23" s="18" t="s">
         <v>159</v>
       </c>
@@ -7039,7 +7043,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A24" s="18" t="s">
         <v>160</v>
       </c>
@@ -7060,7 +7064,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A25" s="18" t="s">
         <v>160</v>
       </c>
@@ -7081,7 +7085,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A26" s="18" t="s">
         <v>160</v>
       </c>
@@ -7100,7 +7104,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A27" s="18" t="s">
         <v>160</v>
       </c>
@@ -7119,7 +7123,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:7" s="2" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:7" s="2" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A28" s="18" t="s">
         <v>162</v>
       </c>
@@ -7138,7 +7142,7 @@
       <c r="F28" s="3"/>
       <c r="G28" s="3"/>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:7" ht="12" x14ac:dyDescent="0.15">
       <c r="A29" s="18" t="s">
         <v>163</v>
       </c>
@@ -7157,7 +7161,7 @@
       <c r="F29" s="3"/>
       <c r="G29" s="3"/>
     </row>
-    <row r="30" spans="1:7" s="2" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:7" s="2" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A30" s="18" t="s">
         <v>217</v>
       </c>
@@ -7176,7 +7180,7 @@
       <c r="F30" s="3"/>
       <c r="G30" s="3"/>
     </row>
-    <row r="31" spans="1:7" s="2" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:7" s="2" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A31" s="18" t="s">
         <v>162</v>
       </c>
@@ -7195,7 +7199,7 @@
       <c r="F31" s="3"/>
       <c r="G31" s="3"/>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:7" ht="12" x14ac:dyDescent="0.15">
       <c r="A32" s="18" t="s">
         <v>163</v>
       </c>
@@ -7214,7 +7218,7 @@
       <c r="F32" s="3"/>
       <c r="G32" s="3"/>
     </row>
-    <row r="33" spans="1:7" s="2" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:7" s="2" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A33" s="18" t="s">
         <v>217</v>
       </c>
@@ -7233,7 +7237,7 @@
       <c r="F33" s="3"/>
       <c r="G33" s="3"/>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:7" ht="12" x14ac:dyDescent="0.15">
       <c r="A34" s="18" t="s">
         <v>162</v>
       </c>
@@ -7252,7 +7256,7 @@
       <c r="F34" s="3"/>
       <c r="G34" s="3"/>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:7" ht="12" x14ac:dyDescent="0.15">
       <c r="A35" s="18" t="s">
         <v>163</v>
       </c>
@@ -7271,7 +7275,7 @@
       <c r="F35" s="3"/>
       <c r="G35" s="3"/>
     </row>
-    <row r="36" spans="1:7" s="2" customFormat="1" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:7" s="2" customFormat="1" ht="13" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A36" s="18" t="s">
         <v>217</v>
       </c>
@@ -7290,7 +7294,7 @@
       <c r="F36" s="3"/>
       <c r="G36" s="3"/>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:7" ht="12" x14ac:dyDescent="0.15">
       <c r="A37" s="18" t="s">
         <v>162</v>
       </c>
@@ -7311,7 +7315,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:7" ht="12" x14ac:dyDescent="0.15">
       <c r="A38" s="18" t="s">
         <v>163</v>
       </c>
@@ -7332,7 +7336,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="39" spans="1:7" s="2" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:7" s="2" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A39" s="18" t="s">
         <v>217</v>
       </c>
@@ -7353,7 +7357,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:7" ht="12" x14ac:dyDescent="0.15">
       <c r="A40" s="18" t="s">
         <v>162</v>
       </c>
@@ -7374,7 +7378,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:7" ht="12" x14ac:dyDescent="0.15">
       <c r="A41" s="18" t="s">
         <v>163</v>
       </c>
@@ -7395,7 +7399,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="42" spans="1:7" s="2" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:7" s="2" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A42" s="18" t="s">
         <v>217</v>
       </c>
@@ -7416,7 +7420,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:7" ht="12" x14ac:dyDescent="0.15">
       <c r="A43" s="18" t="s">
         <v>154</v>
       </c>
@@ -7435,7 +7439,7 @@
       <c r="F43" s="3"/>
       <c r="G43" s="3"/>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A44" s="18" t="s">
         <v>150</v>
       </c>
@@ -7452,7 +7456,7 @@
       <c r="F44" s="3"/>
       <c r="G44" s="3"/>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A45" s="18" t="s">
         <v>151</v>
       </c>
@@ -7469,7 +7473,7 @@
       <c r="F45" s="3"/>
       <c r="G45" s="3"/>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A46" s="18" t="s">
         <v>152</v>
       </c>
@@ -7486,7 +7490,7 @@
       <c r="F46" s="3"/>
       <c r="G46" s="3"/>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A47" s="18" t="s">
         <v>153</v>
       </c>
@@ -7505,7 +7509,7 @@
       <c r="F47" s="3"/>
       <c r="G47" s="3"/>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A48" s="18" t="s">
         <v>155</v>
       </c>
@@ -7524,7 +7528,7 @@
       <c r="F48" s="3"/>
       <c r="G48" s="3"/>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A49" s="18" t="s">
         <v>156</v>
       </c>
@@ -7543,7 +7547,7 @@
       <c r="F49" s="3"/>
       <c r="G49" s="3"/>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A50" s="18" t="s">
         <v>157</v>
       </c>
@@ -7562,7 +7566,7 @@
       <c r="F50" s="3"/>
       <c r="G50" s="3"/>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:7" ht="12" x14ac:dyDescent="0.15">
       <c r="A51" s="18" t="s">
         <v>161</v>
       </c>
@@ -7581,7 +7585,7 @@
       <c r="F51" s="3"/>
       <c r="G51" s="3"/>
     </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:7" ht="12" x14ac:dyDescent="0.15">
       <c r="A52" s="18" t="s">
         <v>161</v>
       </c>
@@ -7600,7 +7604,7 @@
       <c r="F52" s="3"/>
       <c r="G52" s="3"/>
     </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A53" s="18" t="s">
         <v>158</v>
       </c>
@@ -7619,7 +7623,7 @@
       <c r="F53" s="3"/>
       <c r="G53" s="3"/>
     </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A54" s="18" t="s">
         <v>158</v>
       </c>
@@ -7638,7 +7642,7 @@
       <c r="F54" s="3"/>
       <c r="G54" s="3"/>
     </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:7" ht="12" x14ac:dyDescent="0.15">
       <c r="A55" s="18" t="s">
         <v>159</v>
       </c>
@@ -7657,7 +7661,7 @@
       <c r="F55" s="3"/>
       <c r="G55" s="3"/>
     </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:7" ht="12" x14ac:dyDescent="0.15">
       <c r="A56" s="18" t="s">
         <v>159</v>
       </c>
@@ -7676,7 +7680,7 @@
       <c r="F56" s="3"/>
       <c r="G56" s="3"/>
     </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A57" s="18" t="s">
         <v>160</v>
       </c>
@@ -7695,7 +7699,7 @@
       <c r="F57" s="3"/>
       <c r="G57" s="3"/>
     </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A58" s="18" t="s">
         <v>160</v>
       </c>
@@ -7714,7 +7718,7 @@
       <c r="F58" s="3"/>
       <c r="G58" s="3"/>
     </row>
-    <row r="59" spans="1:7" s="2" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:7" s="2" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A59" s="18" t="s">
         <v>162</v>
       </c>
@@ -7733,7 +7737,7 @@
       <c r="F59" s="3"/>
       <c r="G59" s="3"/>
     </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:7" ht="12" x14ac:dyDescent="0.15">
       <c r="A60" s="18" t="s">
         <v>163</v>
       </c>
@@ -7752,7 +7756,7 @@
       <c r="F60" s="3"/>
       <c r="G60" s="3"/>
     </row>
-    <row r="61" spans="1:7" s="2" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:7" s="2" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A61" s="18" t="s">
         <v>217</v>
       </c>
@@ -7771,7 +7775,7 @@
       <c r="F61" s="3"/>
       <c r="G61" s="3"/>
     </row>
-    <row r="62" spans="1:7" s="2" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:7" s="2" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A62" s="18" t="s">
         <v>162</v>
       </c>
@@ -7790,7 +7794,7 @@
       <c r="F62" s="3"/>
       <c r="G62" s="3"/>
     </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:7" ht="12" x14ac:dyDescent="0.15">
       <c r="A63" s="18" t="s">
         <v>163</v>
       </c>
@@ -7809,7 +7813,7 @@
       <c r="F63" s="3"/>
       <c r="G63" s="3"/>
     </row>
-    <row r="64" spans="1:7" s="2" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:7" s="2" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A64" s="18" t="s">
         <v>217</v>
       </c>
@@ -7828,7 +7832,7 @@
       <c r="F64" s="3"/>
       <c r="G64" s="3"/>
     </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:7" ht="12" x14ac:dyDescent="0.15">
       <c r="A65" s="18" t="s">
         <v>162</v>
       </c>
@@ -7847,7 +7851,7 @@
       <c r="F65" s="3"/>
       <c r="G65" s="3"/>
     </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:7" ht="12" x14ac:dyDescent="0.15">
       <c r="A66" s="18" t="s">
         <v>163</v>
       </c>
@@ -7866,7 +7870,7 @@
       <c r="F66" s="3"/>
       <c r="G66" s="3"/>
     </row>
-    <row r="67" spans="1:7" s="2" customFormat="1" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:7" s="2" customFormat="1" ht="13" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A67" s="18" t="s">
         <v>217</v>
       </c>
@@ -7885,7 +7889,7 @@
       <c r="F67" s="3"/>
       <c r="G67" s="3"/>
     </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:7" ht="12" x14ac:dyDescent="0.15">
       <c r="A68" s="18" t="s">
         <v>162</v>
       </c>
@@ -7904,7 +7908,7 @@
       <c r="F68" s="3"/>
       <c r="G68" s="3"/>
     </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:7" ht="12" x14ac:dyDescent="0.15">
       <c r="A69" s="18" t="s">
         <v>163</v>
       </c>
@@ -7923,7 +7927,7 @@
       <c r="F69" s="3"/>
       <c r="G69" s="3"/>
     </row>
-    <row r="70" spans="1:7" s="2" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:7" s="2" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A70" s="18" t="s">
         <v>217</v>
       </c>
@@ -7942,7 +7946,7 @@
       <c r="F70" s="3"/>
       <c r="G70" s="3"/>
     </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:7" ht="12" x14ac:dyDescent="0.15">
       <c r="A71" s="18" t="s">
         <v>162</v>
       </c>
@@ -7961,7 +7965,7 @@
       <c r="F71" s="3"/>
       <c r="G71" s="3"/>
     </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:7" ht="12" x14ac:dyDescent="0.15">
       <c r="A72" s="18" t="s">
         <v>163</v>
       </c>
@@ -7980,7 +7984,7 @@
       <c r="F72" s="3"/>
       <c r="G72" s="3"/>
     </row>
-    <row r="73" spans="1:7" s="2" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:7" s="2" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A73" s="18" t="s">
         <v>217</v>
       </c>
@@ -7999,7 +8003,7 @@
       <c r="F73" s="3"/>
       <c r="G73" s="3"/>
     </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:7" ht="12" x14ac:dyDescent="0.15">
       <c r="A74" s="18" t="s">
         <v>154</v>
       </c>
@@ -8018,7 +8022,7 @@
       <c r="F74" s="3"/>
       <c r="G74" s="3"/>
     </row>
-    <row r="75" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A75" s="18" t="s">
         <v>150</v>
       </c>
@@ -8035,7 +8039,7 @@
       <c r="F75" s="3"/>
       <c r="G75" s="3"/>
     </row>
-    <row r="76" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A76" s="18" t="s">
         <v>151</v>
       </c>
@@ -8052,7 +8056,7 @@
       <c r="F76" s="3"/>
       <c r="G76" s="3"/>
     </row>
-    <row r="77" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A77" s="18" t="s">
         <v>152</v>
       </c>
@@ -8069,7 +8073,7 @@
       <c r="F77" s="3"/>
       <c r="G77" s="3"/>
     </row>
-    <row r="78" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A78" s="18" t="s">
         <v>153</v>
       </c>
@@ -8088,7 +8092,7 @@
       <c r="F78" s="3"/>
       <c r="G78" s="3"/>
     </row>
-    <row r="79" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A79" s="18" t="s">
         <v>155</v>
       </c>
@@ -8107,7 +8111,7 @@
       <c r="F79" s="3"/>
       <c r="G79" s="3"/>
     </row>
-    <row r="80" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A80" s="18" t="s">
         <v>156</v>
       </c>
@@ -8126,7 +8130,7 @@
       <c r="F80" s="3"/>
       <c r="G80" s="3"/>
     </row>
-    <row r="81" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A81" s="18" t="s">
         <v>157</v>
       </c>
@@ -8145,7 +8149,7 @@
       <c r="F81" s="3"/>
       <c r="G81" s="3"/>
     </row>
-    <row r="82" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:7" ht="12" x14ac:dyDescent="0.15">
       <c r="A82" s="18" t="s">
         <v>161</v>
       </c>
@@ -8164,7 +8168,7 @@
       <c r="F82" s="3"/>
       <c r="G82" s="3"/>
     </row>
-    <row r="83" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:7" ht="12" x14ac:dyDescent="0.15">
       <c r="A83" s="18" t="s">
         <v>161</v>
       </c>
@@ -8183,7 +8187,7 @@
       <c r="F83" s="3"/>
       <c r="G83" s="3"/>
     </row>
-    <row r="84" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A84" s="18" t="s">
         <v>158</v>
       </c>
@@ -8202,7 +8206,7 @@
       <c r="F84" s="3"/>
       <c r="G84" s="3"/>
     </row>
-    <row r="85" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A85" s="18" t="s">
         <v>158</v>
       </c>
@@ -8221,7 +8225,7 @@
       <c r="F85" s="3"/>
       <c r="G85" s="3"/>
     </row>
-    <row r="86" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:7" ht="12" x14ac:dyDescent="0.15">
       <c r="A86" s="18" t="s">
         <v>159</v>
       </c>
@@ -8240,7 +8244,7 @@
       <c r="F86" s="3"/>
       <c r="G86" s="3"/>
     </row>
-    <row r="87" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:7" ht="12" x14ac:dyDescent="0.15">
       <c r="A87" s="18" t="s">
         <v>159</v>
       </c>
@@ -8259,7 +8263,7 @@
       <c r="F87" s="3"/>
       <c r="G87" s="3"/>
     </row>
-    <row r="88" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A88" s="18" t="s">
         <v>160</v>
       </c>
@@ -8278,7 +8282,7 @@
       <c r="F88" s="3"/>
       <c r="G88" s="3"/>
     </row>
-    <row r="89" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A89" s="18" t="s">
         <v>160</v>
       </c>
@@ -8297,7 +8301,7 @@
       <c r="F89" s="3"/>
       <c r="G89" s="3"/>
     </row>
-    <row r="90" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:7" ht="12" x14ac:dyDescent="0.15">
       <c r="A90" s="18" t="s">
         <v>154</v>
       </c>
@@ -8316,7 +8320,7 @@
       <c r="F90" s="3"/>
       <c r="G90" s="3"/>
     </row>
-    <row r="91" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A91" s="18" t="s">
         <v>150</v>
       </c>
@@ -8333,7 +8337,7 @@
       <c r="F91" s="3"/>
       <c r="G91" s="3"/>
     </row>
-    <row r="92" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A92" s="18" t="s">
         <v>151</v>
       </c>
@@ -8350,7 +8354,7 @@
       <c r="F92" s="3"/>
       <c r="G92" s="3"/>
     </row>
-    <row r="93" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A93" s="18" t="s">
         <v>152</v>
       </c>
@@ -8367,7 +8371,7 @@
       <c r="F93" s="3"/>
       <c r="G93" s="3"/>
     </row>
-    <row r="94" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A94" s="18" t="s">
         <v>153</v>
       </c>
@@ -8386,7 +8390,7 @@
       <c r="F94" s="3"/>
       <c r="G94" s="3"/>
     </row>
-    <row r="95" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A95" s="18" t="s">
         <v>155</v>
       </c>
@@ -8405,7 +8409,7 @@
       <c r="F95" s="3"/>
       <c r="G95" s="3"/>
     </row>
-    <row r="96" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A96" s="18" t="s">
         <v>156</v>
       </c>
@@ -8424,7 +8428,7 @@
       <c r="F96" s="3"/>
       <c r="G96" s="3"/>
     </row>
-    <row r="97" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A97" s="18" t="s">
         <v>157</v>
       </c>
@@ -8443,7 +8447,7 @@
       <c r="F97" s="3"/>
       <c r="G97" s="3"/>
     </row>
-    <row r="98" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:7" ht="12" x14ac:dyDescent="0.15">
       <c r="A98" s="18" t="s">
         <v>161</v>
       </c>
@@ -8462,7 +8466,7 @@
       <c r="F98" s="3"/>
       <c r="G98" s="3"/>
     </row>
-    <row r="99" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:7" ht="12" x14ac:dyDescent="0.15">
       <c r="A99" s="18" t="s">
         <v>161</v>
       </c>
@@ -8481,7 +8485,7 @@
       <c r="F99" s="3"/>
       <c r="G99" s="3"/>
     </row>
-    <row r="100" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A100" s="18" t="s">
         <v>158</v>
       </c>
@@ -8500,7 +8504,7 @@
       <c r="F100" s="3"/>
       <c r="G100" s="3"/>
     </row>
-    <row r="101" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A101" s="18" t="s">
         <v>158</v>
       </c>
@@ -8519,7 +8523,7 @@
       <c r="F101" s="3"/>
       <c r="G101" s="3"/>
     </row>
-    <row r="102" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A102" s="18" t="s">
         <v>159</v>
       </c>
@@ -8538,7 +8542,7 @@
       <c r="F102" s="3"/>
       <c r="G102" s="3"/>
     </row>
-    <row r="103" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A103" s="18" t="s">
         <v>159</v>
       </c>
@@ -8557,7 +8561,7 @@
       <c r="F103" s="3"/>
       <c r="G103" s="3"/>
     </row>
-    <row r="104" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A104" s="18" t="s">
         <v>160</v>
       </c>
@@ -8576,7 +8580,7 @@
       <c r="F104" s="3"/>
       <c r="G104" s="3"/>
     </row>
-    <row r="105" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A105" s="18" t="s">
         <v>160</v>
       </c>
@@ -8595,7 +8599,7 @@
       <c r="F105" s="3"/>
       <c r="G105" s="3"/>
     </row>
-    <row r="106" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:7" ht="12" x14ac:dyDescent="0.15">
       <c r="A106" s="18" t="s">
         <v>154</v>
       </c>
@@ -8614,7 +8618,7 @@
       <c r="F106" s="3"/>
       <c r="G106" s="3"/>
     </row>
-    <row r="107" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A107" s="18" t="s">
         <v>150</v>
       </c>
@@ -8631,7 +8635,7 @@
       <c r="F107" s="3"/>
       <c r="G107" s="3"/>
     </row>
-    <row r="108" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A108" s="18" t="s">
         <v>151</v>
       </c>
@@ -8648,7 +8652,7 @@
       <c r="F108" s="3"/>
       <c r="G108" s="3"/>
     </row>
-    <row r="109" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A109" s="18" t="s">
         <v>152</v>
       </c>
@@ -8665,7 +8669,7 @@
       <c r="F109" s="3"/>
       <c r="G109" s="3"/>
     </row>
-    <row r="110" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A110" s="18" t="s">
         <v>153</v>
       </c>
@@ -8684,7 +8688,7 @@
       <c r="F110" s="3"/>
       <c r="G110" s="3"/>
     </row>
-    <row r="111" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A111" s="18" t="s">
         <v>155</v>
       </c>
@@ -8703,7 +8707,7 @@
       <c r="F111" s="3"/>
       <c r="G111" s="3"/>
     </row>
-    <row r="112" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A112" s="18" t="s">
         <v>156</v>
       </c>
@@ -8722,7 +8726,7 @@
       <c r="F112" s="3"/>
       <c r="G112" s="3"/>
     </row>
-    <row r="113" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A113" s="18" t="s">
         <v>157</v>
       </c>
@@ -8741,7 +8745,7 @@
       <c r="F113" s="3"/>
       <c r="G113" s="3"/>
     </row>
-    <row r="114" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:7" ht="12" x14ac:dyDescent="0.15">
       <c r="A114" s="18" t="s">
         <v>161</v>
       </c>
@@ -8760,7 +8764,7 @@
       <c r="F114" s="3"/>
       <c r="G114" s="3"/>
     </row>
-    <row r="115" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:7" ht="12" x14ac:dyDescent="0.15">
       <c r="A115" s="18" t="s">
         <v>161</v>
       </c>
@@ -8779,7 +8783,7 @@
       <c r="F115" s="3"/>
       <c r="G115" s="3"/>
     </row>
-    <row r="116" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A116" s="18" t="s">
         <v>158</v>
       </c>
@@ -8798,7 +8802,7 @@
       <c r="F116" s="3"/>
       <c r="G116" s="3"/>
     </row>
-    <row r="117" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A117" s="18" t="s">
         <v>158</v>
       </c>
@@ -8817,7 +8821,7 @@
       <c r="F117" s="3"/>
       <c r="G117" s="3"/>
     </row>
-    <row r="118" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:7" ht="12" x14ac:dyDescent="0.15">
       <c r="A118" s="18" t="s">
         <v>159</v>
       </c>
@@ -8836,7 +8840,7 @@
       <c r="F118" s="3"/>
       <c r="G118" s="3"/>
     </row>
-    <row r="119" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:7" ht="12" x14ac:dyDescent="0.15">
       <c r="A119" s="18" t="s">
         <v>159</v>
       </c>
@@ -8855,7 +8859,7 @@
       <c r="F119" s="3"/>
       <c r="G119" s="3"/>
     </row>
-    <row r="120" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A120" s="18" t="s">
         <v>160</v>
       </c>
@@ -8874,7 +8878,7 @@
       <c r="F120" s="3"/>
       <c r="G120" s="3"/>
     </row>
-    <row r="121" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A121" s="18" t="s">
         <v>160</v>
       </c>
@@ -8893,7 +8897,7 @@
       <c r="F121" s="3"/>
       <c r="G121" s="3"/>
     </row>
-    <row r="122" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:7" ht="12" x14ac:dyDescent="0.15">
       <c r="A122" s="18" t="s">
         <v>154</v>
       </c>
@@ -8912,7 +8916,7 @@
       <c r="F122" s="3"/>
       <c r="G122" s="3"/>
     </row>
-    <row r="123" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A123" s="18" t="s">
         <v>150</v>
       </c>
@@ -8929,7 +8933,7 @@
       <c r="F123" s="3"/>
       <c r="G123" s="3"/>
     </row>
-    <row r="124" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A124" s="18" t="s">
         <v>151</v>
       </c>
@@ -8946,7 +8950,7 @@
       <c r="F124" s="3"/>
       <c r="G124" s="3"/>
     </row>
-    <row r="125" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A125" s="18" t="s">
         <v>152</v>
       </c>
@@ -8963,7 +8967,7 @@
       <c r="F125" s="3"/>
       <c r="G125" s="3"/>
     </row>
-    <row r="126" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A126" s="18" t="s">
         <v>153</v>
       </c>
@@ -8982,7 +8986,7 @@
       <c r="F126" s="3"/>
       <c r="G126" s="3"/>
     </row>
-    <row r="127" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A127" s="18" t="s">
         <v>155</v>
       </c>
@@ -9001,7 +9005,7 @@
       <c r="F127" s="3"/>
       <c r="G127" s="3"/>
     </row>
-    <row r="128" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A128" s="18" t="s">
         <v>156</v>
       </c>
@@ -9020,7 +9024,7 @@
       <c r="F128" s="3"/>
       <c r="G128" s="3"/>
     </row>
-    <row r="129" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A129" s="18" t="s">
         <v>157</v>
       </c>
@@ -9039,7 +9043,7 @@
       <c r="F129" s="3"/>
       <c r="G129" s="3"/>
     </row>
-    <row r="130" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:7" ht="12" x14ac:dyDescent="0.15">
       <c r="A130" s="18" t="s">
         <v>161</v>
       </c>
@@ -9058,7 +9062,7 @@
       <c r="F130" s="3"/>
       <c r="G130" s="3"/>
     </row>
-    <row r="131" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:7" ht="12" x14ac:dyDescent="0.15">
       <c r="A131" s="18" t="s">
         <v>161</v>
       </c>
@@ -9077,7 +9081,7 @@
       <c r="F131" s="3"/>
       <c r="G131" s="3"/>
     </row>
-    <row r="132" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A132" s="18" t="s">
         <v>158</v>
       </c>
@@ -9096,7 +9100,7 @@
       <c r="F132" s="3"/>
       <c r="G132" s="3"/>
     </row>
-    <row r="133" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A133" s="18" t="s">
         <v>158</v>
       </c>
@@ -9115,7 +9119,7 @@
       <c r="F133" s="3"/>
       <c r="G133" s="3"/>
     </row>
-    <row r="134" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:7" ht="12" x14ac:dyDescent="0.15">
       <c r="A134" s="18" t="s">
         <v>159</v>
       </c>
@@ -9134,7 +9138,7 @@
       <c r="F134" s="3"/>
       <c r="G134" s="3"/>
     </row>
-    <row r="135" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:7" ht="12" x14ac:dyDescent="0.15">
       <c r="A135" s="18" t="s">
         <v>159</v>
       </c>
@@ -9153,7 +9157,7 @@
       <c r="F135" s="3"/>
       <c r="G135" s="3"/>
     </row>
-    <row r="136" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A136" s="18" t="s">
         <v>160</v>
       </c>
@@ -9172,7 +9176,7 @@
       <c r="F136" s="3"/>
       <c r="G136" s="3"/>
     </row>
-    <row r="137" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A137" s="18" t="s">
         <v>160</v>
       </c>
@@ -9191,7 +9195,7 @@
       <c r="F137" s="3"/>
       <c r="G137" s="3"/>
     </row>
-    <row r="138" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:7" ht="12" x14ac:dyDescent="0.15">
       <c r="A138" s="18" t="s">
         <v>154</v>
       </c>
@@ -9210,7 +9214,7 @@
       <c r="F138" s="3"/>
       <c r="G138" s="3"/>
     </row>
-    <row r="139" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A139" s="18" t="s">
         <v>150</v>
       </c>
@@ -9227,7 +9231,7 @@
       <c r="F139" s="3"/>
       <c r="G139" s="3"/>
     </row>
-    <row r="140" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A140" s="18" t="s">
         <v>151</v>
       </c>
@@ -9244,7 +9248,7 @@
       <c r="F140" s="3"/>
       <c r="G140" s="3"/>
     </row>
-    <row r="141" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A141" s="18" t="s">
         <v>152</v>
       </c>
@@ -9261,7 +9265,7 @@
       <c r="F141" s="3"/>
       <c r="G141" s="3"/>
     </row>
-    <row r="142" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A142" s="18" t="s">
         <v>153</v>
       </c>
@@ -9280,7 +9284,7 @@
       <c r="F142" s="3"/>
       <c r="G142" s="3"/>
     </row>
-    <row r="143" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="143" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A143" s="18" t="s">
         <v>155</v>
       </c>
@@ -9299,7 +9303,7 @@
       <c r="F143" s="3"/>
       <c r="G143" s="3"/>
     </row>
-    <row r="144" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="144" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A144" s="18" t="s">
         <v>156</v>
       </c>
@@ -9318,7 +9322,7 @@
       <c r="F144" s="3"/>
       <c r="G144" s="3"/>
     </row>
-    <row r="145" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="145" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A145" s="18" t="s">
         <v>157</v>
       </c>
@@ -9337,7 +9341,7 @@
       <c r="F145" s="3"/>
       <c r="G145" s="3"/>
     </row>
-    <row r="146" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="146" spans="1:7" ht="12" x14ac:dyDescent="0.15">
       <c r="A146" s="18" t="s">
         <v>161</v>
       </c>
@@ -9356,7 +9360,7 @@
       <c r="F146" s="3"/>
       <c r="G146" s="3"/>
     </row>
-    <row r="147" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="147" spans="1:7" ht="12" x14ac:dyDescent="0.15">
       <c r="A147" s="18" t="s">
         <v>161</v>
       </c>
@@ -9375,7 +9379,7 @@
       <c r="F147" s="3"/>
       <c r="G147" s="3"/>
     </row>
-    <row r="148" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="148" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A148" s="18" t="s">
         <v>158</v>
       </c>
@@ -9394,7 +9398,7 @@
       <c r="F148" s="3"/>
       <c r="G148" s="3"/>
     </row>
-    <row r="149" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="149" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A149" s="18" t="s">
         <v>158</v>
       </c>
@@ -9413,7 +9417,7 @@
       <c r="F149" s="3"/>
       <c r="G149" s="3"/>
     </row>
-    <row r="150" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="150" spans="1:7" ht="12" x14ac:dyDescent="0.15">
       <c r="A150" s="18" t="s">
         <v>159</v>
       </c>
@@ -9432,7 +9436,7 @@
       <c r="F150" s="3"/>
       <c r="G150" s="3"/>
     </row>
-    <row r="151" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="151" spans="1:7" ht="12" x14ac:dyDescent="0.15">
       <c r="A151" s="18" t="s">
         <v>159</v>
       </c>
@@ -9451,7 +9455,7 @@
       <c r="F151" s="3"/>
       <c r="G151" s="3"/>
     </row>
-    <row r="152" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="152" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A152" s="18" t="s">
         <v>160</v>
       </c>
@@ -9470,7 +9474,7 @@
       <c r="F152" s="3"/>
       <c r="G152" s="3"/>
     </row>
-    <row r="153" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="153" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A153" s="18" t="s">
         <v>160</v>
       </c>
@@ -9489,7 +9493,7 @@
       <c r="F153" s="3"/>
       <c r="G153" s="3"/>
     </row>
-    <row r="154" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="154" spans="1:7" ht="12" x14ac:dyDescent="0.15">
       <c r="A154" s="18" t="s">
         <v>154</v>
       </c>
@@ -9508,7 +9512,7 @@
       <c r="F154" s="3"/>
       <c r="G154" s="3"/>
     </row>
-    <row r="155" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="155" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A155" s="18" t="s">
         <v>150</v>
       </c>
@@ -9525,7 +9529,7 @@
       <c r="F155" s="3"/>
       <c r="G155" s="3"/>
     </row>
-    <row r="156" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="156" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A156" s="18" t="s">
         <v>151</v>
       </c>
@@ -9542,7 +9546,7 @@
       <c r="F156" s="3"/>
       <c r="G156" s="3"/>
     </row>
-    <row r="157" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="157" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A157" s="18" t="s">
         <v>152</v>
       </c>
@@ -9559,7 +9563,7 @@
       <c r="F157" s="3"/>
       <c r="G157" s="3"/>
     </row>
-    <row r="158" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="158" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A158" s="18" t="s">
         <v>153</v>
       </c>
@@ -9578,7 +9582,7 @@
       <c r="F158" s="3"/>
       <c r="G158" s="3"/>
     </row>
-    <row r="159" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="159" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A159" s="18" t="s">
         <v>155</v>
       </c>
@@ -9597,7 +9601,7 @@
       <c r="F159" s="3"/>
       <c r="G159" s="3"/>
     </row>
-    <row r="160" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="160" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A160" s="18" t="s">
         <v>156</v>
       </c>
@@ -9616,7 +9620,7 @@
       <c r="F160" s="3"/>
       <c r="G160" s="3"/>
     </row>
-    <row r="161" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="161" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A161" s="18" t="s">
         <v>157</v>
       </c>
@@ -9635,7 +9639,7 @@
       <c r="F161" s="3"/>
       <c r="G161" s="3"/>
     </row>
-    <row r="162" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="162" spans="1:7" ht="12" x14ac:dyDescent="0.15">
       <c r="A162" s="18" t="s">
         <v>161</v>
       </c>
@@ -9654,7 +9658,7 @@
       <c r="F162" s="3"/>
       <c r="G162" s="3"/>
     </row>
-    <row r="163" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="163" spans="1:7" ht="12" x14ac:dyDescent="0.15">
       <c r="A163" s="18" t="s">
         <v>161</v>
       </c>
@@ -9673,7 +9677,7 @@
       <c r="F163" s="3"/>
       <c r="G163" s="3"/>
     </row>
-    <row r="164" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="164" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A164" s="18" t="s">
         <v>158</v>
       </c>
@@ -9692,7 +9696,7 @@
       <c r="F164" s="3"/>
       <c r="G164" s="3"/>
     </row>
-    <row r="165" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="165" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A165" s="18" t="s">
         <v>158</v>
       </c>
@@ -9711,7 +9715,7 @@
       <c r="F165" s="3"/>
       <c r="G165" s="3"/>
     </row>
-    <row r="166" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="166" spans="1:7" ht="12" x14ac:dyDescent="0.15">
       <c r="A166" s="18" t="s">
         <v>159</v>
       </c>
@@ -9730,7 +9734,7 @@
       <c r="F166" s="3"/>
       <c r="G166" s="3"/>
     </row>
-    <row r="167" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="167" spans="1:7" ht="12" x14ac:dyDescent="0.15">
       <c r="A167" s="18" t="s">
         <v>159</v>
       </c>
@@ -9749,7 +9753,7 @@
       <c r="F167" s="3"/>
       <c r="G167" s="3"/>
     </row>
-    <row r="168" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="168" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A168" s="18" t="s">
         <v>160</v>
       </c>
@@ -9768,7 +9772,7 @@
       <c r="F168" s="3"/>
       <c r="G168" s="3"/>
     </row>
-    <row r="169" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="169" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A169" s="18" t="s">
         <v>160</v>
       </c>
@@ -9787,7 +9791,7 @@
       <c r="F169" s="3"/>
       <c r="G169" s="3"/>
     </row>
-    <row r="170" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="170" spans="1:7" ht="12" x14ac:dyDescent="0.15">
       <c r="A170" s="18" t="s">
         <v>154</v>
       </c>
@@ -9806,7 +9810,7 @@
       <c r="F170" s="3"/>
       <c r="G170" s="3"/>
     </row>
-    <row r="171" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="171" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A171" s="18" t="s">
         <v>150</v>
       </c>
@@ -9823,7 +9827,7 @@
       <c r="F171" s="3"/>
       <c r="G171" s="3"/>
     </row>
-    <row r="172" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="172" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A172" s="18" t="s">
         <v>151</v>
       </c>
@@ -9840,7 +9844,7 @@
       <c r="F172" s="3"/>
       <c r="G172" s="3"/>
     </row>
-    <row r="173" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="173" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A173" s="18" t="s">
         <v>152</v>
       </c>
@@ -9857,7 +9861,7 @@
       <c r="F173" s="3"/>
       <c r="G173" s="3"/>
     </row>
-    <row r="174" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="174" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A174" s="18" t="s">
         <v>153</v>
       </c>
@@ -9876,7 +9880,7 @@
       <c r="F174" s="3"/>
       <c r="G174" s="3"/>
     </row>
-    <row r="175" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="175" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A175" s="18" t="s">
         <v>155</v>
       </c>
@@ -9895,7 +9899,7 @@
       <c r="F175" s="3"/>
       <c r="G175" s="3"/>
     </row>
-    <row r="176" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="176" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A176" s="18" t="s">
         <v>156</v>
       </c>
@@ -9914,7 +9918,7 @@
       <c r="F176" s="3"/>
       <c r="G176" s="3"/>
     </row>
-    <row r="177" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="177" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A177" s="18" t="s">
         <v>157</v>
       </c>
@@ -9933,7 +9937,7 @@
       <c r="F177" s="3"/>
       <c r="G177" s="3"/>
     </row>
-    <row r="178" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="178" spans="1:7" ht="12" x14ac:dyDescent="0.15">
       <c r="A178" s="18" t="s">
         <v>161</v>
       </c>
@@ -9952,7 +9956,7 @@
       <c r="F178" s="3"/>
       <c r="G178" s="3"/>
     </row>
-    <row r="179" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="179" spans="1:7" ht="12" x14ac:dyDescent="0.15">
       <c r="A179" s="18" t="s">
         <v>161</v>
       </c>
@@ -9971,7 +9975,7 @@
       <c r="F179" s="3"/>
       <c r="G179" s="3"/>
     </row>
-    <row r="180" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="180" spans="1:7" ht="12" x14ac:dyDescent="0.15">
       <c r="A180" s="18" t="s">
         <v>161</v>
       </c>
@@ -9990,7 +9994,7 @@
       <c r="F180" s="3"/>
       <c r="G180" s="3"/>
     </row>
-    <row r="181" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="181" spans="1:7" ht="12" x14ac:dyDescent="0.15">
       <c r="A181" s="18" t="s">
         <v>161</v>
       </c>
@@ -10009,7 +10013,7 @@
       <c r="F181" s="3"/>
       <c r="G181" s="3"/>
     </row>
-    <row r="182" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="182" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A182" s="18" t="s">
         <v>158</v>
       </c>
@@ -10028,7 +10032,7 @@
       <c r="F182" s="3"/>
       <c r="G182" s="3"/>
     </row>
-    <row r="183" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="183" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A183" s="18" t="s">
         <v>158</v>
       </c>
@@ -10047,7 +10051,7 @@
       <c r="F183" s="3"/>
       <c r="G183" s="3"/>
     </row>
-    <row r="184" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="184" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A184" s="18" t="s">
         <v>158</v>
       </c>
@@ -10066,7 +10070,7 @@
       <c r="F184" s="3"/>
       <c r="G184" s="3"/>
     </row>
-    <row r="185" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="185" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A185" s="18" t="s">
         <v>158</v>
       </c>
@@ -10085,7 +10089,7 @@
       <c r="F185" s="3"/>
       <c r="G185" s="3"/>
     </row>
-    <row r="186" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="186" spans="1:7" ht="12" x14ac:dyDescent="0.15">
       <c r="A186" s="18" t="s">
         <v>159</v>
       </c>
@@ -10104,7 +10108,7 @@
       <c r="F186" s="3"/>
       <c r="G186" s="3"/>
     </row>
-    <row r="187" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="187" spans="1:7" ht="12" x14ac:dyDescent="0.15">
       <c r="A187" s="18" t="s">
         <v>159</v>
       </c>
@@ -10123,7 +10127,7 @@
       <c r="F187" s="3"/>
       <c r="G187" s="3"/>
     </row>
-    <row r="188" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="188" spans="1:7" ht="12" x14ac:dyDescent="0.15">
       <c r="A188" s="18" t="s">
         <v>159</v>
       </c>
@@ -10142,7 +10146,7 @@
       <c r="F188" s="3"/>
       <c r="G188" s="3"/>
     </row>
-    <row r="189" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="189" spans="1:7" ht="12" x14ac:dyDescent="0.15">
       <c r="A189" s="18" t="s">
         <v>159</v>
       </c>
@@ -10161,7 +10165,7 @@
       <c r="F189" s="3"/>
       <c r="G189" s="3"/>
     </row>
-    <row r="190" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="190" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A190" s="18" t="s">
         <v>160</v>
       </c>
@@ -10180,7 +10184,7 @@
       <c r="F190" s="3"/>
       <c r="G190" s="3"/>
     </row>
-    <row r="191" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="191" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A191" s="18" t="s">
         <v>160</v>
       </c>
@@ -10199,7 +10203,7 @@
       <c r="F191" s="3"/>
       <c r="G191" s="3"/>
     </row>
-    <row r="192" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="192" spans="1:7" ht="12" x14ac:dyDescent="0.15">
       <c r="A192" s="18" t="s">
         <v>154</v>
       </c>
@@ -10218,7 +10222,7 @@
       <c r="F192" s="3"/>
       <c r="G192" s="3"/>
     </row>
-    <row r="193" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="193" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A193" s="18" t="s">
         <v>150</v>
       </c>
@@ -10235,7 +10239,7 @@
       <c r="F193" s="3"/>
       <c r="G193" s="3"/>
     </row>
-    <row r="194" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="194" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A194" s="18" t="s">
         <v>151</v>
       </c>
@@ -10252,7 +10256,7 @@
       <c r="F194" s="3"/>
       <c r="G194" s="3"/>
     </row>
-    <row r="195" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="195" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A195" s="18" t="s">
         <v>152</v>
       </c>
@@ -10269,7 +10273,7 @@
       <c r="F195" s="3"/>
       <c r="G195" s="3"/>
     </row>
-    <row r="196" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="196" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A196" s="18" t="s">
         <v>153</v>
       </c>
@@ -10288,7 +10292,7 @@
       <c r="F196" s="3"/>
       <c r="G196" s="3"/>
     </row>
-    <row r="197" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="197" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A197" s="18" t="s">
         <v>155</v>
       </c>
@@ -10307,7 +10311,7 @@
       <c r="F197" s="3"/>
       <c r="G197" s="3"/>
     </row>
-    <row r="198" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="198" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A198" s="18" t="s">
         <v>156</v>
       </c>
@@ -10326,7 +10330,7 @@
       <c r="F198" s="3"/>
       <c r="G198" s="3"/>
     </row>
-    <row r="199" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="199" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A199" s="18" t="s">
         <v>157</v>
       </c>
@@ -10345,7 +10349,7 @@
       <c r="F199" s="3"/>
       <c r="G199" s="3"/>
     </row>
-    <row r="200" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="200" spans="1:7" ht="12" x14ac:dyDescent="0.15">
       <c r="A200" s="18" t="s">
         <v>161</v>
       </c>
@@ -10364,7 +10368,7 @@
       <c r="F200" s="3"/>
       <c r="G200" s="3"/>
     </row>
-    <row r="201" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="201" spans="1:7" ht="12" x14ac:dyDescent="0.15">
       <c r="A201" s="18" t="s">
         <v>161</v>
       </c>
@@ -10383,7 +10387,7 @@
       <c r="F201" s="3"/>
       <c r="G201" s="3"/>
     </row>
-    <row r="202" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="202" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A202" s="18" t="s">
         <v>158</v>
       </c>
@@ -10402,7 +10406,7 @@
       <c r="F202" s="3"/>
       <c r="G202" s="3"/>
     </row>
-    <row r="203" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="203" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A203" s="18" t="s">
         <v>158</v>
       </c>
@@ -10421,7 +10425,7 @@
       <c r="F203" s="3"/>
       <c r="G203" s="3"/>
     </row>
-    <row r="204" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="204" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A204" s="18" t="s">
         <v>159</v>
       </c>
@@ -10440,7 +10444,7 @@
       <c r="F204" s="3"/>
       <c r="G204" s="3"/>
     </row>
-    <row r="205" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="205" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A205" s="18" t="s">
         <v>159</v>
       </c>
@@ -10459,7 +10463,7 @@
       <c r="F205" s="3"/>
       <c r="G205" s="3"/>
     </row>
-    <row r="206" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="206" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A206" s="18" t="s">
         <v>160</v>
       </c>
@@ -10478,7 +10482,7 @@
       <c r="F206" s="3"/>
       <c r="G206" s="3"/>
     </row>
-    <row r="207" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="207" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A207" s="18" t="s">
         <v>160</v>
       </c>
@@ -10497,7 +10501,7 @@
       <c r="F207" s="3"/>
       <c r="G207" s="3"/>
     </row>
-    <row r="208" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="208" spans="1:7" ht="12" x14ac:dyDescent="0.15">
       <c r="A208" s="18" t="s">
         <v>154</v>
       </c>
@@ -10516,7 +10520,7 @@
       <c r="F208" s="3"/>
       <c r="G208" s="3"/>
     </row>
-    <row r="209" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="209" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A209" s="18" t="s">
         <v>150</v>
       </c>
@@ -10533,7 +10537,7 @@
       <c r="F209" s="3"/>
       <c r="G209" s="3"/>
     </row>
-    <row r="210" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="210" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A210" s="18" t="s">
         <v>151</v>
       </c>
@@ -10550,7 +10554,7 @@
       <c r="F210" s="3"/>
       <c r="G210" s="3"/>
     </row>
-    <row r="211" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="211" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A211" s="18" t="s">
         <v>152</v>
       </c>
@@ -10567,7 +10571,7 @@
       <c r="F211" s="3"/>
       <c r="G211" s="3"/>
     </row>
-    <row r="212" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="212" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A212" s="18" t="s">
         <v>153</v>
       </c>
@@ -10586,7 +10590,7 @@
       <c r="F212" s="3"/>
       <c r="G212" s="3"/>
     </row>
-    <row r="213" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="213" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A213" s="18" t="s">
         <v>155</v>
       </c>
@@ -10605,7 +10609,7 @@
       <c r="F213" s="3"/>
       <c r="G213" s="3"/>
     </row>
-    <row r="214" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="214" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A214" s="18" t="s">
         <v>156</v>
       </c>
@@ -10624,7 +10628,7 @@
       <c r="F214" s="3"/>
       <c r="G214" s="3"/>
     </row>
-    <row r="215" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="215" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A215" s="18" t="s">
         <v>157</v>
       </c>
@@ -10643,7 +10647,7 @@
       <c r="F215" s="3"/>
       <c r="G215" s="3"/>
     </row>
-    <row r="216" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="216" spans="1:7" ht="12" x14ac:dyDescent="0.15">
       <c r="A216" s="18" t="s">
         <v>161</v>
       </c>
@@ -10662,7 +10666,7 @@
       <c r="F216" s="3"/>
       <c r="G216" s="3"/>
     </row>
-    <row r="217" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="217" spans="1:7" ht="12" x14ac:dyDescent="0.15">
       <c r="A217" s="18" t="s">
         <v>161</v>
       </c>
@@ -10681,7 +10685,7 @@
       <c r="F217" s="3"/>
       <c r="G217" s="3"/>
     </row>
-    <row r="218" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="218" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A218" s="18" t="s">
         <v>158</v>
       </c>
@@ -10700,7 +10704,7 @@
       <c r="F218" s="3"/>
       <c r="G218" s="3"/>
     </row>
-    <row r="219" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="219" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A219" s="18" t="s">
         <v>158</v>
       </c>
@@ -10719,7 +10723,7 @@
       <c r="F219" s="3"/>
       <c r="G219" s="3"/>
     </row>
-    <row r="220" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="220" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A220" s="18" t="s">
         <v>159</v>
       </c>
@@ -10738,7 +10742,7 @@
       <c r="F220" s="3"/>
       <c r="G220" s="3"/>
     </row>
-    <row r="221" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="221" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A221" s="18" t="s">
         <v>159</v>
       </c>
@@ -10757,7 +10761,7 @@
       <c r="F221" s="3"/>
       <c r="G221" s="3"/>
     </row>
-    <row r="222" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="222" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A222" s="18" t="s">
         <v>160</v>
       </c>
@@ -10776,7 +10780,7 @@
       <c r="F222" s="3"/>
       <c r="G222" s="3"/>
     </row>
-    <row r="223" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="223" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A223" s="18" t="s">
         <v>160</v>
       </c>
@@ -10796,7 +10800,7 @@
       <c r="G223" s="3"/>
     </row>
   </sheetData>
-  <sortState ref="A1:P15">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A1:P15">
     <sortCondition descending="1" ref="A1:A15"/>
   </sortState>
   <mergeCells count="2">

</xml_diff>